<commit_message>
#Familias Definidas Completo #Fix funciones iteradoradoras en BLLFamilia para definir permisos de usuario en interfaz
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="89">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -231,13 +231,73 @@
   </si>
   <si>
     <t>Usuario Password</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Ingresos y Gastos</t>
+  </si>
+  <si>
+    <t>Solicitudes y Cotizaciones</t>
+  </si>
+  <si>
+    <t>Solicitudes y Cotizaciones Admin</t>
+  </si>
+  <si>
+    <t>Ingresos y Gastos Admin</t>
+  </si>
+  <si>
+    <t>Adquisiciones y Asignacion Admin</t>
+  </si>
+  <si>
+    <t>Administracion Total</t>
+  </si>
+  <si>
+    <t>Administracion Sistema</t>
+  </si>
+  <si>
+    <t>Patentes/Familias</t>
+  </si>
+  <si>
+    <t>Adquisicion y Asignacion</t>
+  </si>
+  <si>
+    <t>Buscar Categoria</t>
+  </si>
+  <si>
+    <t>Buscar Proveedor</t>
+  </si>
+  <si>
+    <t>Buscar Familia</t>
+  </si>
+  <si>
+    <t>Buscar Usuario</t>
+  </si>
+  <si>
+    <t>Lola</t>
+  </si>
+  <si>
+    <t>mgulli</t>
+  </si>
+  <si>
+    <t>paco</t>
+  </si>
+  <si>
+    <t>jlopez</t>
+  </si>
+  <si>
+    <t>pargi</t>
+  </si>
+  <si>
+    <t>adminsistema</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,16 +305,63 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -262,12 +369,271 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,335 +914,1286 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="C3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="24"/>
+      <c r="B6" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B7" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24"/>
+      <c r="B8" s="6" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="C9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
+      <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="C10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="23"/>
+      <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="C11" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="C13" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C14" s="13"/>
+      <c r="D14" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
+      <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="23"/>
+      <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="11"/>
+      <c r="J18" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="J20" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="24"/>
+      <c r="B21" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" s="13"/>
+      <c r="J21" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B22" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" s="9"/>
+      <c r="J22" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="23"/>
+      <c r="B23" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I23" s="11"/>
+      <c r="J23" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="23"/>
+      <c r="B24" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="24"/>
+      <c r="B25" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I25" s="13"/>
+      <c r="J25" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B26" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="C26" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="23"/>
+      <c r="B27" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="C27" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
+      <c r="B28" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="C28" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="24"/>
+      <c r="B29" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="C29" s="13"/>
+      <c r="D29" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B30" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+      <c r="C30" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I30" s="9"/>
+      <c r="J30" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+      <c r="B32" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="23"/>
+      <c r="B33" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="24"/>
+      <c r="B34" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B35" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="23"/>
+      <c r="B36" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+      <c r="C36" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="I36" s="11"/>
+      <c r="J36" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="24"/>
+      <c r="B37" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B38" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="23"/>
+      <c r="B39" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
+      <c r="B40" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="23"/>
+      <c r="B41" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G41" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H41" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="I41" s="15"/>
+      <c r="J41" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="24"/>
+      <c r="B42" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B43" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="I43" s="9"/>
+      <c r="J43" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="23"/>
+      <c r="B44" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="I44" s="11"/>
+      <c r="J44" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="23"/>
+      <c r="B45" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="I45" s="11"/>
+      <c r="J45" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
+      <c r="B46" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G46" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H46" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="I46" s="15"/>
+      <c r="J46" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="24"/>
+      <c r="B47" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I47" s="13"/>
+      <c r="J47" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B48" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J48" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="23"/>
+      <c r="B49" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J49" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="23"/>
+      <c r="B50" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J50" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="23"/>
+      <c r="B51" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="23"/>
+      <c r="B52" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J52" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="24"/>
+      <c r="B53" s="6" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="C53" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="J53" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B54" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J54" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="24"/>
+      <c r="B55" s="6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="J55" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B56" s="8" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="J56" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B57" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="23"/>
+      <c r="B58" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="23"/>
+      <c r="B59" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="24"/>
+      <c r="B60" s="6" t="s">
         <v>64</v>
       </c>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>84</v>
+      </c>
+      <c r="E62" t="s">
+        <v>85</v>
+      </c>
+      <c r="F62" t="s">
+        <v>83</v>
+      </c>
+      <c r="H62" t="s">
+        <v>86</v>
+      </c>
+      <c r="I62" t="s">
+        <v>88</v>
+      </c>
+      <c r="J62" s="25" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="A48:A53"/>
+    <mergeCell ref="A54:A55"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#Autorización en interfaz realizados: •	Crear Solicitud •	Buscar Solicitud •	Modificar Solicitud •	Cancelar Solicitud •	Solicitar Cotizacion •	Agregar Cotizacion •	Crear Partida •	Buscar Partida •	Modificar Partida •	Cancelar Partida •	Asociar Partida •	Registrar Adquisicion •	Buscar Adquisicion •	Modificar Adquisicion
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="89">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -335,7 +335,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -360,6 +360,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -571,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -622,6 +628,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -631,9 +640,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -918,7 +927,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,10 +975,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="9"/>
@@ -988,8 +997,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -1016,8 +1025,8 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="27" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="11"/>
@@ -1036,8 +1045,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="11"/>
@@ -1054,7 +1063,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="6" t="s">
         <v>45</v>
       </c>
@@ -1072,10 +1081,10 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="26" t="s">
         <v>66</v>
       </c>
       <c r="C7" s="9"/>
@@ -1094,8 +1103,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="28" t="s">
         <v>67</v>
       </c>
       <c r="C8" s="13"/>
@@ -1114,10 +1123,10 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="26" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1136,8 +1145,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="27" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -1152,16 +1161,20 @@
       <c r="F10" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="G10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>69</v>
+      </c>
       <c r="I10" s="11"/>
       <c r="J10" s="12" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="27" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -1180,8 +1193,8 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="24"/>
+      <c r="B12" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="11"/>
@@ -1198,8 +1211,8 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="5" t="s">
+      <c r="A13" s="24"/>
+      <c r="B13" s="27" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -1218,7 +1231,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="6" t="s">
         <v>44</v>
       </c>
@@ -1236,10 +1249,10 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="26" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="9"/>
@@ -1258,12 +1271,16 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="24"/>
+      <c r="B16" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="C16" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>69</v>
+      </c>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11" t="s">
@@ -1278,8 +1295,8 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="24"/>
+      <c r="B17" s="27" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="11"/>
@@ -1298,7 +1315,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
@@ -1316,7 +1333,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="5" t="s">
         <v>15</v>
       </c>
@@ -1336,7 +1353,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
@@ -1356,7 +1373,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="24"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="6" t="s">
         <v>18</v>
       </c>
@@ -1376,7 +1393,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1398,7 +1415,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="5" t="s">
         <v>21</v>
       </c>
@@ -1418,7 +1435,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="5" t="s">
         <v>22</v>
       </c>
@@ -1438,7 +1455,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="24"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="6" t="s">
         <v>23</v>
       </c>
@@ -1456,7 +1473,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="23" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1478,7 +1495,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
+      <c r="A27" s="24"/>
       <c r="B27" s="5" t="s">
         <v>26</v>
       </c>
@@ -1498,7 +1515,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="5" t="s">
         <v>27</v>
       </c>
@@ -1518,7 +1535,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="24"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="6" t="s">
         <v>28</v>
       </c>
@@ -1536,7 +1553,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="23" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -1566,7 +1583,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="5" t="s">
         <v>31</v>
       </c>
@@ -1584,7 +1601,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="5" t="s">
         <v>32</v>
       </c>
@@ -1602,7 +1619,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="5" t="s">
         <v>33</v>
       </c>
@@ -1620,7 +1637,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="24"/>
+      <c r="A34" s="25"/>
       <c r="B34" s="6" t="s">
         <v>43</v>
       </c>
@@ -1638,7 +1655,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="23" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -1658,7 +1675,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="5" t="s">
         <v>36</v>
       </c>
@@ -1686,7 +1703,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="24"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="6" t="s">
         <v>37</v>
       </c>
@@ -1704,7 +1721,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="23" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -1724,7 +1741,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="5" t="s">
         <v>40</v>
       </c>
@@ -1742,7 +1759,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
+      <c r="A40" s="24"/>
       <c r="B40" s="5" t="s">
         <v>41</v>
       </c>
@@ -1760,7 +1777,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
+      <c r="A41" s="24"/>
       <c r="B41" s="3" t="s">
         <v>79</v>
       </c>
@@ -1784,7 +1801,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="24"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="6" t="s">
         <v>42</v>
       </c>
@@ -1802,7 +1819,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="23" t="s">
         <v>46</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -1824,7 +1841,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
+      <c r="A44" s="24"/>
       <c r="B44" s="5" t="s">
         <v>48</v>
       </c>
@@ -1844,7 +1861,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
+      <c r="A45" s="24"/>
       <c r="B45" s="5" t="s">
         <v>49</v>
       </c>
@@ -1864,7 +1881,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
+      <c r="A46" s="24"/>
       <c r="B46" s="3" t="s">
         <v>80</v>
       </c>
@@ -1892,7 +1909,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="24"/>
+      <c r="A47" s="25"/>
       <c r="B47" s="6" t="s">
         <v>50</v>
       </c>
@@ -1912,7 +1929,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="22" t="s">
+      <c r="A48" s="23" t="s">
         <v>51</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -1932,7 +1949,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
+      <c r="A49" s="24"/>
       <c r="B49" s="5" t="s">
         <v>53</v>
       </c>
@@ -1950,7 +1967,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
+      <c r="A50" s="24"/>
       <c r="B50" s="5" t="s">
         <v>54</v>
       </c>
@@ -1968,7 +1985,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
+      <c r="A51" s="24"/>
       <c r="B51" s="5" t="s">
         <v>55</v>
       </c>
@@ -1986,7 +2003,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
+      <c r="A52" s="24"/>
       <c r="B52" s="3" t="s">
         <v>82</v>
       </c>
@@ -2004,7 +2021,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="24"/>
+      <c r="A53" s="25"/>
       <c r="B53" s="6" t="s">
         <v>68</v>
       </c>
@@ -2034,7 +2051,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="22" t="s">
+      <c r="A54" s="23" t="s">
         <v>56</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -2054,7 +2071,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="24"/>
+      <c r="A55" s="25"/>
       <c r="B55" s="6" t="s">
         <v>58</v>
       </c>
@@ -2092,7 +2109,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="22" t="s">
+      <c r="A57" s="23" t="s">
         <v>61</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -2110,7 +2127,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="23"/>
+      <c r="A58" s="24"/>
       <c r="B58" s="5" t="s">
         <v>63</v>
       </c>
@@ -2126,7 +2143,7 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
+      <c r="A59" s="24"/>
       <c r="B59" s="3" t="s">
         <v>81</v>
       </c>
@@ -2142,7 +2159,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="24"/>
+      <c r="A60" s="25"/>
       <c r="B60" s="6" t="s">
         <v>64</v>
       </c>
@@ -2173,18 +2190,12 @@
       <c r="I62" t="s">
         <v>88</v>
       </c>
-      <c r="J62" s="25" t="s">
+      <c r="J62" s="22" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A22:A25"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A37"/>
@@ -2192,6 +2203,12 @@
     <mergeCell ref="A43:A47"/>
     <mergeCell ref="A48:A53"/>
     <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#Fix Autorizaciones (directamente true o false en enabled desde la funcion BuscarPermisos)
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -631,6 +631,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -640,9 +643,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,7 +927,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,10 +975,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="9"/>
@@ -997,8 +997,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -1025,8 +1025,8 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="27" t="s">
+      <c r="A4" s="27"/>
+      <c r="B4" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="11"/>
@@ -1045,8 +1045,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="27" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="24" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="11"/>
@@ -1063,7 +1063,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="6" t="s">
         <v>45</v>
       </c>
@@ -1081,10 +1081,10 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="23" t="s">
         <v>66</v>
       </c>
       <c r="C7" s="9"/>
@@ -1103,8 +1103,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="28" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="25" t="s">
         <v>67</v>
       </c>
       <c r="C8" s="13"/>
@@ -1123,10 +1123,10 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="23" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1145,8 +1145,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="27" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -1173,8 +1173,8 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="27" t="s">
+      <c r="A11" s="27"/>
+      <c r="B11" s="24" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -1193,8 +1193,8 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="27" t="s">
+      <c r="A12" s="27"/>
+      <c r="B12" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="11"/>
@@ -1211,8 +1211,8 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="27" t="s">
+      <c r="A13" s="27"/>
+      <c r="B13" s="24" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -1231,7 +1231,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="6" t="s">
         <v>44</v>
       </c>
@@ -1249,10 +1249,10 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="23" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="9"/>
@@ -1271,8 +1271,8 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="27" t="s">
+      <c r="A16" s="27"/>
+      <c r="B16" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="11" t="s">
@@ -1295,8 +1295,8 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="27" t="s">
+      <c r="A17" s="27"/>
+      <c r="B17" s="24" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="11"/>
@@ -1315,7 +1315,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
@@ -1333,7 +1333,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="5" t="s">
         <v>15</v>
       </c>
@@ -1353,7 +1353,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
@@ -1373,7 +1373,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="25"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="6" t="s">
         <v>18</v>
       </c>
@@ -1393,7 +1393,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="26" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1415,7 +1415,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="5" t="s">
         <v>21</v>
       </c>
@@ -1435,7 +1435,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="5" t="s">
         <v>22</v>
       </c>
@@ -1455,7 +1455,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="25"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="6" t="s">
         <v>23</v>
       </c>
@@ -1473,7 +1473,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="26" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1495,7 +1495,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="5" t="s">
         <v>26</v>
       </c>
@@ -1515,7 +1515,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="5" t="s">
         <v>27</v>
       </c>
@@ -1535,7 +1535,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="25"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="6" t="s">
         <v>28</v>
       </c>
@@ -1553,7 +1553,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -1583,7 +1583,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="5" t="s">
         <v>31</v>
       </c>
@@ -1601,7 +1601,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="5" t="s">
         <v>32</v>
       </c>
@@ -1619,7 +1619,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="5" t="s">
         <v>33</v>
       </c>
@@ -1637,7 +1637,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="25"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="6" t="s">
         <v>43</v>
       </c>
@@ -1655,7 +1655,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
+      <c r="A35" s="26" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -1675,7 +1675,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="5" t="s">
         <v>36</v>
       </c>
@@ -1703,7 +1703,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="25"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="6" t="s">
         <v>37</v>
       </c>
@@ -1721,7 +1721,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="26" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -1741,7 +1741,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="5" t="s">
         <v>40</v>
       </c>
@@ -1759,7 +1759,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
+      <c r="A40" s="27"/>
       <c r="B40" s="5" t="s">
         <v>41</v>
       </c>
@@ -1777,7 +1777,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
+      <c r="A41" s="27"/>
       <c r="B41" s="3" t="s">
         <v>79</v>
       </c>
@@ -1801,7 +1801,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="25"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="6" t="s">
         <v>42</v>
       </c>
@@ -1819,7 +1819,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="26" t="s">
         <v>46</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -1841,7 +1841,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
+      <c r="A44" s="27"/>
       <c r="B44" s="5" t="s">
         <v>48</v>
       </c>
@@ -1861,7 +1861,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
+      <c r="A45" s="27"/>
       <c r="B45" s="5" t="s">
         <v>49</v>
       </c>
@@ -1881,7 +1881,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="24"/>
+      <c r="A46" s="27"/>
       <c r="B46" s="3" t="s">
         <v>80</v>
       </c>
@@ -1909,7 +1909,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="25"/>
+      <c r="A47" s="28"/>
       <c r="B47" s="6" t="s">
         <v>50</v>
       </c>
@@ -1929,7 +1929,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="26" t="s">
         <v>51</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -1949,7 +1949,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="24"/>
+      <c r="A49" s="27"/>
       <c r="B49" s="5" t="s">
         <v>53</v>
       </c>
@@ -1967,7 +1967,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="24"/>
+      <c r="A50" s="27"/>
       <c r="B50" s="5" t="s">
         <v>54</v>
       </c>
@@ -1985,7 +1985,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="24"/>
+      <c r="A51" s="27"/>
       <c r="B51" s="5" t="s">
         <v>55</v>
       </c>
@@ -2003,7 +2003,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="24"/>
+      <c r="A52" s="27"/>
       <c r="B52" s="3" t="s">
         <v>82</v>
       </c>
@@ -2021,7 +2021,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="25"/>
+      <c r="A53" s="28"/>
       <c r="B53" s="6" t="s">
         <v>68</v>
       </c>
@@ -2051,7 +2051,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="23" t="s">
+      <c r="A54" s="26" t="s">
         <v>56</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -2071,7 +2071,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="25"/>
+      <c r="A55" s="28"/>
       <c r="B55" s="6" t="s">
         <v>58</v>
       </c>
@@ -2109,7 +2109,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="23" t="s">
+      <c r="A57" s="26" t="s">
         <v>61</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -2127,7 +2127,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="24"/>
+      <c r="A58" s="27"/>
       <c r="B58" s="5" t="s">
         <v>63</v>
       </c>
@@ -2143,7 +2143,7 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="24"/>
+      <c r="A59" s="27"/>
       <c r="B59" s="3" t="s">
         <v>81</v>
       </c>
@@ -2159,7 +2159,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="25"/>
+      <c r="A60" s="28"/>
       <c r="B60" s="6" t="s">
         <v>64</v>
       </c>
@@ -2196,6 +2196,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A22:A25"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A37"/>
@@ -2203,12 +2209,6 @@
     <mergeCell ref="A43:A47"/>
     <mergeCell ref="A48:A53"/>
     <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#Autorizacion modificacion para utilizar Diccionario en .tag, y tener las claves "Permisos" e "Idioma": Permisos realizados en Interfaz y BLL (agregué revisión de permisos en BLL): - Crear Solicitud - Buscar Solicitud - Modificar Solicitud - Cancelar Solicitud
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -335,7 +335,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,6 +366,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -577,7 +583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -643,6 +649,8 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,7 +935,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,7 +986,7 @@
       <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="9"/>
@@ -998,7 +1006,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -1026,7 +1034,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="29" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="11"/>
@@ -1046,7 +1054,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="27"/>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="29" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="11"/>
@@ -2196,12 +2204,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A22:A25"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A37"/>
@@ -2209,6 +2211,12 @@
     <mergeCell ref="A43:A47"/>
     <mergeCell ref="A48:A53"/>
     <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
1.	Permisos en interfaz: •	Crear Solicitud •	Buscar Solicitud •	Modificar Solicitud •	Cancelar Solicitud •	Solicitar Cotizacion •	Agregar Cotizacion •	Crear Partida •	Buscar Partida •	Modificar Partida •	Cancelar Partida •	Asociar Partida •	Registrar Adquisicion •	Buscar Adquisicion •	Modificar Adquisicion •	Adquisicion Eliminar •	Modificar Inventario •	Agregar Inventario •	Inventario Eliminar • 2.	Permisos en BLL •	Modificar Solicitud •	Cancelar Solicitud •	Buscar Solicitud •	Solicitud Crear •	Crear Partida •	Modificar Partida •	Cancelar Partida •	Asociar Partida •	Registrar Adquisicion •	Buscar Adquisicion •	Modificar Adquisicion •	Adquisicion Eliminar •	Modificar Inventario •	Agregar Inventario •	Inventario Eliminar
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="90">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>adminsistema</t>
+  </si>
+  <si>
+    <t>mshar</t>
   </si>
 </sst>
 </file>
@@ -335,7 +338,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,12 +365,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -583,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -637,9 +634,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -649,8 +645,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -933,9 +928,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,10 +978,10 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="9"/>
@@ -1005,8 +1000,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="29" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="23" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -1033,8 +1028,8 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="29" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="23" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="11"/>
@@ -1053,8 +1048,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="29" t="s">
+      <c r="A5" s="26"/>
+      <c r="B5" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="11"/>
@@ -1071,7 +1066,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="6" t="s">
         <v>45</v>
       </c>
@@ -1089,10 +1084,10 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="24" t="s">
         <v>66</v>
       </c>
       <c r="C7" s="9"/>
@@ -1111,8 +1106,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="25" t="s">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28" t="s">
         <v>67</v>
       </c>
       <c r="C8" s="13"/>
@@ -1131,10 +1126,10 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="24" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1153,8 +1148,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="24" t="s">
+      <c r="A10" s="26"/>
+      <c r="B10" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="11" t="s">
@@ -1181,8 +1176,8 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="24" t="s">
+      <c r="A11" s="26"/>
+      <c r="B11" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -1201,8 +1196,8 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="24" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="11"/>
@@ -1219,8 +1214,8 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="24" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="23" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -1239,7 +1234,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="6" t="s">
         <v>44</v>
       </c>
@@ -1257,10 +1252,10 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="24" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="9"/>
@@ -1279,8 +1274,8 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="24" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="23" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="11" t="s">
@@ -1303,8 +1298,8 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="24" t="s">
+      <c r="A17" s="26"/>
+      <c r="B17" s="23" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="11"/>
@@ -1323,8 +1318,8 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="5" t="s">
+      <c r="A18" s="26"/>
+      <c r="B18" s="23" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="11"/>
@@ -1341,8 +1336,8 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="23" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="11"/>
@@ -1361,7 +1356,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
@@ -1381,8 +1376,8 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="27"/>
+      <c r="B21" s="28" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="13"/>
@@ -1401,7 +1396,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1423,7 +1418,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="5" t="s">
         <v>21</v>
       </c>
@@ -1443,7 +1438,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="5" t="s">
         <v>22</v>
       </c>
@@ -1463,7 +1458,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="28"/>
+      <c r="A25" s="27"/>
       <c r="B25" s="6" t="s">
         <v>23</v>
       </c>
@@ -1481,7 +1476,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="25" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
@@ -1503,7 +1498,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="5" t="s">
         <v>26</v>
       </c>
@@ -1523,7 +1518,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="5" t="s">
         <v>27</v>
       </c>
@@ -1543,7 +1538,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="28"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="6" t="s">
         <v>28</v>
       </c>
@@ -1561,7 +1556,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="25" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -1591,7 +1586,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="5" t="s">
         <v>31</v>
       </c>
@@ -1609,7 +1604,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="5" t="s">
         <v>32</v>
       </c>
@@ -1627,7 +1622,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="5" t="s">
         <v>33</v>
       </c>
@@ -1645,7 +1640,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="28"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="6" t="s">
         <v>43</v>
       </c>
@@ -1663,7 +1658,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="26" t="s">
+      <c r="A35" s="25" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -1683,7 +1678,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="5" t="s">
         <v>36</v>
       </c>
@@ -1711,7 +1706,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="28"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="6" t="s">
         <v>37</v>
       </c>
@@ -1729,7 +1724,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="25" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -1749,7 +1744,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="5" t="s">
         <v>40</v>
       </c>
@@ -1767,7 +1762,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="5" t="s">
         <v>41</v>
       </c>
@@ -1785,7 +1780,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
+      <c r="A41" s="26"/>
       <c r="B41" s="3" t="s">
         <v>79</v>
       </c>
@@ -1809,7 +1804,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="28"/>
+      <c r="A42" s="27"/>
       <c r="B42" s="6" t="s">
         <v>42</v>
       </c>
@@ -1827,7 +1822,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
+      <c r="A43" s="25" t="s">
         <v>46</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -1849,7 +1844,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="27"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="5" t="s">
         <v>48</v>
       </c>
@@ -1869,7 +1864,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="27"/>
+      <c r="A45" s="26"/>
       <c r="B45" s="5" t="s">
         <v>49</v>
       </c>
@@ -1889,7 +1884,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="27"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="3" t="s">
         <v>80</v>
       </c>
@@ -1917,7 +1912,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="28"/>
+      <c r="A47" s="27"/>
       <c r="B47" s="6" t="s">
         <v>50</v>
       </c>
@@ -1937,7 +1932,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
+      <c r="A48" s="25" t="s">
         <v>51</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -1957,7 +1952,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="27"/>
+      <c r="A49" s="26"/>
       <c r="B49" s="5" t="s">
         <v>53</v>
       </c>
@@ -1975,7 +1970,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="27"/>
+      <c r="A50" s="26"/>
       <c r="B50" s="5" t="s">
         <v>54</v>
       </c>
@@ -1993,7 +1988,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="27"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="5" t="s">
         <v>55</v>
       </c>
@@ -2011,7 +2006,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="27"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="3" t="s">
         <v>82</v>
       </c>
@@ -2029,7 +2024,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="28"/>
+      <c r="A53" s="27"/>
       <c r="B53" s="6" t="s">
         <v>68</v>
       </c>
@@ -2059,7 +2054,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="26" t="s">
+      <c r="A54" s="25" t="s">
         <v>56</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -2079,7 +2074,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="28"/>
+      <c r="A55" s="27"/>
       <c r="B55" s="6" t="s">
         <v>58</v>
       </c>
@@ -2117,7 +2112,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="26" t="s">
+      <c r="A57" s="25" t="s">
         <v>61</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -2135,7 +2130,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="27"/>
+      <c r="A58" s="26"/>
       <c r="B58" s="5" t="s">
         <v>63</v>
       </c>
@@ -2151,7 +2146,7 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="27"/>
+      <c r="A59" s="26"/>
       <c r="B59" s="3" t="s">
         <v>81</v>
       </c>
@@ -2167,7 +2162,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="28"/>
+      <c r="A60" s="27"/>
       <c r="B60" s="6" t="s">
         <v>64</v>
       </c>
@@ -2192,6 +2187,9 @@
       <c r="F62" t="s">
         <v>83</v>
       </c>
+      <c r="G62" t="s">
+        <v>89</v>
+      </c>
       <c r="H62" t="s">
         <v>86</v>
       </c>
@@ -2204,6 +2202,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A22:A25"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A37"/>
@@ -2211,12 +2215,6 @@
     <mergeCell ref="A43:A47"/>
     <mergeCell ref="A48:A53"/>
     <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Permisos en Interfaz: •	Adquisicion Eliminar •	Modificar Inventario •	Agregar Inventario •	Inventario Eliminar •	Asignacion Crear •	Asignacion Buscar •	Asignacion Modificar •	Asignacion Eliminar •	Rendicion Crear •	Rendicion Modificar •	Rendicion Eliminar •	Rendicion Buscar •	Buscar Dependencia •	Crear Dependencia •	Modificar Dependencia •	Eliminar Dependencia •	Reactivar Dependencia
Permisos en BLL:
•	Crear Partida
•	Modificar Partida
•	Cancelar Partida
•	Asociar Partida
•	Registrar Adquisicion
•	Buscar Adquisicion
•	Modificar Adquisicion
•	Adquisicion Eliminar
•	Modificar Inventario
•	Agregar Inventario
•	Inventario Eliminar
•	Asignacion Crear
•	Asignacion Buscar
•	Asignacion Modificar
•	Asignacion Eliminar
•	Rendicion Crear
•	Rendicion Modificar
•	Rendicion Eliminar
•	Rendicion Buscar
•	Crear Dependencia
•	Modificar Dependencia
•	Eliminar Dependencia
•	Reactivar Dependencia
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -636,6 +636,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -645,7 +646,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -929,8 +929,8 @@
   <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G53" sqref="G53"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,7 +978,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -1000,7 +1000,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="23" t="s">
         <v>2</v>
       </c>
@@ -1028,7 +1028,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="23" t="s">
         <v>3</v>
       </c>
@@ -1048,7 +1048,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="23" t="s">
         <v>4</v>
       </c>
@@ -1066,7 +1066,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="6" t="s">
         <v>45</v>
       </c>
@@ -1084,7 +1084,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>65</v>
       </c>
       <c r="B7" s="24" t="s">
@@ -1106,8 +1106,8 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27"/>
-      <c r="B8" s="28" t="s">
+      <c r="A8" s="28"/>
+      <c r="B8" s="25" t="s">
         <v>67</v>
       </c>
       <c r="C8" s="13"/>
@@ -1126,7 +1126,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="24" t="s">
@@ -1148,7 +1148,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="23" t="s">
         <v>7</v>
       </c>
@@ -1176,7 +1176,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="23" t="s">
         <v>8</v>
       </c>
@@ -1196,7 +1196,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="23" t="s">
         <v>9</v>
       </c>
@@ -1214,7 +1214,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="23" t="s">
         <v>10</v>
       </c>
@@ -1234,7 +1234,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="6" t="s">
         <v>44</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="26" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="24" t="s">
@@ -1274,7 +1274,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="23" t="s">
         <v>12</v>
       </c>
@@ -1298,7 +1298,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="23" t="s">
         <v>13</v>
       </c>
@@ -1318,7 +1318,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="23" t="s">
         <v>14</v>
       </c>
@@ -1336,7 +1336,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="23" t="s">
         <v>15</v>
       </c>
@@ -1356,8 +1356,8 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="27"/>
+      <c r="B20" s="23" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="11"/>
@@ -1376,8 +1376,8 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="27"/>
-      <c r="B21" s="28" t="s">
+      <c r="A21" s="28"/>
+      <c r="B21" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="13"/>
@@ -1396,10 +1396,10 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="24" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="9"/>
@@ -1418,8 +1418,8 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="27"/>
+      <c r="B23" s="23" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="11"/>
@@ -1438,8 +1438,8 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="5" t="s">
+      <c r="A24" s="27"/>
+      <c r="B24" s="23" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="11"/>
@@ -1458,8 +1458,8 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="27"/>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="28"/>
+      <c r="B25" s="25" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="13"/>
@@ -1476,10 +1476,10 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="9" t="s">
@@ -1498,8 +1498,8 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="5" t="s">
+      <c r="A27" s="27"/>
+      <c r="B27" s="23" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -1518,8 +1518,8 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="5" t="s">
+      <c r="A28" s="27"/>
+      <c r="B28" s="23" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -1538,8 +1538,8 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="27"/>
-      <c r="B29" s="6" t="s">
+      <c r="A29" s="28"/>
+      <c r="B29" s="25" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="13"/>
@@ -1556,10 +1556,10 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="24" t="s">
         <v>30</v>
       </c>
       <c r="C30" s="9" t="s">
@@ -1586,8 +1586,8 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
-      <c r="B31" s="5" t="s">
+      <c r="A31" s="27"/>
+      <c r="B31" s="23" t="s">
         <v>31</v>
       </c>
       <c r="C31" s="11"/>
@@ -1604,8 +1604,8 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="27"/>
+      <c r="B32" s="23" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="11"/>
@@ -1622,8 +1622,8 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="5" t="s">
+      <c r="A33" s="27"/>
+      <c r="B33" s="23" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="11"/>
@@ -1640,8 +1640,8 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="27"/>
-      <c r="B34" s="6" t="s">
+      <c r="A34" s="28"/>
+      <c r="B34" s="25" t="s">
         <v>43</v>
       </c>
       <c r="C34" s="13"/>
@@ -1658,7 +1658,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="26" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
@@ -1678,7 +1678,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="5" t="s">
         <v>36</v>
       </c>
@@ -1706,7 +1706,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="27"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="6" t="s">
         <v>37</v>
       </c>
@@ -1724,7 +1724,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="26" t="s">
         <v>38</v>
       </c>
       <c r="B38" s="4" t="s">
@@ -1744,7 +1744,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="26"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="5" t="s">
         <v>40</v>
       </c>
@@ -1762,7 +1762,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
+      <c r="A40" s="27"/>
       <c r="B40" s="5" t="s">
         <v>41</v>
       </c>
@@ -1780,7 +1780,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
+      <c r="A41" s="27"/>
       <c r="B41" s="3" t="s">
         <v>79</v>
       </c>
@@ -1804,7 +1804,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="27"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="6" t="s">
         <v>42</v>
       </c>
@@ -1822,7 +1822,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="26" t="s">
         <v>46</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -1844,7 +1844,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
+      <c r="A44" s="27"/>
       <c r="B44" s="5" t="s">
         <v>48</v>
       </c>
@@ -1864,7 +1864,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="26"/>
+      <c r="A45" s="27"/>
       <c r="B45" s="5" t="s">
         <v>49</v>
       </c>
@@ -1884,7 +1884,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
+      <c r="A46" s="27"/>
       <c r="B46" s="3" t="s">
         <v>80</v>
       </c>
@@ -1912,7 +1912,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="27"/>
+      <c r="A47" s="28"/>
       <c r="B47" s="6" t="s">
         <v>50</v>
       </c>
@@ -1932,7 +1932,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="26" t="s">
         <v>51</v>
       </c>
       <c r="B48" s="4" t="s">
@@ -1952,7 +1952,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="26"/>
+      <c r="A49" s="27"/>
       <c r="B49" s="5" t="s">
         <v>53</v>
       </c>
@@ -1970,7 +1970,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
+      <c r="A50" s="27"/>
       <c r="B50" s="5" t="s">
         <v>54</v>
       </c>
@@ -1988,7 +1988,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="26"/>
+      <c r="A51" s="27"/>
       <c r="B51" s="5" t="s">
         <v>55</v>
       </c>
@@ -2006,7 +2006,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="26"/>
+      <c r="A52" s="27"/>
       <c r="B52" s="3" t="s">
         <v>82</v>
       </c>
@@ -2024,7 +2024,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="27"/>
+      <c r="A53" s="28"/>
       <c r="B53" s="6" t="s">
         <v>68</v>
       </c>
@@ -2054,7 +2054,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="s">
+      <c r="A54" s="26" t="s">
         <v>56</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -2074,7 +2074,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="27"/>
+      <c r="A55" s="28"/>
       <c r="B55" s="6" t="s">
         <v>58</v>
       </c>
@@ -2112,7 +2112,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="25" t="s">
+      <c r="A57" s="26" t="s">
         <v>61</v>
       </c>
       <c r="B57" s="4" t="s">
@@ -2130,7 +2130,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="26"/>
+      <c r="A58" s="27"/>
       <c r="B58" s="5" t="s">
         <v>63</v>
       </c>
@@ -2146,7 +2146,7 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="26"/>
+      <c r="A59" s="27"/>
       <c r="B59" s="3" t="s">
         <v>81</v>
       </c>
@@ -2162,7 +2162,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="27"/>
+      <c r="A60" s="28"/>
       <c r="B60" s="6" t="s">
         <v>64</v>
       </c>
@@ -2202,12 +2202,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A22:A25"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A37"/>
@@ -2215,6 +2209,12 @@
     <mergeCell ref="A43:A47"/>
     <mergeCell ref="A48:A53"/>
     <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#Casos de uso agregados: - USC XX Buscar Solicitud.docx - USC XX Modificar Solicitud.docx (Sin terminar) - X Registrar Adquisicion.docx
#Mejoría en Registrar Adquisición (Software)
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -662,6 +662,32 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -670,32 +696,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -979,9 +979,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B54" sqref="B54:J54"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1003,7 @@
       <c r="B1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="30" t="s">
         <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1029,13 +1029,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="29"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
         <v>69</v>
@@ -1051,11 +1051,11 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="29" t="s">
         <v>69</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -1079,11 +1079,11 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="32"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
         <v>69</v>
@@ -1099,11 +1099,11 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="32"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
@@ -1117,11 +1117,11 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28"/>
-      <c r="B6" s="36" t="s">
+      <c r="A6" s="38"/>
+      <c r="B6" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="30"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
@@ -1135,15 +1135,15 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="36" t="s">
         <v>65</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="29"/>
+      <c r="C7" s="26"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="26" t="s">
         <v>69</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -1157,13 +1157,13 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="27" t="s">
         <v>69</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -1177,20 +1177,20 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="36" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="29" t="s">
+      <c r="C9" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="26" t="s">
         <v>69</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="28" t="s">
         <v>69</v>
       </c>
       <c r="G9" s="5"/>
@@ -1201,11 +1201,11 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="29" t="s">
         <v>69</v>
       </c>
       <c r="D10" s="7" t="s">
@@ -1229,18 +1229,18 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="32" t="s">
+      <c r="C11" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="29" t="s">
         <v>69</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="28" t="s">
         <v>69</v>
       </c>
       <c r="G11" s="7"/>
@@ -1251,11 +1251,11 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="37"/>
       <c r="B12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="32"/>
+      <c r="C12" s="29"/>
       <c r="D12" s="7" t="s">
         <v>69</v>
       </c>
@@ -1269,11 +1269,11 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="29" t="s">
         <v>69</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -1289,12 +1289,12 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
-      <c r="B14" s="36" t="s">
+      <c r="A14" s="38"/>
+      <c r="B14" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="37" t="s">
+      <c r="C14" s="27"/>
+      <c r="D14" s="34" t="s">
         <v>69</v>
       </c>
       <c r="E14" s="9"/>
@@ -1307,13 +1307,13 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="29"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -1329,11 +1329,11 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="29" t="s">
         <v>69</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -1353,11 +1353,11 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="32"/>
+      <c r="C17" s="29"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -1373,11 +1373,11 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="32"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -1391,11 +1391,11 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="32"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -1411,11 +1411,11 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="32"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -1431,11 +1431,11 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
+      <c r="A21" s="38"/>
       <c r="B21" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="30"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -1451,13 +1451,13 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="36" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="29"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1473,11 +1473,11 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
+      <c r="A23" s="37"/>
       <c r="B23" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="32"/>
+      <c r="C23" s="29"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -1493,11 +1493,11 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="32"/>
+      <c r="C24" s="29"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -1513,11 +1513,11 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="28"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="30"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
@@ -1531,13 +1531,13 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="36" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="26" t="s">
         <v>69</v>
       </c>
       <c r="D26" s="5" t="s">
@@ -1553,11 +1553,11 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
+      <c r="A27" s="37"/>
       <c r="B27" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="29" t="s">
         <v>69</v>
       </c>
       <c r="D27" s="7" t="s">
@@ -1573,11 +1573,11 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
+      <c r="A28" s="37"/>
       <c r="B28" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="29" t="s">
         <v>69</v>
       </c>
       <c r="D28" s="7" t="s">
@@ -1593,11 +1593,11 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="28"/>
+      <c r="A29" s="38"/>
       <c r="B29" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="30"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="9" t="s">
         <v>69</v>
       </c>
@@ -1611,13 +1611,13 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="26" t="s">
         <v>69</v>
       </c>
       <c r="D30" s="5" t="s">
@@ -1641,16 +1641,16 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="32"/>
+      <c r="C31" s="29"/>
       <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="E31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
@@ -1659,16 +1659,16 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
+      <c r="A32" s="37"/>
       <c r="B32" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="32"/>
+      <c r="C32" s="29"/>
       <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="E32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="7"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
@@ -1677,16 +1677,16 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
+      <c r="A33" s="37"/>
       <c r="B33" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="32"/>
+      <c r="C33" s="29"/>
       <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="E33" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" s="7"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
@@ -1695,16 +1695,16 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="28"/>
+      <c r="A34" s="38"/>
       <c r="B34" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="30"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9" t="s">
-        <v>69</v>
-      </c>
+      <c r="E34" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
@@ -1713,13 +1713,13 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="26" t="s">
+      <c r="A35" s="36" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="29"/>
+      <c r="C35" s="26"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5" t="s">
@@ -1733,11 +1733,11 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
+      <c r="A36" s="37"/>
       <c r="B36" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="29" t="s">
         <v>69</v>
       </c>
       <c r="D36" s="7" t="s">
@@ -1761,11 +1761,11 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="27"/>
+      <c r="A37" s="37"/>
       <c r="B37" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="34"/>
+      <c r="C37" s="31"/>
       <c r="D37" s="22"/>
       <c r="E37" s="22"/>
       <c r="F37" s="22" t="s">
@@ -1779,11 +1779,11 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="28"/>
+      <c r="A38" s="38"/>
       <c r="B38" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="30"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
       <c r="F38" s="9" t="s">
@@ -1797,13 +1797,13 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
+      <c r="A39" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="29"/>
+      <c r="C39" s="26"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5" t="s">
@@ -1817,11 +1817,11 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
+      <c r="A40" s="37"/>
       <c r="B40" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="32"/>
+      <c r="C40" s="29"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="7" t="s">
@@ -1835,11 +1835,11 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
+      <c r="A41" s="37"/>
       <c r="B41" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="32"/>
+      <c r="C41" s="29"/>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7" t="s">
@@ -1853,11 +1853,11 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
+      <c r="A42" s="37"/>
       <c r="B42" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="34"/>
+      <c r="C42" s="31"/>
       <c r="D42" s="11"/>
       <c r="E42" s="11" t="s">
         <v>69</v>
@@ -1877,11 +1877,11 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="28"/>
+      <c r="A43" s="38"/>
       <c r="B43" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="30"/>
+      <c r="C43" s="27"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
       <c r="F43" s="9" t="s">
@@ -1895,13 +1895,13 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="36" t="s">
         <v>46</v>
       </c>
       <c r="B44" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="29"/>
+      <c r="C44" s="26"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5" t="s">
@@ -1917,11 +1917,11 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="27"/>
+      <c r="A45" s="37"/>
       <c r="B45" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="32"/>
+      <c r="C45" s="29"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
       <c r="F45" s="7" t="s">
@@ -1937,11 +1937,11 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="27"/>
+      <c r="A46" s="37"/>
       <c r="B46" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="32"/>
+      <c r="C46" s="29"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7" t="s">
@@ -1957,11 +1957,11 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="27"/>
+      <c r="A47" s="37"/>
       <c r="B47" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="34" t="s">
+      <c r="C47" s="31" t="s">
         <v>69</v>
       </c>
       <c r="D47" s="11" t="s">
@@ -1985,11 +1985,11 @@
       </c>
     </row>
     <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="28"/>
+      <c r="A48" s="38"/>
       <c r="B48" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="30"/>
+      <c r="C48" s="27"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
       <c r="F48" s="9" t="s">
@@ -2005,13 +2005,13 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="36" t="s">
         <v>51</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="29"/>
+      <c r="C49" s="26"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -2025,11 +2025,11 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="27"/>
+      <c r="A50" s="37"/>
       <c r="B50" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="32"/>
+      <c r="C50" s="29"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
@@ -2043,11 +2043,11 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="27"/>
+      <c r="A51" s="37"/>
       <c r="B51" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="32"/>
+      <c r="C51" s="29"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -2061,11 +2061,11 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="27"/>
+      <c r="A52" s="37"/>
       <c r="B52" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="32"/>
+      <c r="C52" s="29"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
@@ -2079,11 +2079,11 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="27"/>
+      <c r="A53" s="37"/>
       <c r="B53" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="34"/>
+      <c r="C53" s="31"/>
       <c r="D53" s="11"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
@@ -2097,43 +2097,43 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="28"/>
-      <c r="B54" s="36" t="s">
+      <c r="A54" s="38"/>
+      <c r="B54" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C54" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="D54" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="E54" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="F54" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="G54" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="H54" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="I54" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="J54" s="38" t="s">
+      <c r="C54" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E54" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="F54" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="G54" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="H54" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="I54" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="J54" s="35" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="26" t="s">
+      <c r="A55" s="36" t="s">
         <v>56</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="29"/>
+      <c r="C55" s="26"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
@@ -2147,11 +2147,11 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="28"/>
+      <c r="A56" s="38"/>
       <c r="B56" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="30"/>
+      <c r="C56" s="27"/>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
@@ -2171,7 +2171,7 @@
       <c r="B57" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C57" s="35"/>
+      <c r="C57" s="32"/>
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
       <c r="F57" s="16"/>
@@ -2185,13 +2185,13 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="26" t="s">
+      <c r="A58" s="36" t="s">
         <v>61</v>
       </c>
       <c r="B58" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C58" s="29"/>
+      <c r="C58" s="26"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
@@ -2203,11 +2203,11 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="27"/>
+      <c r="A59" s="37"/>
       <c r="B59" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C59" s="32"/>
+      <c r="C59" s="29"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
@@ -2219,11 +2219,11 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="27"/>
+      <c r="A60" s="37"/>
       <c r="B60" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C60" s="34"/>
+      <c r="C60" s="31"/>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>
@@ -2235,11 +2235,11 @@
       </c>
     </row>
     <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="28"/>
+      <c r="A61" s="38"/>
       <c r="B61" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C61" s="30"/>
+      <c r="C61" s="27"/>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
       <c r="F61" s="9"/>
@@ -2275,6 +2275,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A22:A25"/>
     <mergeCell ref="A58:A61"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A38"/>
@@ -2282,12 +2288,6 @@
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A49:A54"/>
     <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#Casos de uso - SC013 - Buscar Agente.docx - SC015 - Modificar Agente.docx - SC005 - Solicitar Cotizacion.docx
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="141">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -297,6 +297,156 @@
   </si>
   <si>
     <t>Adquisiciones y Asignacion Admin (Compras Jefe)</t>
+  </si>
+  <si>
+    <t>SC001</t>
+  </si>
+  <si>
+    <t>SC002</t>
+  </si>
+  <si>
+    <t>SC003</t>
+  </si>
+  <si>
+    <t>SC004</t>
+  </si>
+  <si>
+    <t>SC005</t>
+  </si>
+  <si>
+    <t>SC006</t>
+  </si>
+  <si>
+    <t>IG001</t>
+  </si>
+  <si>
+    <t>IG002</t>
+  </si>
+  <si>
+    <t>IG003</t>
+  </si>
+  <si>
+    <t>IG004</t>
+  </si>
+  <si>
+    <t>IG005</t>
+  </si>
+  <si>
+    <t>IG006</t>
+  </si>
+  <si>
+    <t>IG007</t>
+  </si>
+  <si>
+    <t>IG008</t>
+  </si>
+  <si>
+    <t>IG009</t>
+  </si>
+  <si>
+    <t>AA001</t>
+  </si>
+  <si>
+    <t>AA002</t>
+  </si>
+  <si>
+    <t>AA003</t>
+  </si>
+  <si>
+    <t>AA004</t>
+  </si>
+  <si>
+    <t>AA005</t>
+  </si>
+  <si>
+    <t>AA006</t>
+  </si>
+  <si>
+    <t>AA007</t>
+  </si>
+  <si>
+    <t>AA008</t>
+  </si>
+  <si>
+    <t>AA009</t>
+  </si>
+  <si>
+    <t>AA010</t>
+  </si>
+  <si>
+    <t>AA011</t>
+  </si>
+  <si>
+    <t>SC007</t>
+  </si>
+  <si>
+    <t>SC008</t>
+  </si>
+  <si>
+    <t>SC009</t>
+  </si>
+  <si>
+    <t>SC010</t>
+  </si>
+  <si>
+    <t>SC011</t>
+  </si>
+  <si>
+    <t>SC012</t>
+  </si>
+  <si>
+    <t>SC013</t>
+  </si>
+  <si>
+    <t>SC014</t>
+  </si>
+  <si>
+    <t>SC015</t>
+  </si>
+  <si>
+    <t>SC016</t>
+  </si>
+  <si>
+    <t>SC017</t>
+  </si>
+  <si>
+    <t>SC018</t>
+  </si>
+  <si>
+    <t>SC019</t>
+  </si>
+  <si>
+    <t>SC020</t>
+  </si>
+  <si>
+    <t>SC021</t>
+  </si>
+  <si>
+    <t>SC022</t>
+  </si>
+  <si>
+    <t>SC023</t>
+  </si>
+  <si>
+    <t>SC024</t>
+  </si>
+  <si>
+    <t>SC025</t>
+  </si>
+  <si>
+    <t>AD001</t>
+  </si>
+  <si>
+    <t>AD002</t>
+  </si>
+  <si>
+    <t>AD003</t>
+  </si>
+  <si>
+    <t>AD004</t>
+  </si>
+  <si>
+    <t>AD005</t>
   </si>
 </sst>
 </file>
@@ -341,7 +491,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,6 +540,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -601,7 +757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -697,6 +853,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -977,88 +1134,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="36" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
-        <v>69</v>
-      </c>
+      <c r="C2" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="26"/>
+      <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="J2" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="5"/>
+      <c r="K2" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37"/>
       <c r="B3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="29" t="s">
         <v>69</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -1073,142 +1235,161 @@
       <c r="H3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="37"/>
       <c r="B4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="C4" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="7"/>
+      <c r="K4" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="37"/>
       <c r="B5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="7"/>
+      <c r="C5" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="29"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="7"/>
+      <c r="K5" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="38"/>
       <c r="B6" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="9"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="9"/>
+      <c r="K6" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
         <v>65</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="5"/>
+      <c r="C7" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J7" s="5"/>
+      <c r="K7" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="38"/>
       <c r="B8" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="9"/>
+      <c r="C8" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
-      <c r="J8" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" s="9"/>
+      <c r="K8" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>69</v>
+      <c r="C9" s="39" t="s">
+        <v>97</v>
       </c>
       <c r="D9" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" s="5"/>
+      <c r="E9" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="28" t="s">
+        <v>69</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="5"/>
+      <c r="K9" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="37"/>
       <c r="B10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="29" t="s">
         <v>69</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -1223,404 +1404,462 @@
       <c r="H10" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="37"/>
       <c r="B11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>69</v>
+      <c r="C11" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="7"/>
+      <c r="E11" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="28" t="s">
+        <v>69</v>
+      </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J11" s="7"/>
+      <c r="K11" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="37"/>
       <c r="B12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="7"/>
+      <c r="C12" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" s="7"/>
+      <c r="K12" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="37"/>
       <c r="B13" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="7"/>
+      <c r="C13" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="7"/>
+      <c r="K13" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38"/>
       <c r="B14" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="9"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="34" t="s">
+        <v>69</v>
+      </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14" s="9"/>
+      <c r="K14" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="26"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="5" t="s">
-        <v>69</v>
-      </c>
+      <c r="G15" s="5"/>
       <c r="H15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="37"/>
       <c r="B16" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="7"/>
+      <c r="C16" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="F16" s="7"/>
-      <c r="G16" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="G16" s="7"/>
       <c r="H16" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I16" s="7"/>
-      <c r="J16" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16" s="7"/>
+      <c r="K16" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="37"/>
       <c r="B17" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="7"/>
+      <c r="C17" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="29"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="G17" s="7"/>
       <c r="H17" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I17" s="7"/>
-      <c r="J17" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="37"/>
       <c r="B18" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="7"/>
+      <c r="C18" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="29"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I18" s="7"/>
-      <c r="J18" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H18" s="7"/>
+      <c r="I18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J18" s="7"/>
+      <c r="K18" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="37"/>
       <c r="B19" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="7"/>
+      <c r="C19" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="29"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="G19" s="7"/>
       <c r="H19" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I19" s="7"/>
-      <c r="J19" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J19" s="7"/>
+      <c r="K19" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37"/>
       <c r="B20" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="7"/>
+      <c r="C20" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="29"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="G20" s="7"/>
       <c r="H20" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I20" s="7"/>
-      <c r="J20" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J20" s="7"/>
+      <c r="K20" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="38"/>
       <c r="B21" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="9"/>
+      <c r="C21" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" s="27"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="9" t="s">
-        <v>69</v>
-      </c>
+      <c r="G21" s="9"/>
       <c r="H21" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="I21" s="9"/>
-      <c r="J21" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I21" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J21" s="9"/>
+      <c r="K21" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="36" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="5"/>
+      <c r="C22" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="26"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="5" t="s">
-        <v>69</v>
-      </c>
+      <c r="G22" s="5"/>
       <c r="H22" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J22" s="5"/>
+      <c r="K22" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="37"/>
       <c r="B23" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="7"/>
+      <c r="C23" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="29"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="G23" s="7"/>
       <c r="H23" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J23" s="7"/>
+      <c r="K23" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="37"/>
       <c r="B24" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="7"/>
+      <c r="C24" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="29"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="7" t="s">
-        <v>69</v>
-      </c>
+      <c r="G24" s="7"/>
       <c r="H24" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I24" s="7"/>
-      <c r="J24" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J24" s="7"/>
+      <c r="K24" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="38"/>
       <c r="B25" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="9"/>
+      <c r="C25" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="27"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I25" s="9"/>
-      <c r="J25" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H25" s="9"/>
+      <c r="I25" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J25" s="9"/>
+      <c r="K25" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="36" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="5"/>
+      <c r="C26" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
-      <c r="J26" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J26" s="5"/>
+      <c r="K26" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37"/>
       <c r="B27" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="7"/>
+      <c r="C27" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
-      <c r="J27" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J27" s="7"/>
+      <c r="K27" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37"/>
       <c r="B28" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" s="7"/>
+      <c r="C28" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
-      <c r="J28" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J28" s="7"/>
+      <c r="K28" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="38"/>
       <c r="B29" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" s="9"/>
+      <c r="C29" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="27"/>
+      <c r="E29" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J29" s="9"/>
+      <c r="K29" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="5" t="s">
+      <c r="C30" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="26" t="s">
         <v>69</v>
       </c>
       <c r="E30" s="5" t="s">
@@ -1635,112 +1874,130 @@
       <c r="H30" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I30" s="5"/>
-      <c r="J30" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I30" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="37"/>
       <c r="B31" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F31" s="7"/>
+      <c r="C31" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="29"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
-      <c r="J31" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J31" s="7"/>
+      <c r="K31" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="37"/>
       <c r="B32" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="29"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="7"/>
+      <c r="C32" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="D32" s="29"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
-      <c r="J32" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J32" s="7"/>
+      <c r="K32" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="37"/>
       <c r="B33" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="29"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F33" s="7"/>
+      <c r="C33" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="29"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
-      <c r="J33" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J33" s="7"/>
+      <c r="K33" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F34" s="9"/>
+      <c r="C34" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="27"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
       <c r="I34" s="9"/>
-      <c r="J34" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J34" s="9"/>
+      <c r="K34" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="36" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="5"/>
+      <c r="C35" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" s="26"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
-      <c r="J35" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J35" s="5"/>
+      <c r="K35" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="37"/>
       <c r="B36" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="7" t="s">
+      <c r="C36" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="29" t="s">
         <v>69</v>
       </c>
       <c r="E36" s="7" t="s">
@@ -1755,113 +2012,131 @@
       <c r="H36" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="I36" s="7"/>
-      <c r="J36" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I36" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J36" s="7"/>
+      <c r="K36" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="37"/>
       <c r="B37" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="22"/>
+      <c r="C37" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37" s="31"/>
       <c r="E37" s="22"/>
-      <c r="F37" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="G37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22" t="s">
+        <v>69</v>
+      </c>
       <c r="H37" s="22"/>
       <c r="I37" s="22"/>
-      <c r="J37" s="23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J37" s="22"/>
+      <c r="K37" s="23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="38"/>
       <c r="B38" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="27"/>
-      <c r="D38" s="9"/>
+      <c r="C38" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" s="27"/>
       <c r="E38" s="9"/>
-      <c r="F38" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
-      <c r="J38" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J38" s="9"/>
+      <c r="K38" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="5"/>
+      <c r="C39" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="D39" s="26"/>
       <c r="E39" s="5"/>
-      <c r="F39" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
-      <c r="J39" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J39" s="5"/>
+      <c r="K39" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="37"/>
       <c r="B40" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="7"/>
+      <c r="C40" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="29"/>
       <c r="E40" s="7"/>
-      <c r="F40" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
-      <c r="J40" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J40" s="7"/>
+      <c r="K40" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="37"/>
       <c r="B41" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="29"/>
-      <c r="D41" s="7"/>
+      <c r="C41" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="29"/>
       <c r="E41" s="7"/>
-      <c r="F41" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
-      <c r="J41" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J41" s="7"/>
+      <c r="K41" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="37"/>
       <c r="B42" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11" t="s">
-        <v>69</v>
-      </c>
+      <c r="C42" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="31"/>
+      <c r="E42" s="11"/>
       <c r="F42" s="11" t="s">
         <v>69</v>
       </c>
@@ -1871,100 +2146,115 @@
       <c r="H42" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="I42" s="11"/>
-      <c r="J42" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I42" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J42" s="11"/>
+      <c r="K42" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="38"/>
       <c r="B43" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="27"/>
-      <c r="D43" s="9"/>
+      <c r="C43" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="D43" s="27"/>
       <c r="E43" s="9"/>
-      <c r="F43" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G43" s="13"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="H43" s="13"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I43" s="13"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="36" t="s">
         <v>46</v>
       </c>
       <c r="B44" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="26"/>
-      <c r="D44" s="5"/>
+      <c r="C44" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" s="26"/>
       <c r="E44" s="5"/>
-      <c r="F44" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="I44" s="5"/>
-      <c r="J44" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F44" s="5"/>
+      <c r="G44" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J44" s="5"/>
+      <c r="K44" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="37"/>
       <c r="B45" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="29"/>
-      <c r="D45" s="7"/>
+      <c r="C45" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="29"/>
       <c r="E45" s="7"/>
-      <c r="F45" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="I45" s="7"/>
-      <c r="J45" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F45" s="7"/>
+      <c r="G45" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J45" s="7"/>
+      <c r="K45" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="37"/>
       <c r="B46" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="29"/>
-      <c r="D46" s="7"/>
+      <c r="C46" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="D46" s="29"/>
       <c r="E46" s="7"/>
-      <c r="F46" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="I46" s="7"/>
-      <c r="J46" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F46" s="7"/>
+      <c r="G46" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J46" s="7"/>
+      <c r="K46" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="37"/>
       <c r="B47" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="D47" s="11" t="s">
+      <c r="C47" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D47" s="31" t="s">
         <v>69</v>
       </c>
       <c r="E47" s="11" t="s">
@@ -1979,131 +2269,150 @@
       <c r="H47" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="I47" s="11"/>
-      <c r="J47" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I47" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J47" s="11"/>
+      <c r="K47" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="38"/>
       <c r="B48" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="27"/>
-      <c r="D48" s="9"/>
+      <c r="C48" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" s="27"/>
       <c r="E48" s="9"/>
-      <c r="F48" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I48" s="9"/>
-      <c r="J48" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F48" s="9"/>
+      <c r="G48" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J48" s="9"/>
+      <c r="K48" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="36" t="s">
         <v>51</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="26"/>
-      <c r="D49" s="5"/>
+      <c r="C49" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" s="26"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
-      <c r="I49" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J49" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I49" s="5"/>
+      <c r="J49" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K49" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="37"/>
       <c r="B50" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="7"/>
+      <c r="C50" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="D50" s="29"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
-      <c r="I50" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="J50" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I50" s="7"/>
+      <c r="J50" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K50" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="37"/>
       <c r="B51" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="29"/>
-      <c r="D51" s="7"/>
+      <c r="C51" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="D51" s="29"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
-      <c r="I51" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="J51" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I51" s="7"/>
+      <c r="J51" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K51" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="37"/>
       <c r="B52" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="29"/>
-      <c r="D52" s="7"/>
+      <c r="C52" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="D52" s="29"/>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
-      <c r="I52" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="J52" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I52" s="7"/>
+      <c r="J52" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="37"/>
       <c r="B53" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="31"/>
-      <c r="D53" s="11"/>
+      <c r="C53" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="D53" s="31"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
-      <c r="I53" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="J53" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I53" s="11"/>
+      <c r="J53" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K53" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="38"/>
       <c r="B54" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C54" s="34" t="s">
-        <v>69</v>
-      </c>
+      <c r="C54" s="33"/>
       <c r="D54" s="34" t="s">
         <v>69</v>
       </c>
@@ -2122,165 +2431,169 @@
       <c r="I54" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="J54" s="35" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J54" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="K54" s="35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="36" t="s">
         <v>56</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="26"/>
-      <c r="D55" s="5"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="26"/>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
-      <c r="I55" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J55" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I55" s="5"/>
+      <c r="J55" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="38"/>
       <c r="B56" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="27"/>
-      <c r="D56" s="9"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="27"/>
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
-      <c r="I56" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="J56" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I56" s="9"/>
+      <c r="J56" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K56" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>59</v>
       </c>
       <c r="B57" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C57" s="32"/>
-      <c r="D57" s="16"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="32"/>
       <c r="E57" s="16"/>
       <c r="F57" s="16"/>
       <c r="G57" s="16"/>
       <c r="H57" s="16"/>
-      <c r="I57" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="J57" s="17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I57" s="16"/>
+      <c r="J57" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K57" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="36" t="s">
         <v>61</v>
       </c>
       <c r="B58" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C58" s="26"/>
-      <c r="D58" s="5"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="26"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
-      <c r="J58" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J58" s="5"/>
+      <c r="K58" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="37"/>
       <c r="B59" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C59" s="29"/>
-      <c r="D59" s="7"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="29"/>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
-      <c r="J59" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J59" s="7"/>
+      <c r="K59" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="37"/>
       <c r="B60" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C60" s="31"/>
-      <c r="D60" s="11"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="31"/>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>
       <c r="G60" s="11"/>
       <c r="H60" s="11"/>
       <c r="I60" s="11"/>
-      <c r="J60" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J60" s="11"/>
+      <c r="K60" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="38"/>
       <c r="B61" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C61" s="27"/>
-      <c r="D61" s="9"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="27"/>
       <c r="E61" s="9"/>
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
       <c r="I61" s="9"/>
-      <c r="J61" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D63" t="s">
+      <c r="J61" s="9"/>
+      <c r="K61" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
         <v>78</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>79</v>
       </c>
-      <c r="F63" t="s">
+      <c r="G63" t="s">
         <v>77</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>83</v>
       </c>
-      <c r="H63" t="s">
+      <c r="I63" t="s">
         <v>80</v>
       </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
         <v>82</v>
       </c>
-      <c r="J63" s="18" t="s">
+      <c r="K63" s="18" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A22:A25"/>
     <mergeCell ref="A58:A61"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A38"/>
@@ -2288,6 +2601,12 @@
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A49:A54"/>
     <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Casos de uso: - Casos uso/SC001 - Crear Solicitud.docx (Modif por extensión de adjuntos) - Casos uso/SC005 - Solicitar Cotizacion.docx (Modif una linea) - Casos uso/SC006 - Agregar Cotizacion.docx
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -844,6 +844,7 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -853,7 +854,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1137,8 +1137,8 @@
   <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,13 +1188,13 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="36" t="s">
         <v>91</v>
       </c>
       <c r="D2" s="26"/>
@@ -1213,11 +1213,11 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37"/>
+      <c r="A3" s="38"/>
       <c r="B3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="36" t="s">
         <v>92</v>
       </c>
       <c r="D3" s="29" t="s">
@@ -1244,11 +1244,11 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="36" t="s">
         <v>93</v>
       </c>
       <c r="D4" s="29"/>
@@ -1267,11 +1267,11 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="36" t="s">
         <v>94</v>
       </c>
       <c r="D5" s="29"/>
@@ -1288,7 +1288,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="33" t="s">
         <v>45</v>
       </c>
@@ -1307,13 +1307,13 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="36" t="s">
         <v>95</v>
       </c>
       <c r="D7" s="26"/>
@@ -1332,11 +1332,11 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="36" t="s">
         <v>96</v>
       </c>
       <c r="D8" s="27"/>
@@ -1355,13 +1355,13 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="36" t="s">
         <v>97</v>
       </c>
       <c r="D9" s="26" t="s">
@@ -1382,11 +1382,11 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="36" t="s">
         <v>98</v>
       </c>
       <c r="D10" s="29" t="s">
@@ -1413,7 +1413,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="19" t="s">
         <v>8</v>
       </c>
@@ -1438,11 +1438,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="36" t="s">
         <v>100</v>
       </c>
       <c r="D12" s="29"/>
@@ -1459,11 +1459,11 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="36" t="s">
         <v>101</v>
       </c>
       <c r="D13" s="29" t="s">
@@ -1482,7 +1482,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="33" t="s">
         <v>44</v>
       </c>
@@ -1501,13 +1501,13 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="37" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="36" t="s">
         <v>106</v>
       </c>
       <c r="D15" s="26"/>
@@ -1526,11 +1526,11 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="36" t="s">
         <v>107</v>
       </c>
       <c r="D16" s="29" t="s">
@@ -1553,7 +1553,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="19" t="s">
         <v>13</v>
       </c>
@@ -1576,7 +1576,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="19" t="s">
         <v>14</v>
       </c>
@@ -1597,7 +1597,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
+      <c r="A19" s="38"/>
       <c r="B19" s="19" t="s">
         <v>15</v>
       </c>
@@ -1620,7 +1620,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="37"/>
+      <c r="A20" s="38"/>
       <c r="B20" s="19" t="s">
         <v>16</v>
       </c>
@@ -1643,7 +1643,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="38"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="21" t="s">
         <v>18</v>
       </c>
@@ -1666,7 +1666,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="37" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="20" t="s">
@@ -1691,11 +1691,11 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="37"/>
+      <c r="A23" s="38"/>
       <c r="B23" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="36" t="s">
         <v>114</v>
       </c>
       <c r="D23" s="29"/>
@@ -1714,7 +1714,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="37"/>
+      <c r="A24" s="38"/>
       <c r="B24" s="19" t="s">
         <v>22</v>
       </c>
@@ -1737,7 +1737,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="38"/>
+      <c r="A25" s="39"/>
       <c r="B25" s="21" t="s">
         <v>23</v>
       </c>
@@ -1758,13 +1758,13 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="37" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="C26" s="36" t="s">
         <v>102</v>
       </c>
       <c r="D26" s="26" t="s">
@@ -1783,11 +1783,11 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="37"/>
+      <c r="A27" s="38"/>
       <c r="B27" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="36" t="s">
         <v>103</v>
       </c>
       <c r="D27" s="29" t="s">
@@ -1806,11 +1806,11 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="37"/>
+      <c r="A28" s="38"/>
       <c r="B28" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="39" t="s">
+      <c r="C28" s="36" t="s">
         <v>104</v>
       </c>
       <c r="D28" s="29" t="s">
@@ -1829,7 +1829,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="38"/>
+      <c r="A29" s="39"/>
       <c r="B29" s="21" t="s">
         <v>28</v>
       </c>
@@ -1850,13 +1850,13 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="37" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="36" t="s">
         <v>117</v>
       </c>
       <c r="D30" s="26" t="s">
@@ -1883,11 +1883,11 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="37"/>
+      <c r="A31" s="38"/>
       <c r="B31" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="39" t="s">
+      <c r="C31" s="36" t="s">
         <v>118</v>
       </c>
       <c r="D31" s="29"/>
@@ -1904,11 +1904,11 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="37"/>
+      <c r="A32" s="38"/>
       <c r="B32" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="36" t="s">
         <v>119</v>
       </c>
       <c r="D32" s="29"/>
@@ -1925,7 +1925,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="37"/>
+      <c r="A33" s="38"/>
       <c r="B33" s="19" t="s">
         <v>33</v>
       </c>
@@ -1946,7 +1946,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="38"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="21" t="s">
         <v>43</v>
       </c>
@@ -1967,7 +1967,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="36" t="s">
+      <c r="A35" s="37" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="20" t="s">
@@ -1990,11 +1990,11 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="37"/>
+      <c r="A36" s="38"/>
       <c r="B36" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="39" t="s">
+      <c r="C36" s="36" t="s">
         <v>123</v>
       </c>
       <c r="D36" s="29" t="s">
@@ -2021,7 +2021,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="37"/>
+      <c r="A37" s="38"/>
       <c r="B37" s="24" t="s">
         <v>84</v>
       </c>
@@ -2042,11 +2042,11 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="38"/>
+      <c r="A38" s="39"/>
       <c r="B38" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="36" t="s">
         <v>125</v>
       </c>
       <c r="D38" s="27"/>
@@ -2063,13 +2063,13 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="37" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="39" t="s">
+      <c r="C39" s="36" t="s">
         <v>126</v>
       </c>
       <c r="D39" s="26"/>
@@ -2086,7 +2086,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="37"/>
+      <c r="A40" s="38"/>
       <c r="B40" s="19" t="s">
         <v>40</v>
       </c>
@@ -2107,11 +2107,11 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="37"/>
+      <c r="A41" s="38"/>
       <c r="B41" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C41" s="36" t="s">
         <v>128</v>
       </c>
       <c r="D41" s="29"/>
@@ -2128,7 +2128,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="37"/>
+      <c r="A42" s="38"/>
       <c r="B42" s="24" t="s">
         <v>73</v>
       </c>
@@ -2155,11 +2155,11 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="38"/>
+      <c r="A43" s="39"/>
       <c r="B43" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C43" s="36" t="s">
         <v>130</v>
       </c>
       <c r="D43" s="27"/>
@@ -2176,13 +2176,13 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="36" t="s">
+      <c r="A44" s="37" t="s">
         <v>46</v>
       </c>
       <c r="B44" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="39" t="s">
+      <c r="C44" s="36" t="s">
         <v>131</v>
       </c>
       <c r="D44" s="26"/>
@@ -2201,7 +2201,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="37"/>
+      <c r="A45" s="38"/>
       <c r="B45" s="19" t="s">
         <v>48</v>
       </c>
@@ -2224,11 +2224,11 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="37"/>
+      <c r="A46" s="38"/>
       <c r="B46" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="39" t="s">
+      <c r="C46" s="36" t="s">
         <v>133</v>
       </c>
       <c r="D46" s="29"/>
@@ -2247,7 +2247,7 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="37"/>
+      <c r="A47" s="38"/>
       <c r="B47" s="24" t="s">
         <v>74</v>
       </c>
@@ -2278,11 +2278,11 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="38"/>
+      <c r="A48" s="39"/>
       <c r="B48" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="39" t="s">
+      <c r="C48" s="36" t="s">
         <v>135</v>
       </c>
       <c r="D48" s="27"/>
@@ -2301,13 +2301,13 @@
       </c>
     </row>
     <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="36" t="s">
+      <c r="A49" s="37" t="s">
         <v>51</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="39" t="s">
+      <c r="C49" s="36" t="s">
         <v>136</v>
       </c>
       <c r="D49" s="26"/>
@@ -2324,7 +2324,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="37"/>
+      <c r="A50" s="38"/>
       <c r="B50" s="19" t="s">
         <v>53</v>
       </c>
@@ -2345,11 +2345,11 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="37"/>
+      <c r="A51" s="38"/>
       <c r="B51" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="39" t="s">
+      <c r="C51" s="36" t="s">
         <v>138</v>
       </c>
       <c r="D51" s="29"/>
@@ -2366,11 +2366,11 @@
       </c>
     </row>
     <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="37"/>
+      <c r="A52" s="38"/>
       <c r="B52" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="39" t="s">
+      <c r="C52" s="36" t="s">
         <v>139</v>
       </c>
       <c r="D52" s="29"/>
@@ -2387,7 +2387,7 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="37"/>
+      <c r="A53" s="38"/>
       <c r="B53" s="24" t="s">
         <v>76</v>
       </c>
@@ -2408,7 +2408,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="38"/>
+      <c r="A54" s="39"/>
       <c r="B54" s="33" t="s">
         <v>68</v>
       </c>
@@ -2439,7 +2439,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="36" t="s">
+      <c r="A55" s="37" t="s">
         <v>56</v>
       </c>
       <c r="B55" s="20" t="s">
@@ -2460,7 +2460,7 @@
       </c>
     </row>
     <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="38"/>
+      <c r="A56" s="39"/>
       <c r="B56" s="21" t="s">
         <v>58</v>
       </c>
@@ -2500,13 +2500,13 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="36" t="s">
+      <c r="A58" s="37" t="s">
         <v>61</v>
       </c>
       <c r="B58" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C58" s="39"/>
+      <c r="C58" s="36"/>
       <c r="D58" s="26"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
@@ -2519,7 +2519,7 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="37"/>
+      <c r="A59" s="38"/>
       <c r="B59" s="19" t="s">
         <v>63</v>
       </c>
@@ -2536,7 +2536,7 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="37"/>
+      <c r="A60" s="38"/>
       <c r="B60" s="24" t="s">
         <v>75</v>
       </c>
@@ -2553,7 +2553,7 @@
       </c>
     </row>
     <row r="61" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="38"/>
+      <c r="A61" s="39"/>
       <c r="B61" s="21" t="s">
         <v>64</v>
       </c>
@@ -2594,6 +2594,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A22:A25"/>
     <mergeCell ref="A58:A61"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A38"/>
@@ -2601,12 +2607,6 @@
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A49:A54"/>
     <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#Fix Imprimir, agregar para imprimir cotizaciones, se probó y funciona imprimir seleccionando la impresora docx y jpg (en partidamodificar esta la prueba)
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -491,7 +491,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,6 +546,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -757,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -854,6 +860,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1138,7 +1145,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,7 +1936,7 @@
       <c r="B33" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="40" t="s">
         <v>120</v>
       </c>
       <c r="D33" s="29"/>
@@ -1950,7 +1957,7 @@
       <c r="B34" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="40" t="s">
         <v>121</v>
       </c>
       <c r="D34" s="27"/>
@@ -2090,7 +2097,7 @@
       <c r="B40" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="20" t="s">
+      <c r="C40" s="40" t="s">
         <v>127</v>
       </c>
       <c r="D40" s="29"/>
@@ -2132,7 +2139,7 @@
       <c r="B42" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="20" t="s">
+      <c r="C42" s="40" t="s">
         <v>129</v>
       </c>
       <c r="D42" s="31"/>
@@ -2205,7 +2212,7 @@
       <c r="B45" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C45" s="40" t="s">
         <v>132</v>
       </c>
       <c r="D45" s="29"/>
@@ -2251,7 +2258,7 @@
       <c r="B47" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="40" t="s">
         <v>134</v>
       </c>
       <c r="D47" s="31" t="s">
@@ -2391,7 +2398,7 @@
       <c r="B53" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="20" t="s">
+      <c r="C53" s="40" t="s">
         <v>140</v>
       </c>
       <c r="D53" s="31"/>
@@ -2594,12 +2601,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A22:A25"/>
     <mergeCell ref="A58:A61"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A38"/>
@@ -2607,6 +2608,12 @@
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A49:A54"/>
     <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#Imprimir partida y cotizaciones OK (Falta quitar bmp y png y pdf)
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -763,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -851,6 +851,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -860,7 +861,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1144,8 +1145,8 @@
   <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,7 +1196,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
@@ -1220,7 +1221,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="19" t="s">
         <v>2</v>
       </c>
@@ -1251,7 +1252,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="19" t="s">
         <v>3</v>
       </c>
@@ -1274,7 +1275,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="19" t="s">
         <v>4</v>
       </c>
@@ -1295,7 +1296,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="33" t="s">
         <v>45</v>
       </c>
@@ -1314,7 +1315,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="38" t="s">
         <v>65</v>
       </c>
       <c r="B7" s="20" t="s">
@@ -1339,7 +1340,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="21" t="s">
         <v>67</v>
       </c>
@@ -1362,7 +1363,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -1389,7 +1390,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="19" t="s">
         <v>7</v>
       </c>
@@ -1420,7 +1421,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="38"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="19" t="s">
         <v>8</v>
       </c>
@@ -1445,7 +1446,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="19" t="s">
         <v>9</v>
       </c>
@@ -1466,7 +1467,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="19" t="s">
         <v>10</v>
       </c>
@@ -1489,7 +1490,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="33" t="s">
         <v>44</v>
       </c>
@@ -1508,7 +1509,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="38" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -1533,7 +1534,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="38"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="19" t="s">
         <v>12</v>
       </c>
@@ -1560,7 +1561,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="38"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="19" t="s">
         <v>13</v>
       </c>
@@ -1583,7 +1584,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="38"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="19" t="s">
         <v>14</v>
       </c>
@@ -1604,7 +1605,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="38"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="19" t="s">
         <v>15</v>
       </c>
@@ -1627,7 +1628,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="38"/>
+      <c r="A20" s="39"/>
       <c r="B20" s="19" t="s">
         <v>16</v>
       </c>
@@ -1650,7 +1651,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="39"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="21" t="s">
         <v>18</v>
       </c>
@@ -1673,7 +1674,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="38" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="20" t="s">
@@ -1698,7 +1699,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="38"/>
+      <c r="A23" s="39"/>
       <c r="B23" s="19" t="s">
         <v>21</v>
       </c>
@@ -1721,7 +1722,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="38"/>
+      <c r="A24" s="39"/>
       <c r="B24" s="19" t="s">
         <v>22</v>
       </c>
@@ -1744,7 +1745,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="39"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="21" t="s">
         <v>23</v>
       </c>
@@ -1765,7 +1766,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="38" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="20" t="s">
@@ -1790,7 +1791,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="38"/>
+      <c r="A27" s="39"/>
       <c r="B27" s="19" t="s">
         <v>26</v>
       </c>
@@ -1813,7 +1814,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="38"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="19" t="s">
         <v>27</v>
       </c>
@@ -1836,7 +1837,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="39"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="21" t="s">
         <v>28</v>
       </c>
@@ -1857,7 +1858,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="38" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="20" t="s">
@@ -1890,7 +1891,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="38"/>
+      <c r="A31" s="39"/>
       <c r="B31" s="19" t="s">
         <v>31</v>
       </c>
@@ -1911,7 +1912,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="38"/>
+      <c r="A32" s="39"/>
       <c r="B32" s="19" t="s">
         <v>32</v>
       </c>
@@ -1932,11 +1933,11 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="38"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="C33" s="37" t="s">
         <v>120</v>
       </c>
       <c r="D33" s="29"/>
@@ -1953,11 +1954,11 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="39"/>
+      <c r="A34" s="40"/>
       <c r="B34" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="37" t="s">
         <v>121</v>
       </c>
       <c r="D34" s="27"/>
@@ -1974,13 +1975,13 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="38" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="37" t="s">
         <v>122</v>
       </c>
       <c r="D35" s="26"/>
@@ -1997,7 +1998,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="38"/>
+      <c r="A36" s="39"/>
       <c r="B36" s="19" t="s">
         <v>36</v>
       </c>
@@ -2028,11 +2029,11 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="38"/>
+      <c r="A37" s="39"/>
       <c r="B37" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="41" t="s">
         <v>124</v>
       </c>
       <c r="D37" s="31"/>
@@ -2049,7 +2050,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="39"/>
+      <c r="A38" s="40"/>
       <c r="B38" s="21" t="s">
         <v>37</v>
       </c>
@@ -2070,7 +2071,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="38" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="20" t="s">
@@ -2093,11 +2094,11 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="38"/>
+      <c r="A40" s="39"/>
       <c r="B40" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="40" t="s">
+      <c r="C40" s="37" t="s">
         <v>127</v>
       </c>
       <c r="D40" s="29"/>
@@ -2114,7 +2115,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="38"/>
+      <c r="A41" s="39"/>
       <c r="B41" s="19" t="s">
         <v>41</v>
       </c>
@@ -2135,11 +2136,11 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="38"/>
+      <c r="A42" s="39"/>
       <c r="B42" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="40" t="s">
+      <c r="C42" s="37" t="s">
         <v>129</v>
       </c>
       <c r="D42" s="31"/>
@@ -2162,7 +2163,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="39"/>
+      <c r="A43" s="40"/>
       <c r="B43" s="21" t="s">
         <v>42</v>
       </c>
@@ -2183,7 +2184,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="37" t="s">
+      <c r="A44" s="38" t="s">
         <v>46</v>
       </c>
       <c r="B44" s="20" t="s">
@@ -2208,11 +2209,11 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="38"/>
+      <c r="A45" s="39"/>
       <c r="B45" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="40" t="s">
+      <c r="C45" s="37" t="s">
         <v>132</v>
       </c>
       <c r="D45" s="29"/>
@@ -2231,7 +2232,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="38"/>
+      <c r="A46" s="39"/>
       <c r="B46" s="19" t="s">
         <v>49</v>
       </c>
@@ -2254,11 +2255,11 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="38"/>
+      <c r="A47" s="39"/>
       <c r="B47" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="40" t="s">
+      <c r="C47" s="37" t="s">
         <v>134</v>
       </c>
       <c r="D47" s="31" t="s">
@@ -2285,7 +2286,7 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="39"/>
+      <c r="A48" s="40"/>
       <c r="B48" s="21" t="s">
         <v>50</v>
       </c>
@@ -2308,7 +2309,7 @@
       </c>
     </row>
     <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="37" t="s">
+      <c r="A49" s="38" t="s">
         <v>51</v>
       </c>
       <c r="B49" s="20" t="s">
@@ -2331,11 +2332,11 @@
       </c>
     </row>
     <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="38"/>
+      <c r="A50" s="39"/>
       <c r="B50" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="20" t="s">
+      <c r="C50" s="37" t="s">
         <v>137</v>
       </c>
       <c r="D50" s="29"/>
@@ -2352,7 +2353,7 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="38"/>
+      <c r="A51" s="39"/>
       <c r="B51" s="19" t="s">
         <v>54</v>
       </c>
@@ -2373,7 +2374,7 @@
       </c>
     </row>
     <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="38"/>
+      <c r="A52" s="39"/>
       <c r="B52" s="19" t="s">
         <v>55</v>
       </c>
@@ -2394,11 +2395,11 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="38"/>
+      <c r="A53" s="39"/>
       <c r="B53" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="40" t="s">
+      <c r="C53" s="37" t="s">
         <v>140</v>
       </c>
       <c r="D53" s="31"/>
@@ -2415,7 +2416,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="39"/>
+      <c r="A54" s="40"/>
       <c r="B54" s="33" t="s">
         <v>68</v>
       </c>
@@ -2446,7 +2447,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="37" t="s">
+      <c r="A55" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B55" s="20" t="s">
@@ -2467,7 +2468,7 @@
       </c>
     </row>
     <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="39"/>
+      <c r="A56" s="40"/>
       <c r="B56" s="21" t="s">
         <v>58</v>
       </c>
@@ -2507,7 +2508,7 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="37" t="s">
+      <c r="A58" s="38" t="s">
         <v>61</v>
       </c>
       <c r="B58" s="20" t="s">
@@ -2526,7 +2527,7 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="38"/>
+      <c r="A59" s="39"/>
       <c r="B59" s="19" t="s">
         <v>63</v>
       </c>
@@ -2543,7 +2544,7 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="38"/>
+      <c r="A60" s="39"/>
       <c r="B60" s="24" t="s">
         <v>75</v>
       </c>
@@ -2560,7 +2561,7 @@
       </c>
     </row>
     <row r="61" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="39"/>
+      <c r="A61" s="40"/>
       <c r="B61" s="21" t="s">
         <v>64</v>
       </c>
@@ -2601,6 +2602,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A22:A25"/>
     <mergeCell ref="A58:A61"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A38"/>
@@ -2608,12 +2615,6 @@
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A49:A54"/>
     <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#Casos uso/SC001 - Crear Solicitud.docx (Modificacion minima)
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -763,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -852,6 +852,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -861,7 +862,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1146,7 +1147,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,7 +1160,7 @@
     <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="41" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1196,7 +1197,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
@@ -1221,7 +1222,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="19" t="s">
         <v>2</v>
       </c>
@@ -1252,7 +1253,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="19" t="s">
         <v>3</v>
       </c>
@@ -1275,7 +1276,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="19" t="s">
         <v>4</v>
       </c>
@@ -1296,7 +1297,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="33" t="s">
         <v>45</v>
       </c>
@@ -1315,7 +1316,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="39" t="s">
         <v>65</v>
       </c>
       <c r="B7" s="20" t="s">
@@ -1340,7 +1341,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="40"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="21" t="s">
         <v>67</v>
       </c>
@@ -1363,7 +1364,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="39" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -1390,7 +1391,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="19" t="s">
         <v>7</v>
       </c>
@@ -1421,7 +1422,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="39"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="19" t="s">
         <v>8</v>
       </c>
@@ -1446,7 +1447,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="39"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="19" t="s">
         <v>9</v>
       </c>
@@ -1467,7 +1468,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="19" t="s">
         <v>10</v>
       </c>
@@ -1490,7 +1491,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="40"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="33" t="s">
         <v>44</v>
       </c>
@@ -1509,7 +1510,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="39" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -1534,7 +1535,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="19" t="s">
         <v>12</v>
       </c>
@@ -1561,7 +1562,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="39"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="19" t="s">
         <v>13</v>
       </c>
@@ -1584,7 +1585,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="19" t="s">
         <v>14</v>
       </c>
@@ -1605,7 +1606,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="19" t="s">
         <v>15</v>
       </c>
@@ -1628,7 +1629,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="19" t="s">
         <v>16</v>
       </c>
@@ -1651,7 +1652,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="21" t="s">
         <v>18</v>
       </c>
@@ -1674,13 +1675,13 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="39" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="37" t="s">
         <v>113</v>
       </c>
       <c r="D22" s="26"/>
@@ -1699,7 +1700,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="39"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="19" t="s">
         <v>21</v>
       </c>
@@ -1722,11 +1723,11 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="39"/>
-      <c r="B24" s="19" t="s">
+      <c r="A24" s="40"/>
+      <c r="B24" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="37" t="s">
         <v>115</v>
       </c>
       <c r="D24" s="29"/>
@@ -1745,11 +1746,11 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="40"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="37" t="s">
         <v>116</v>
       </c>
       <c r="D25" s="27"/>
@@ -1766,7 +1767,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="39" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="20" t="s">
@@ -1791,7 +1792,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="39"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="19" t="s">
         <v>26</v>
       </c>
@@ -1814,7 +1815,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="39"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="19" t="s">
         <v>27</v>
       </c>
@@ -1837,11 +1838,11 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="40"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="37" t="s">
         <v>105</v>
       </c>
       <c r="D29" s="27"/>
@@ -1858,7 +1859,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="20" t="s">
@@ -1891,7 +1892,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="39"/>
+      <c r="A31" s="40"/>
       <c r="B31" s="19" t="s">
         <v>31</v>
       </c>
@@ -1912,7 +1913,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="39"/>
+      <c r="A32" s="40"/>
       <c r="B32" s="19" t="s">
         <v>32</v>
       </c>
@@ -1933,7 +1934,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="39"/>
+      <c r="A33" s="40"/>
       <c r="B33" s="19" t="s">
         <v>33</v>
       </c>
@@ -1954,7 +1955,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="40"/>
+      <c r="A34" s="41"/>
       <c r="B34" s="21" t="s">
         <v>43</v>
       </c>
@@ -1975,7 +1976,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="38" t="s">
+      <c r="A35" s="39" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="20" t="s">
@@ -1998,7 +1999,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="39"/>
+      <c r="A36" s="40"/>
       <c r="B36" s="19" t="s">
         <v>36</v>
       </c>
@@ -2029,11 +2030,11 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="39"/>
+      <c r="A37" s="40"/>
       <c r="B37" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="38" t="s">
         <v>124</v>
       </c>
       <c r="D37" s="31"/>
@@ -2050,7 +2051,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="40"/>
+      <c r="A38" s="41"/>
       <c r="B38" s="21" t="s">
         <v>37</v>
       </c>
@@ -2071,7 +2072,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="38" t="s">
+      <c r="A39" s="39" t="s">
         <v>38</v>
       </c>
       <c r="B39" s="20" t="s">
@@ -2094,7 +2095,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="39"/>
+      <c r="A40" s="40"/>
       <c r="B40" s="19" t="s">
         <v>40</v>
       </c>
@@ -2115,7 +2116,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="39"/>
+      <c r="A41" s="40"/>
       <c r="B41" s="19" t="s">
         <v>41</v>
       </c>
@@ -2136,7 +2137,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="39"/>
+      <c r="A42" s="40"/>
       <c r="B42" s="24" t="s">
         <v>73</v>
       </c>
@@ -2163,7 +2164,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="40"/>
+      <c r="A43" s="41"/>
       <c r="B43" s="21" t="s">
         <v>42</v>
       </c>
@@ -2184,7 +2185,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="39" t="s">
         <v>46</v>
       </c>
       <c r="B44" s="20" t="s">
@@ -2209,7 +2210,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="39"/>
+      <c r="A45" s="40"/>
       <c r="B45" s="19" t="s">
         <v>48</v>
       </c>
@@ -2232,7 +2233,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="39"/>
+      <c r="A46" s="40"/>
       <c r="B46" s="19" t="s">
         <v>49</v>
       </c>
@@ -2255,7 +2256,7 @@
       </c>
     </row>
     <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="39"/>
+      <c r="A47" s="40"/>
       <c r="B47" s="24" t="s">
         <v>74</v>
       </c>
@@ -2286,7 +2287,7 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="40"/>
+      <c r="A48" s="41"/>
       <c r="B48" s="21" t="s">
         <v>50</v>
       </c>
@@ -2309,7 +2310,7 @@
       </c>
     </row>
     <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="38" t="s">
+      <c r="A49" s="39" t="s">
         <v>51</v>
       </c>
       <c r="B49" s="20" t="s">
@@ -2332,7 +2333,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="39"/>
+      <c r="A50" s="40"/>
       <c r="B50" s="19" t="s">
         <v>53</v>
       </c>
@@ -2353,7 +2354,7 @@
       </c>
     </row>
     <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="39"/>
+      <c r="A51" s="40"/>
       <c r="B51" s="19" t="s">
         <v>54</v>
       </c>
@@ -2374,7 +2375,7 @@
       </c>
     </row>
     <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="39"/>
+      <c r="A52" s="40"/>
       <c r="B52" s="19" t="s">
         <v>55</v>
       </c>
@@ -2395,7 +2396,7 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="39"/>
+      <c r="A53" s="40"/>
       <c r="B53" s="24" t="s">
         <v>76</v>
       </c>
@@ -2416,7 +2417,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="40"/>
+      <c r="A54" s="41"/>
       <c r="B54" s="33" t="s">
         <v>68</v>
       </c>
@@ -2447,7 +2448,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="38" t="s">
+      <c r="A55" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B55" s="20" t="s">
@@ -2468,7 +2469,7 @@
       </c>
     </row>
     <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="40"/>
+      <c r="A56" s="41"/>
       <c r="B56" s="21" t="s">
         <v>58</v>
       </c>
@@ -2508,7 +2509,7 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="38" t="s">
+      <c r="A58" s="39" t="s">
         <v>61</v>
       </c>
       <c r="B58" s="20" t="s">
@@ -2527,7 +2528,7 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="39"/>
+      <c r="A59" s="40"/>
       <c r="B59" s="19" t="s">
         <v>63</v>
       </c>
@@ -2544,7 +2545,7 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="39"/>
+      <c r="A60" s="40"/>
       <c r="B60" s="24" t="s">
         <v>75</v>
       </c>
@@ -2561,7 +2562,7 @@
       </c>
     </row>
     <row r="61" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="40"/>
+      <c r="A61" s="41"/>
       <c r="B61" s="21" t="s">
         <v>64</v>
       </c>
@@ -2602,12 +2603,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="A22:A25"/>
     <mergeCell ref="A58:A61"/>
     <mergeCell ref="A30:A34"/>
     <mergeCell ref="A35:A38"/>
@@ -2615,6 +2610,12 @@
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A49:A54"/>
     <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="A22:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#Diagramas Secuencia: - IG001 - Solicitar Partida Especial.docx - IG003 - Modificar Partida.docx - IG002 - Buscar Partida
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="143">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>ALT</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -543,6 +546,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -778,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -845,7 +860,14 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -855,14 +877,17 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1147,7 +1172,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,7 +1180,7 @@
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="41" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33" bestFit="1" customWidth="1"/>
@@ -1181,7 +1206,7 @@
       <c r="F1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="51" t="s">
         <v>85</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1190,34 +1215,34 @@
       <c r="I1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="24" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="41"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
         <v>66</v>
@@ -1233,18 +1258,18 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
-      <c r="B3" s="19" t="s">
+      <c r="A3" s="39"/>
+      <c r="B3" s="42" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="7" t="s">
         <v>66</v>
       </c>
@@ -1266,16 +1291,16 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="39"/>
+      <c r="B4" s="42" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
         <v>66</v>
@@ -1291,16 +1316,16 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="39"/>
+      <c r="B5" s="42" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
@@ -1314,22 +1339,22 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="41" t="s">
         <v>64</v>
       </c>
       <c r="C6" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="30" t="s">
         <v>141</v>
       </c>
       <c r="G6" s="5"/>
@@ -1345,18 +1370,18 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33"/>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="40"/>
+      <c r="B7" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="9"/>
       <c r="H7" s="13"/>
       <c r="I7" s="9" t="s">
@@ -1370,23 +1395,25 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="48" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="14"/>
+      <c r="D8" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="26" t="s">
+        <v>66</v>
+      </c>
       <c r="H8" s="5"/>
-      <c r="I8" s="26" t="s">
-        <v>66</v>
-      </c>
+      <c r="I8" s="14"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1395,23 +1422,25 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="39"/>
+      <c r="B9" s="49" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
+      <c r="D9" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
       <c r="G9" s="7" t="s">
         <v>66</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="22" t="s">
         <v>66</v>
       </c>
       <c r="J9" s="7" t="s">
@@ -1426,21 +1455,23 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
-      <c r="B10" s="19" t="s">
+      <c r="A10" s="39"/>
+      <c r="B10" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="15"/>
+      <c r="D10" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="26" t="s">
+        <v>66</v>
+      </c>
       <c r="H10" s="7"/>
-      <c r="I10" s="26" t="s">
-        <v>66</v>
-      </c>
+      <c r="I10" s="15"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
@@ -1449,16 +1480,16 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="32"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="39"/>
+      <c r="B11" s="49" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
       <c r="G11" s="7" t="s">
         <v>66</v>
       </c>
@@ -1472,16 +1503,16 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="39"/>
+      <c r="B12" s="49" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
       <c r="G12" s="7" t="s">
         <v>66</v>
       </c>
@@ -1495,18 +1526,18 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="45" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1522,16 +1553,16 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="32"/>
-      <c r="B14" s="19" t="s">
+      <c r="A14" s="39"/>
+      <c r="B14" s="46" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
       <c r="G14" s="7" t="s">
         <v>66</v>
       </c>
@@ -1549,16 +1580,16 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="32"/>
-      <c r="B15" s="19" t="s">
+      <c r="A15" s="39"/>
+      <c r="B15" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -1574,16 +1605,16 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="32"/>
-      <c r="B16" s="19" t="s">
+      <c r="A16" s="39"/>
+      <c r="B16" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -1597,16 +1628,16 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="32"/>
-      <c r="B17" s="19" t="s">
+      <c r="A17" s="39"/>
+      <c r="B17" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -1622,16 +1653,16 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
-      <c r="B18" s="19" t="s">
+      <c r="A18" s="39"/>
+      <c r="B18" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -1647,16 +1678,16 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="33"/>
-      <c r="B19" s="21" t="s">
+      <c r="A19" s="40"/>
+      <c r="B19" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -1672,18 +1703,18 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="45" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1699,16 +1730,16 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="32"/>
-      <c r="B21" s="19" t="s">
+      <c r="A21" s="39"/>
+      <c r="B21" s="46" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -1724,16 +1755,16 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="32"/>
-      <c r="B22" s="30" t="s">
+      <c r="A22" s="39"/>
+      <c r="B22" s="46" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -1749,16 +1780,16 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="33"/>
-      <c r="B23" s="21" t="s">
+      <c r="A23" s="40"/>
+      <c r="B23" s="47" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
@@ -1772,18 +1803,18 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="48" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
       <c r="G24" s="5" t="s">
         <v>66</v>
       </c>
@@ -1797,16 +1828,16 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="32"/>
-      <c r="B25" s="19" t="s">
+      <c r="A25" s="39"/>
+      <c r="B25" s="49" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="7" t="s">
         <v>66</v>
       </c>
@@ -1820,16 +1851,16 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="32"/>
-      <c r="B26" s="19" t="s">
+      <c r="A26" s="39"/>
+      <c r="B26" s="49" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="7" t="s">
         <v>66</v>
       </c>
@@ -1843,16 +1874,16 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="33"/>
-      <c r="B27" s="21" t="s">
+      <c r="A27" s="40"/>
+      <c r="B27" s="50" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
       <c r="G27" s="9" t="s">
         <v>66</v>
       </c>
@@ -1866,18 +1897,18 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="41" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
       <c r="G28" s="5" t="s">
         <v>66</v>
       </c>
@@ -1899,16 +1930,16 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="32"/>
-      <c r="B29" s="19" t="s">
+      <c r="A29" s="39"/>
+      <c r="B29" s="42" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7" t="s">
         <v>66</v>
@@ -1922,16 +1953,16 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="32"/>
-      <c r="B30" s="19" t="s">
+      <c r="A30" s="39"/>
+      <c r="B30" s="42" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7" t="s">
         <v>66</v>
@@ -1945,16 +1976,16 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="32"/>
-      <c r="B31" s="19" t="s">
+      <c r="A31" s="39"/>
+      <c r="B31" s="42" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7" t="s">
         <v>66</v>
@@ -1968,16 +1999,16 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="33"/>
-      <c r="B32" s="21" t="s">
+      <c r="A32" s="40"/>
+      <c r="B32" s="43" t="s">
         <v>43</v>
       </c>
       <c r="C32" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9" t="s">
         <v>66</v>
@@ -1991,18 +2022,18 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="41" t="s">
         <v>35</v>
       </c>
       <c r="C33" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5" t="s">
@@ -2016,16 +2047,16 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="32"/>
-      <c r="B34" s="19" t="s">
+      <c r="A34" s="39"/>
+      <c r="B34" s="42" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="7" t="s">
         <v>66</v>
       </c>
@@ -2047,16 +2078,16 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="32"/>
-      <c r="B35" s="24" t="s">
+      <c r="A35" s="39"/>
+      <c r="B35" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C35" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
       <c r="G35" s="22"/>
       <c r="H35" s="22"/>
       <c r="I35" s="22" t="s">
@@ -2070,16 +2101,16 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="33"/>
-      <c r="B36" s="21" t="s">
+      <c r="A36" s="40"/>
+      <c r="B36" s="43" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9" t="s">
@@ -2093,18 +2124,18 @@
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="41" t="s">
         <v>39</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5" t="s">
@@ -2118,16 +2149,16 @@
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="32"/>
-      <c r="B38" s="19" t="s">
+      <c r="A38" s="39"/>
+      <c r="B38" s="42" t="s">
         <v>40</v>
       </c>
       <c r="C38" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7" t="s">
@@ -2141,16 +2172,16 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="32"/>
-      <c r="B39" s="19" t="s">
+      <c r="A39" s="39"/>
+      <c r="B39" s="42" t="s">
         <v>41</v>
       </c>
       <c r="C39" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7" t="s">
@@ -2164,16 +2195,16 @@
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="32"/>
-      <c r="B40" s="24" t="s">
+      <c r="A40" s="39"/>
+      <c r="B40" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C40" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
       <c r="G40" s="11"/>
       <c r="H40" s="11" t="s">
         <v>66</v>
@@ -2193,16 +2224,16 @@
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="33"/>
-      <c r="B41" s="21" t="s">
+      <c r="A41" s="40"/>
+      <c r="B41" s="43" t="s">
         <v>42</v>
       </c>
       <c r="C41" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
       <c r="I41" s="9" t="s">
@@ -2216,18 +2247,18 @@
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="41" t="s">
         <v>45</v>
       </c>
       <c r="C42" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5" t="s">
@@ -2243,16 +2274,16 @@
       </c>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="32"/>
-      <c r="B43" s="19" t="s">
+      <c r="A43" s="39"/>
+      <c r="B43" s="42" t="s">
         <v>46</v>
       </c>
       <c r="C43" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7" t="s">
@@ -2268,16 +2299,16 @@
       </c>
     </row>
     <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="32"/>
-      <c r="B44" s="19" t="s">
+      <c r="A44" s="39"/>
+      <c r="B44" s="42" t="s">
         <v>47</v>
       </c>
       <c r="C44" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
       <c r="I44" s="7" t="s">
@@ -2293,16 +2324,16 @@
       </c>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="32"/>
-      <c r="B45" s="24" t="s">
+      <c r="A45" s="39"/>
+      <c r="B45" s="1" t="s">
         <v>71</v>
       </c>
       <c r="C45" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="32"/>
       <c r="G45" s="11" t="s">
         <v>66</v>
       </c>
@@ -2324,16 +2355,16 @@
       </c>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="33"/>
-      <c r="B46" s="21" t="s">
+      <c r="A46" s="40"/>
+      <c r="B46" s="43" t="s">
         <v>48</v>
       </c>
       <c r="C46" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
       <c r="I46" s="9" t="s">
@@ -2349,7 +2380,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="38" t="s">
         <v>49</v>
       </c>
       <c r="B47" s="20" t="s">
@@ -2358,9 +2389,9 @@
       <c r="C47" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -2374,16 +2405,16 @@
       </c>
     </row>
     <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="32"/>
+      <c r="A48" s="39"/>
       <c r="B48" s="19" t="s">
         <v>51</v>
       </c>
       <c r="C48" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
@@ -2397,16 +2428,16 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="32"/>
+      <c r="A49" s="39"/>
       <c r="B49" s="19" t="s">
         <v>52</v>
       </c>
       <c r="C49" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="35"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="35"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
@@ -2420,16 +2451,16 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="32"/>
+      <c r="A50" s="39"/>
       <c r="B50" s="19" t="s">
         <v>53</v>
       </c>
       <c r="C50" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D50" s="35"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
@@ -2443,16 +2474,16 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="32"/>
+      <c r="A51" s="39"/>
       <c r="B51" s="24" t="s">
         <v>73</v>
       </c>
       <c r="C51" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
       <c r="I51" s="11"/>
@@ -2466,16 +2497,16 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="38" t="s">
         <v>54</v>
       </c>
       <c r="B52" s="20" t="s">
         <v>55</v>
       </c>
       <c r="C52" s="20"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
@@ -2489,14 +2520,14 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="33"/>
+      <c r="A53" s="40"/>
       <c r="B53" s="21" t="s">
         <v>56</v>
       </c>
       <c r="C53" s="21"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="33"/>
       <c r="G53" s="9"/>
       <c r="H53" s="9"/>
       <c r="I53" s="9"/>
@@ -2517,9 +2548,9 @@
         <v>58</v>
       </c>
       <c r="C54" s="25"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="34"/>
       <c r="G54" s="16"/>
       <c r="H54" s="16"/>
       <c r="I54" s="16"/>
@@ -2533,16 +2564,16 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="38" t="s">
         <v>59</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>60</v>
       </c>
       <c r="C55" s="27"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="34"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="30"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
@@ -2554,14 +2585,14 @@
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="32"/>
+      <c r="A56" s="39"/>
       <c r="B56" s="19" t="s">
         <v>61</v>
       </c>
       <c r="C56" s="19"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="39"/>
-      <c r="F56" s="39"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="35"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
@@ -2573,14 +2604,14 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="32"/>
+      <c r="A57" s="39"/>
       <c r="B57" s="24" t="s">
         <v>72</v>
       </c>
       <c r="C57" s="24"/>
-      <c r="D57" s="40"/>
-      <c r="E57" s="40"/>
-      <c r="F57" s="40"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="36"/>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
       <c r="I57" s="11"/>
@@ -2592,14 +2623,14 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="33"/>
+      <c r="A58" s="40"/>
       <c r="B58" s="21" t="s">
         <v>62</v>
       </c>
       <c r="C58" s="21"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="37"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="33"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
@@ -2635,12 +2666,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A33:A36"/>
@@ -2648,6 +2673,12 @@
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#Modificar estado solicDetalle al asociar partida dentro de DAL, hecho #Diagramas de secuencia: IG003 - Buscar Partida IG004 - Cancelar Partida.docx IG005 - Asociar Partida Especial.docx
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="143">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -868,15 +868,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -888,6 +879,15 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1172,7 +1172,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1206,7 @@
       <c r="F1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="48" t="s">
         <v>85</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1215,10 +1215,10 @@
       <c r="I1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="44" t="s">
+      <c r="J1" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="41" t="s">
         <v>86</v>
       </c>
       <c r="L1" s="24" t="s">
@@ -1229,10 +1229,10 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="27" t="s">
@@ -1258,8 +1258,8 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39"/>
-      <c r="B3" s="42" t="s">
+      <c r="A3" s="50"/>
+      <c r="B3" s="39" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="27" t="s">
@@ -1291,8 +1291,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
-      <c r="B4" s="42" t="s">
+      <c r="A4" s="50"/>
+      <c r="B4" s="39" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="27" t="s">
@@ -1316,8 +1316,8 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
-      <c r="B5" s="42" t="s">
+      <c r="A5" s="50"/>
+      <c r="B5" s="39" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="27" t="s">
@@ -1339,10 +1339,10 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="38" t="s">
         <v>64</v>
       </c>
       <c r="C6" s="27" t="s">
@@ -1370,8 +1370,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="40"/>
-      <c r="B7" s="43" t="s">
+      <c r="A7" s="51"/>
+      <c r="B7" s="40" t="s">
         <v>65</v>
       </c>
       <c r="C7" s="27" t="s">
@@ -1395,10 +1395,10 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="45" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="27" t="s">
@@ -1422,8 +1422,8 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
-      <c r="B9" s="49" t="s">
+      <c r="A9" s="50"/>
+      <c r="B9" s="46" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="27" t="s">
@@ -1455,8 +1455,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39"/>
-      <c r="B10" s="49" t="s">
+      <c r="A10" s="50"/>
+      <c r="B10" s="46" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="27" t="s">
@@ -1480,14 +1480,16 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="39"/>
-      <c r="B11" s="49" t="s">
+      <c r="A11" s="50"/>
+      <c r="B11" s="46" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="31"/>
+      <c r="D11" s="31" t="s">
+        <v>141</v>
+      </c>
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
       <c r="G11" s="7" t="s">
@@ -1503,14 +1505,16 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="39"/>
-      <c r="B12" s="49" t="s">
+      <c r="A12" s="50"/>
+      <c r="B12" s="46" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="31"/>
+      <c r="D12" s="31" t="s">
+        <v>142</v>
+      </c>
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
       <c r="G12" s="7" t="s">
@@ -1526,10 +1530,10 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="42" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="27" t="s">
@@ -1553,8 +1557,8 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
-      <c r="B14" s="46" t="s">
+      <c r="A14" s="50"/>
+      <c r="B14" s="43" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="27" t="s">
@@ -1580,8 +1584,8 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
-      <c r="B15" s="46" t="s">
+      <c r="A15" s="50"/>
+      <c r="B15" s="43" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="28" t="s">
@@ -1605,8 +1609,8 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
-      <c r="B16" s="46" t="s">
+      <c r="A16" s="50"/>
+      <c r="B16" s="43" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="28" t="s">
@@ -1628,8 +1632,8 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="39"/>
-      <c r="B17" s="46" t="s">
+      <c r="A17" s="50"/>
+      <c r="B17" s="43" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="28" t="s">
@@ -1653,8 +1657,8 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
-      <c r="B18" s="46" t="s">
+      <c r="A18" s="50"/>
+      <c r="B18" s="43" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="28" t="s">
@@ -1678,8 +1682,8 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
-      <c r="B19" s="47" t="s">
+      <c r="A19" s="51"/>
+      <c r="B19" s="44" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="28" t="s">
@@ -1703,10 +1707,10 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="42" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="28" t="s">
@@ -1730,8 +1734,8 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="39"/>
-      <c r="B21" s="46" t="s">
+      <c r="A21" s="50"/>
+      <c r="B21" s="43" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="27" t="s">
@@ -1755,8 +1759,8 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="39"/>
-      <c r="B22" s="46" t="s">
+      <c r="A22" s="50"/>
+      <c r="B22" s="43" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="28" t="s">
@@ -1780,8 +1784,8 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="40"/>
-      <c r="B23" s="47" t="s">
+      <c r="A23" s="51"/>
+      <c r="B23" s="44" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="28" t="s">
@@ -1803,10 +1807,10 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="48" t="s">
+      <c r="B24" s="45" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="27" t="s">
@@ -1828,8 +1832,8 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="39"/>
-      <c r="B25" s="49" t="s">
+      <c r="A25" s="50"/>
+      <c r="B25" s="46" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="27" t="s">
@@ -1851,8 +1855,8 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="39"/>
-      <c r="B26" s="49" t="s">
+      <c r="A26" s="50"/>
+      <c r="B26" s="46" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="27" t="s">
@@ -1874,8 +1878,8 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="40"/>
-      <c r="B27" s="50" t="s">
+      <c r="A27" s="51"/>
+      <c r="B27" s="47" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="28" t="s">
@@ -1897,10 +1901,10 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="38" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="27" t="s">
@@ -1930,8 +1934,8 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="39"/>
-      <c r="B29" s="42" t="s">
+      <c r="A29" s="50"/>
+      <c r="B29" s="39" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="27" t="s">
@@ -1953,8 +1957,8 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="39"/>
-      <c r="B30" s="42" t="s">
+      <c r="A30" s="50"/>
+      <c r="B30" s="39" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="27" t="s">
@@ -1976,8 +1980,8 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="39"/>
-      <c r="B31" s="42" t="s">
+      <c r="A31" s="50"/>
+      <c r="B31" s="39" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="28" t="s">
@@ -1999,8 +2003,8 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="40"/>
-      <c r="B32" s="43" t="s">
+      <c r="A32" s="51"/>
+      <c r="B32" s="40" t="s">
         <v>43</v>
       </c>
       <c r="C32" s="28" t="s">
@@ -2022,10 +2026,10 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="38" t="s">
+      <c r="A33" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="41" t="s">
+      <c r="B33" s="38" t="s">
         <v>35</v>
       </c>
       <c r="C33" s="28" t="s">
@@ -2047,8 +2051,8 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="39"/>
-      <c r="B34" s="42" t="s">
+      <c r="A34" s="50"/>
+      <c r="B34" s="39" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="27" t="s">
@@ -2078,7 +2082,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="39"/>
+      <c r="A35" s="50"/>
       <c r="B35" s="1" t="s">
         <v>81</v>
       </c>
@@ -2101,8 +2105,8 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="40"/>
-      <c r="B36" s="43" t="s">
+      <c r="A36" s="51"/>
+      <c r="B36" s="40" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="27" t="s">
@@ -2124,10 +2128,10 @@
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="38" t="s">
+      <c r="A37" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="38" t="s">
         <v>39</v>
       </c>
       <c r="C37" s="27" t="s">
@@ -2149,8 +2153,8 @@
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="39"/>
-      <c r="B38" s="42" t="s">
+      <c r="A38" s="50"/>
+      <c r="B38" s="39" t="s">
         <v>40</v>
       </c>
       <c r="C38" s="28" t="s">
@@ -2172,8 +2176,8 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="39"/>
-      <c r="B39" s="42" t="s">
+      <c r="A39" s="50"/>
+      <c r="B39" s="39" t="s">
         <v>41</v>
       </c>
       <c r="C39" s="27" t="s">
@@ -2195,7 +2199,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="39"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="1" t="s">
         <v>70</v>
       </c>
@@ -2224,8 +2228,8 @@
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="40"/>
-      <c r="B41" s="43" t="s">
+      <c r="A41" s="51"/>
+      <c r="B41" s="40" t="s">
         <v>42</v>
       </c>
       <c r="C41" s="27" t="s">
@@ -2247,10 +2251,10 @@
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="38" t="s">
         <v>45</v>
       </c>
       <c r="C42" s="27" t="s">
@@ -2274,8 +2278,8 @@
       </c>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="39"/>
-      <c r="B43" s="42" t="s">
+      <c r="A43" s="50"/>
+      <c r="B43" s="39" t="s">
         <v>46</v>
       </c>
       <c r="C43" s="28" t="s">
@@ -2299,8 +2303,8 @@
       </c>
     </row>
     <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="39"/>
-      <c r="B44" s="42" t="s">
+      <c r="A44" s="50"/>
+      <c r="B44" s="39" t="s">
         <v>47</v>
       </c>
       <c r="C44" s="27" t="s">
@@ -2324,7 +2328,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="39"/>
+      <c r="A45" s="50"/>
       <c r="B45" s="1" t="s">
         <v>71</v>
       </c>
@@ -2355,8 +2359,8 @@
       </c>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="40"/>
-      <c r="B46" s="43" t="s">
+      <c r="A46" s="51"/>
+      <c r="B46" s="40" t="s">
         <v>48</v>
       </c>
       <c r="C46" s="27" t="s">
@@ -2380,7 +2384,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="49" t="s">
         <v>49</v>
       </c>
       <c r="B47" s="20" t="s">
@@ -2405,7 +2409,7 @@
       </c>
     </row>
     <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="39"/>
+      <c r="A48" s="50"/>
       <c r="B48" s="19" t="s">
         <v>51</v>
       </c>
@@ -2428,7 +2432,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="39"/>
+      <c r="A49" s="50"/>
       <c r="B49" s="19" t="s">
         <v>52</v>
       </c>
@@ -2451,7 +2455,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="39"/>
+      <c r="A50" s="50"/>
       <c r="B50" s="19" t="s">
         <v>53</v>
       </c>
@@ -2474,7 +2478,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="39"/>
+      <c r="A51" s="50"/>
       <c r="B51" s="24" t="s">
         <v>73</v>
       </c>
@@ -2497,7 +2501,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="38" t="s">
+      <c r="A52" s="49" t="s">
         <v>54</v>
       </c>
       <c r="B52" s="20" t="s">
@@ -2520,7 +2524,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="40"/>
+      <c r="A53" s="51"/>
       <c r="B53" s="21" t="s">
         <v>56</v>
       </c>
@@ -2564,7 +2568,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="38" t="s">
+      <c r="A55" s="49" t="s">
         <v>59</v>
       </c>
       <c r="B55" s="20" t="s">
@@ -2585,7 +2589,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="39"/>
+      <c r="A56" s="50"/>
       <c r="B56" s="19" t="s">
         <v>61</v>
       </c>
@@ -2604,7 +2608,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="39"/>
+      <c r="A57" s="50"/>
       <c r="B57" s="24" t="s">
         <v>72</v>
       </c>
@@ -2623,7 +2627,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="40"/>
+      <c r="A58" s="51"/>
       <c r="B58" s="21" t="s">
         <v>62</v>
       </c>
@@ -2666,6 +2670,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A33:A36"/>
@@ -2673,12 +2683,6 @@
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#Secuencia - IG006 CrearRendicion
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="143">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -1171,8 +1171,8 @@
   <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,7 +1816,9 @@
       <c r="C24" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="30"/>
+      <c r="D24" s="30" t="s">
+        <v>141</v>
+      </c>
       <c r="E24" s="30"/>
       <c r="F24" s="30"/>
       <c r="G24" s="5" t="s">
@@ -2670,6 +2672,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A33:A36"/>
@@ -2677,12 +2685,6 @@
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Diagramas secuencia y copiado a carpeta de las cosas Crear Solicitud	SC001	CARPETA Buscar Solicitud	SC002	CARPETA Modificar Solicitud	SC003 Cancelar Solicitud	SC004 Solicitar Cotizacion	SC005	CARPETA Agregar Cotizacion	SC006	CARPETA Solicitar Partida Especial	IG001	ALT CARPETA Buscar Partida Especial	IG002	ALT CARPETA Modificar Partida Especial	IG003	CARPETA Cancelar Partida Especial	IG004	CARPETA Asociar Partida Especial	IG005	ALT CARPETA Registrar Adquisicion	AA001	CARPETA Buscar Adquisicion	AA002	OK Modificar Adquisicion	AA003	OK Eliminar Adquisicion	AA004 Modificar Inventario	AA005 Eliminar Inventario	AA006 Agregar Inventario	AA007 Crear Asignacion	AA008 Buscar Asignacion	AA009 Modificar Asignacion	AA010 Eliminar Asignacion	AA011 Crear Rendicion	IG006	CARPETA Buscar Rendicion	IG007	CARPETA ReGenerar Rendicion	IG008	CARPETA Eliminar Rendicion	IG009	CARPETA
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="144">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -44,21 +44,6 @@
     <t>Partidas</t>
   </si>
   <si>
-    <t>Crear Partida</t>
-  </si>
-  <si>
-    <t>Buscar Partida</t>
-  </si>
-  <si>
-    <t>Modificar Partida</t>
-  </si>
-  <si>
-    <t>Cancelar Partida</t>
-  </si>
-  <si>
-    <t>Asociar Partida</t>
-  </si>
-  <si>
     <t>Adquisiciones</t>
   </si>
   <si>
@@ -77,9 +62,6 @@
     <t>Eliminar Inventario</t>
   </si>
   <si>
-    <t>Registrar Adquisicion/Inventario</t>
-  </si>
-  <si>
     <t>Agregar Inventario</t>
   </si>
   <si>
@@ -452,7 +434,28 @@
     <t>OK</t>
   </si>
   <si>
-    <t>ALT</t>
+    <t>CARPETA</t>
+  </si>
+  <si>
+    <t>Registrar Adquisicion</t>
+  </si>
+  <si>
+    <t>Solicitar Partida Especial</t>
+  </si>
+  <si>
+    <t>ALT CARPETA</t>
+  </si>
+  <si>
+    <t>Modificar Partida Especial</t>
+  </si>
+  <si>
+    <t>Buscar Partida Especial</t>
+  </si>
+  <si>
+    <t>Cancelar Partida Especial</t>
+  </si>
+  <si>
+    <t>Asociar Partida Especial</t>
   </si>
 </sst>
 </file>
@@ -1171,15 +1174,18 @@
   <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="41" bestFit="1" customWidth="1"/>
@@ -1192,40 +1198,40 @@
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G1" s="48" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="J1" s="41" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="K1" s="41" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="L1" s="24" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="M1" s="24" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1236,25 +1242,25 @@
         <v>0</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E2" s="30"/>
       <c r="F2" s="37"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1263,31 +1269,31 @@
         <v>2</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E3" s="31"/>
       <c r="F3" s="31"/>
       <c r="G3" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1296,23 +1302,23 @@
         <v>3</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D4" s="31"/>
       <c r="E4" s="31"/>
       <c r="F4" s="31"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1321,7 +1327,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
@@ -1329,69 +1335,69 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="49" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F6" s="30" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="14"/>
       <c r="I6" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="51"/>
       <c r="B7" s="40" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E7" s="32"/>
       <c r="F7" s="32"/>
       <c r="G7" s="9"/>
       <c r="H7" s="13"/>
       <c r="I7" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1399,18 +1405,18 @@
         <v>5</v>
       </c>
       <c r="B8" s="45" t="s">
-        <v>6</v>
+        <v>138</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="26" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="14"/>
@@ -1418,57 +1424,57 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="50"/>
       <c r="B9" s="46" t="s">
-        <v>7</v>
+        <v>141</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E9" s="31"/>
       <c r="F9" s="31"/>
       <c r="G9" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L9" s="7"/>
       <c r="M9" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="50"/>
       <c r="B10" s="46" t="s">
-        <v>8</v>
+        <v>140</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
       <c r="G10" s="26" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="15"/>
@@ -1476,24 +1482,24 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="50"/>
       <c r="B11" s="46" t="s">
-        <v>9</v>
+        <v>142</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E11" s="31"/>
       <c r="F11" s="31"/>
       <c r="G11" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -1501,24 +1507,24 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="50"/>
       <c r="B12" s="46" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
       <c r="G12" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -1526,95 +1532,101 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="49" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B13" s="42" t="s">
-        <v>17</v>
+        <v>137</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="30"/>
+        <v>96</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>136</v>
+      </c>
       <c r="E13" s="30"/>
       <c r="F13" s="30"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="50"/>
       <c r="B14" s="43" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" s="31"/>
+        <v>97</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>135</v>
+      </c>
       <c r="E14" s="31"/>
       <c r="F14" s="31"/>
       <c r="G14" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="50"/>
       <c r="B15" s="43" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="D15" s="31"/>
+        <v>8</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>135</v>
+      </c>
       <c r="E15" s="31"/>
       <c r="F15" s="31"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="50"/>
       <c r="B16" s="43" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D16" s="31"/>
       <c r="E16" s="31"/>
@@ -1624,20 +1636,20 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L16" s="7"/>
       <c r="M16" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="50"/>
       <c r="B17" s="43" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D17" s="31"/>
       <c r="E17" s="31"/>
@@ -1646,23 +1658,23 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="50"/>
       <c r="B18" s="43" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D18" s="31"/>
       <c r="E18" s="31"/>
@@ -1671,23 +1683,23 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="51"/>
       <c r="B19" s="44" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
@@ -1696,25 +1708,25 @@
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="49" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
@@ -1723,23 +1735,23 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L20" s="5"/>
       <c r="M20" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="50"/>
       <c r="B21" s="43" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D21" s="31"/>
       <c r="E21" s="31"/>
@@ -1748,23 +1760,23 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L21" s="7"/>
       <c r="M21" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="50"/>
       <c r="B22" s="43" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
@@ -1773,23 +1785,23 @@
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L22" s="7"/>
       <c r="M22" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="51"/>
       <c r="B23" s="44" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D23" s="32"/>
       <c r="E23" s="32"/>
@@ -1799,30 +1811,30 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L23" s="9"/>
       <c r="M23" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="49" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B24" s="45" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E24" s="30"/>
       <c r="F24" s="30"/>
       <c r="G24" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1830,22 +1842,24 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
       <c r="M24" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="50"/>
       <c r="B25" s="46" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" s="31"/>
+        <v>93</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>136</v>
+      </c>
       <c r="E25" s="31"/>
       <c r="F25" s="31"/>
       <c r="G25" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -1853,22 +1867,24 @@
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
       <c r="M25" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="50"/>
       <c r="B26" s="46" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="31"/>
+        <v>94</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>136</v>
+      </c>
       <c r="E26" s="31"/>
       <c r="F26" s="31"/>
       <c r="G26" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
@@ -1876,22 +1892,24 @@
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
       <c r="M26" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="51"/>
       <c r="B27" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" s="32"/>
+        <v>22</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>136</v>
+      </c>
       <c r="E27" s="32"/>
       <c r="F27" s="32"/>
       <c r="G27" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
@@ -1899,143 +1917,143 @@
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="49" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D28" s="30"/>
       <c r="E28" s="30"/>
       <c r="F28" s="30"/>
       <c r="G28" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L28" s="5"/>
       <c r="M28" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="50"/>
       <c r="B29" s="39" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D29" s="31"/>
       <c r="E29" s="31"/>
       <c r="F29" s="31"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="50"/>
       <c r="B30" s="39" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D30" s="31"/>
       <c r="E30" s="31"/>
       <c r="F30" s="31"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="50"/>
       <c r="B31" s="39" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D31" s="31"/>
       <c r="E31" s="31"/>
       <c r="F31" s="31"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
       <c r="M31" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="51"/>
       <c r="B32" s="40" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D32" s="32"/>
       <c r="E32" s="32"/>
       <c r="F32" s="32"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
       <c r="M32" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="49" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D33" s="30"/>
       <c r="E33" s="30"/>
@@ -2043,53 +2061,53 @@
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
       <c r="M33" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="50"/>
       <c r="B34" s="39" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D34" s="31"/>
       <c r="E34" s="31"/>
       <c r="F34" s="31"/>
       <c r="G34" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L34" s="7"/>
       <c r="M34" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="50"/>
       <c r="B35" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D35" s="32"/>
       <c r="E35" s="32"/>
@@ -2097,22 +2115,22 @@
       <c r="G35" s="22"/>
       <c r="H35" s="22"/>
       <c r="I35" s="22" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J35" s="22"/>
       <c r="K35" s="22"/>
       <c r="L35" s="22"/>
       <c r="M35" s="23" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="51"/>
       <c r="B36" s="40" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D36" s="33"/>
       <c r="E36" s="33"/>
@@ -2120,24 +2138,24 @@
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
       <c r="L36" s="9"/>
       <c r="M36" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="49" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D37" s="30"/>
       <c r="E37" s="30"/>
@@ -2145,22 +2163,22 @@
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
       <c r="M37" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="50"/>
       <c r="B38" s="39" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D38" s="31"/>
       <c r="E38" s="31"/>
@@ -2168,22 +2186,22 @@
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
       <c r="L38" s="7"/>
       <c r="M38" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="50"/>
       <c r="B39" s="39" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D39" s="31"/>
       <c r="E39" s="31"/>
@@ -2191,51 +2209,51 @@
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
       <c r="M39" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="50"/>
       <c r="B40" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D40" s="32"/>
       <c r="E40" s="32"/>
       <c r="F40" s="32"/>
       <c r="G40" s="11"/>
       <c r="H40" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K40" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L40" s="11"/>
       <c r="M40" s="12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="51"/>
       <c r="B41" s="40" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D41" s="32"/>
       <c r="E41" s="32"/>
@@ -2243,24 +2261,24 @@
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
       <c r="I41" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J41" s="13"/>
       <c r="K41" s="13"/>
       <c r="L41" s="9"/>
       <c r="M41" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="49" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D42" s="30"/>
       <c r="E42" s="30"/>
@@ -2268,24 +2286,24 @@
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J42" s="14"/>
       <c r="K42" s="14" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L42" s="5"/>
       <c r="M42" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="50"/>
       <c r="B43" s="39" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D43" s="31"/>
       <c r="E43" s="31"/>
@@ -2293,24 +2311,24 @@
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J43" s="15"/>
       <c r="K43" s="15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L43" s="7"/>
       <c r="M43" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="50"/>
       <c r="B44" s="39" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D44" s="31"/>
       <c r="E44" s="31"/>
@@ -2318,55 +2336,55 @@
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
       <c r="I44" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J44" s="15"/>
       <c r="K44" s="15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L44" s="7"/>
       <c r="M44" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="50"/>
       <c r="B45" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D45" s="32"/>
       <c r="E45" s="32"/>
       <c r="F45" s="32"/>
       <c r="G45" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J45" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K45" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L45" s="11"/>
       <c r="M45" s="12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="51"/>
       <c r="B46" s="40" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D46" s="32"/>
       <c r="E46" s="32"/>
@@ -2374,26 +2392,26 @@
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
       <c r="I46" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J46" s="9"/>
       <c r="K46" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L46" s="9"/>
       <c r="M46" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="49" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="30"/>
@@ -2404,19 +2422,19 @@
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
       <c r="L47" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="50"/>
       <c r="B48" s="19" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D48" s="31"/>
       <c r="E48" s="31"/>
@@ -2427,19 +2445,19 @@
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
       <c r="L48" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="M48" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="50"/>
       <c r="B49" s="19" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D49" s="31"/>
       <c r="E49" s="31"/>
@@ -2450,19 +2468,19 @@
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
       <c r="L49" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="M49" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="50"/>
       <c r="B50" s="19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D50" s="31"/>
       <c r="E50" s="31"/>
@@ -2473,19 +2491,19 @@
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
       <c r="L50" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="M50" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="50"/>
       <c r="B51" s="24" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D51" s="32"/>
       <c r="E51" s="32"/>
@@ -2496,18 +2514,18 @@
       <c r="J51" s="11"/>
       <c r="K51" s="11"/>
       <c r="L51" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="M51" s="12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="49" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C52" s="20"/>
       <c r="D52" s="30"/>
@@ -2519,16 +2537,16 @@
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
       <c r="L52" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="M52" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="51"/>
       <c r="B53" s="21" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="33"/>
@@ -2540,18 +2558,18 @@
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
       <c r="L53" s="9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="M53" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C54" s="25"/>
       <c r="D54" s="34"/>
@@ -2563,18 +2581,18 @@
       <c r="J54" s="16"/>
       <c r="K54" s="16"/>
       <c r="L54" s="16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="M54" s="17" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="49" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C55" s="27"/>
       <c r="D55" s="30"/>
@@ -2587,13 +2605,13 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
       <c r="M55" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="50"/>
       <c r="B56" s="19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C56" s="19"/>
       <c r="D56" s="35"/>
@@ -2606,13 +2624,13 @@
       <c r="K56" s="7"/>
       <c r="L56" s="7"/>
       <c r="M56" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="50"/>
       <c r="B57" s="24" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C57" s="24"/>
       <c r="D57" s="36"/>
@@ -2625,13 +2643,13 @@
       <c r="K57" s="11"/>
       <c r="L57" s="11"/>
       <c r="M57" s="12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="51"/>
       <c r="B58" s="21" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C58" s="21"/>
       <c r="D58" s="33"/>
@@ -2644,30 +2662,30 @@
       <c r="K58" s="9"/>
       <c r="L58" s="9"/>
       <c r="M58" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G60" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H60" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I60" t="s">
+        <v>68</v>
+      </c>
+      <c r="J60" t="s">
         <v>74</v>
       </c>
-      <c r="J60" t="s">
-        <v>80</v>
-      </c>
       <c r="K60" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="L60" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="M60" s="18" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
# Comprobar Solic Pendiente en: - frmAdquisicionGestion - frmRendicionCrear - frmRendicionModif # DS: - AA003 Modificar Adquisicion - AA004 - Eliminar Adquisición - AA007 - Agregar Inventario # Modificaciones en varios CU y DS
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="146">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -456,13 +456,19 @@
   </si>
   <si>
     <t>Asociar Partida Especial</t>
+  </si>
+  <si>
+    <t>Recopiar Sec</t>
+  </si>
+  <si>
+    <t>Recopiar Todo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,6 +500,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -796,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -891,6 +905,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1173,9 +1188,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,10 +1640,12 @@
       <c r="B16" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="31"/>
+      <c r="D16" s="31" t="s">
+        <v>135</v>
+      </c>
       <c r="E16" s="31"/>
       <c r="F16" s="31"/>
       <c r="G16" s="7"/>
@@ -1698,10 +1715,12 @@
       <c r="B19" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="32"/>
+      <c r="D19" s="32" t="s">
+        <v>135</v>
+      </c>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
       <c r="G19" s="9"/>
@@ -1829,7 +1848,7 @@
         <v>92</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="E24" s="30"/>
       <c r="F24" s="30"/>
@@ -1879,7 +1898,7 @@
         <v>94</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="E26" s="31"/>
       <c r="F26" s="31"/>
@@ -1904,7 +1923,7 @@
         <v>95</v>
       </c>
       <c r="D27" s="32" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="E27" s="32"/>
       <c r="F27" s="32"/>
@@ -1930,7 +1949,7 @@
       <c r="C28" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D28" s="30"/>
+      <c r="D28" s="52"/>
       <c r="E28" s="30"/>
       <c r="F28" s="30"/>
       <c r="G28" s="5" t="s">
@@ -2690,12 +2709,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A33:A36"/>
@@ -2703,6 +2716,12 @@
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#DS: Eliminar Adquisicion	AA004	OK Modificar Inventario	AA005	OK Eliminar Inventario	AA006	OK Agregar Inventario	AA007	OK Crear Asignacion	AA008	OK Buscar Asignacion	AA009	OK
#Corección de varios CU asociados a los DS
##Corrección de archivos código asociados a lo trabajado
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="146">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -896,6 +896,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -905,7 +906,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1190,7 +1190,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,7 +1250,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="38" t="s">
@@ -1279,7 +1279,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="39" t="s">
         <v>2</v>
       </c>
@@ -1312,7 +1312,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="39" t="s">
         <v>3</v>
       </c>
@@ -1337,7 +1337,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="39" t="s">
         <v>4</v>
       </c>
@@ -1360,7 +1360,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="50" t="s">
         <v>57</v>
       </c>
       <c r="B6" s="38" t="s">
@@ -1391,7 +1391,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="51"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="40" t="s">
         <v>59</v>
       </c>
@@ -1416,7 +1416,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="50" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="45" t="s">
@@ -1443,7 +1443,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="46" t="s">
         <v>141</v>
       </c>
@@ -1476,7 +1476,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="50"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="46" t="s">
         <v>140</v>
       </c>
@@ -1501,7 +1501,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="50"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="46" t="s">
         <v>142</v>
       </c>
@@ -1526,7 +1526,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="46" t="s">
         <v>143</v>
       </c>
@@ -1551,7 +1551,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="50" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="42" t="s">
@@ -1580,7 +1580,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="50"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="43" t="s">
         <v>7</v>
       </c>
@@ -1609,7 +1609,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="50"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="43" t="s">
         <v>8</v>
       </c>
@@ -1636,7 +1636,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="50"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="43" t="s">
         <v>9</v>
       </c>
@@ -1661,14 +1661,16 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="50"/>
+      <c r="A17" s="51"/>
       <c r="B17" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="31"/>
+      <c r="D17" s="31" t="s">
+        <v>135</v>
+      </c>
       <c r="E17" s="31"/>
       <c r="F17" s="31"/>
       <c r="G17" s="7"/>
@@ -1686,14 +1688,16 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="50"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="31"/>
+      <c r="D18" s="31" t="s">
+        <v>135</v>
+      </c>
       <c r="E18" s="31"/>
       <c r="F18" s="31"/>
       <c r="G18" s="7"/>
@@ -1711,7 +1715,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="51"/>
+      <c r="A19" s="52"/>
       <c r="B19" s="44" t="s">
         <v>12</v>
       </c>
@@ -1738,16 +1742,18 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="49" t="s">
+      <c r="A20" s="50" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="D20" s="30"/>
+      <c r="D20" s="30" t="s">
+        <v>135</v>
+      </c>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
       <c r="G20" s="5"/>
@@ -1765,14 +1771,16 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50"/>
+      <c r="A21" s="51"/>
       <c r="B21" s="43" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="31"/>
+      <c r="D21" s="31" t="s">
+        <v>135</v>
+      </c>
       <c r="E21" s="31"/>
       <c r="F21" s="31"/>
       <c r="G21" s="7"/>
@@ -1790,7 +1798,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="50"/>
+      <c r="A22" s="51"/>
       <c r="B22" s="43" t="s">
         <v>16</v>
       </c>
@@ -1815,7 +1823,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="51"/>
+      <c r="A23" s="52"/>
       <c r="B23" s="44" t="s">
         <v>17</v>
       </c>
@@ -1838,7 +1846,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="49" t="s">
+      <c r="A24" s="50" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="45" t="s">
@@ -1865,7 +1873,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="50"/>
+      <c r="A25" s="51"/>
       <c r="B25" s="46" t="s">
         <v>20</v>
       </c>
@@ -1890,7 +1898,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="50"/>
+      <c r="A26" s="51"/>
       <c r="B26" s="46" t="s">
         <v>21</v>
       </c>
@@ -1915,7 +1923,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="51"/>
+      <c r="A27" s="52"/>
       <c r="B27" s="47" t="s">
         <v>22</v>
       </c>
@@ -1940,7 +1948,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="50" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="38" t="s">
@@ -1949,7 +1957,7 @@
       <c r="C28" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D28" s="52"/>
+      <c r="D28" s="49"/>
       <c r="E28" s="30"/>
       <c r="F28" s="30"/>
       <c r="G28" s="5" t="s">
@@ -1973,7 +1981,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="50"/>
+      <c r="A29" s="51"/>
       <c r="B29" s="39" t="s">
         <v>25</v>
       </c>
@@ -1996,7 +2004,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="50"/>
+      <c r="A30" s="51"/>
       <c r="B30" s="39" t="s">
         <v>26</v>
       </c>
@@ -2019,7 +2027,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="50"/>
+      <c r="A31" s="51"/>
       <c r="B31" s="39" t="s">
         <v>27</v>
       </c>
@@ -2042,7 +2050,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="51"/>
+      <c r="A32" s="52"/>
       <c r="B32" s="40" t="s">
         <v>37</v>
       </c>
@@ -2065,7 +2073,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="50" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="38" t="s">
@@ -2090,7 +2098,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="50"/>
+      <c r="A34" s="51"/>
       <c r="B34" s="39" t="s">
         <v>30</v>
       </c>
@@ -2121,7 +2129,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="50"/>
+      <c r="A35" s="51"/>
       <c r="B35" s="1" t="s">
         <v>75</v>
       </c>
@@ -2144,7 +2152,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="51"/>
+      <c r="A36" s="52"/>
       <c r="B36" s="40" t="s">
         <v>31</v>
       </c>
@@ -2167,7 +2175,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="49" t="s">
+      <c r="A37" s="50" t="s">
         <v>32</v>
       </c>
       <c r="B37" s="38" t="s">
@@ -2192,7 +2200,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="50"/>
+      <c r="A38" s="51"/>
       <c r="B38" s="39" t="s">
         <v>34</v>
       </c>
@@ -2215,7 +2223,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="50"/>
+      <c r="A39" s="51"/>
       <c r="B39" s="39" t="s">
         <v>35</v>
       </c>
@@ -2238,7 +2246,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="50"/>
+      <c r="A40" s="51"/>
       <c r="B40" s="1" t="s">
         <v>64</v>
       </c>
@@ -2267,7 +2275,7 @@
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="51"/>
+      <c r="A41" s="52"/>
       <c r="B41" s="40" t="s">
         <v>36</v>
       </c>
@@ -2290,7 +2298,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="49" t="s">
+      <c r="A42" s="50" t="s">
         <v>38</v>
       </c>
       <c r="B42" s="38" t="s">
@@ -2317,7 +2325,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="50"/>
+      <c r="A43" s="51"/>
       <c r="B43" s="39" t="s">
         <v>40</v>
       </c>
@@ -2342,7 +2350,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="50"/>
+      <c r="A44" s="51"/>
       <c r="B44" s="39" t="s">
         <v>41</v>
       </c>
@@ -2367,7 +2375,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="50"/>
+      <c r="A45" s="51"/>
       <c r="B45" s="1" t="s">
         <v>65</v>
       </c>
@@ -2398,7 +2406,7 @@
       </c>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="51"/>
+      <c r="A46" s="52"/>
       <c r="B46" s="40" t="s">
         <v>42</v>
       </c>
@@ -2423,7 +2431,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="49" t="s">
+      <c r="A47" s="50" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="20" t="s">
@@ -2448,7 +2456,7 @@
       </c>
     </row>
     <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="50"/>
+      <c r="A48" s="51"/>
       <c r="B48" s="19" t="s">
         <v>45</v>
       </c>
@@ -2471,7 +2479,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="50"/>
+      <c r="A49" s="51"/>
       <c r="B49" s="19" t="s">
         <v>46</v>
       </c>
@@ -2494,7 +2502,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="50"/>
+      <c r="A50" s="51"/>
       <c r="B50" s="19" t="s">
         <v>47</v>
       </c>
@@ -2517,7 +2525,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="50"/>
+      <c r="A51" s="51"/>
       <c r="B51" s="24" t="s">
         <v>67</v>
       </c>
@@ -2540,7 +2548,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="49" t="s">
+      <c r="A52" s="50" t="s">
         <v>48</v>
       </c>
       <c r="B52" s="20" t="s">
@@ -2563,7 +2571,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="51"/>
+      <c r="A53" s="52"/>
       <c r="B53" s="21" t="s">
         <v>50</v>
       </c>
@@ -2607,7 +2615,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="49" t="s">
+      <c r="A55" s="50" t="s">
         <v>53</v>
       </c>
       <c r="B55" s="20" t="s">
@@ -2628,7 +2636,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="50"/>
+      <c r="A56" s="51"/>
       <c r="B56" s="19" t="s">
         <v>55</v>
       </c>
@@ -2647,7 +2655,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="50"/>
+      <c r="A57" s="51"/>
       <c r="B57" s="24" t="s">
         <v>66</v>
       </c>
@@ -2666,7 +2674,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="51"/>
+      <c r="A58" s="52"/>
       <c r="B58" s="21" t="s">
         <v>56</v>
       </c>
@@ -2709,6 +2717,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A33:A36"/>
@@ -2716,12 +2730,6 @@
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#DS Modificar Asignacion	AA010 Eliminar Asignacion	AA011 Agregar Detalle de Solicitud	SC026
#Casos de uso:
SC003 - Modificar Solicitud.docx
SC026 - Agregar Detalle de Solicitud.docx
SC027 - Cambiar Oficio.docx
SC028 - Eliminar Detalle de Solicitud.docx
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="152">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -462,6 +462,24 @@
   </si>
   <si>
     <t>Recopiar Todo</t>
+  </si>
+  <si>
+    <t>Agregar Detalle de Solicitud</t>
+  </si>
+  <si>
+    <t>SC026</t>
+  </si>
+  <si>
+    <t>Cambiar Oficio</t>
+  </si>
+  <si>
+    <t>Eliminar Detalle de Solicitud</t>
+  </si>
+  <si>
+    <t>SC027</t>
+  </si>
+  <si>
+    <t>SC028</t>
   </si>
 </sst>
 </file>
@@ -810,7 +828,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -906,6 +924,14 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1186,11 +1212,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M60"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,10 +1828,12 @@
       <c r="B22" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="31"/>
+      <c r="D22" s="31" t="s">
+        <v>135</v>
+      </c>
       <c r="E22" s="31"/>
       <c r="F22" s="31"/>
       <c r="G22" s="7"/>
@@ -1827,10 +1855,12 @@
       <c r="B23" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="32"/>
+      <c r="D23" s="32" t="s">
+        <v>135</v>
+      </c>
       <c r="E23" s="32"/>
       <c r="F23" s="32"/>
       <c r="G23" s="9"/>
@@ -2692,37 +2722,106 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G60" t="s">
+    <row r="59" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="53"/>
+      <c r="B59" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="D59" s="56" t="s">
+        <v>135</v>
+      </c>
+      <c r="G59" s="55"/>
+      <c r="H59" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="I59" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="J59" s="55"/>
+      <c r="K59" s="55"/>
+      <c r="L59" s="55"/>
+      <c r="M59" s="55"/>
+    </row>
+    <row r="60" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="53"/>
+      <c r="B60" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="C60" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="G60" s="55"/>
+      <c r="H60" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="I60" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="J60" s="55"/>
+      <c r="K60" s="55"/>
+      <c r="L60" s="55"/>
+      <c r="M60" s="55"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="53"/>
+      <c r="B61" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="G61" s="55"/>
+      <c r="H61" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="I61" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="J61" s="55"/>
+      <c r="K61" s="55"/>
+      <c r="L61" s="55"/>
+      <c r="M61" s="55"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="53"/>
+      <c r="B62" s="54"/>
+      <c r="C62" s="54"/>
+      <c r="G62" s="55"/>
+      <c r="H62" s="55"/>
+      <c r="I62" s="55"/>
+      <c r="J62" s="55"/>
+      <c r="K62" s="55"/>
+      <c r="L62" s="55"/>
+      <c r="M62" s="55"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
         <v>69</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H64" t="s">
         <v>70</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I64" t="s">
         <v>68</v>
       </c>
-      <c r="J60" t="s">
+      <c r="J64" t="s">
         <v>74</v>
       </c>
-      <c r="K60" t="s">
+      <c r="K64" t="s">
         <v>71</v>
       </c>
-      <c r="L60" t="s">
+      <c r="L64" t="s">
         <v>73</v>
       </c>
-      <c r="M60" s="18" t="s">
+      <c r="M64" s="18" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A33:A36"/>
@@ -2730,6 +2829,12 @@
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#Todos los casos de uso y diagramas de secuencia del negocio REALIZADOS #Manual del usuario empezado #Mapa de navegación
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="152">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -486,7 +486,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,16 +523,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -577,12 +569,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -828,7 +814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -893,8 +879,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -906,15 +890,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -924,14 +915,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1215,8 +1198,8 @@
   <dimension ref="A1:M64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,7 +1236,7 @@
       <c r="F1" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="46" t="s">
         <v>79</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1262,10 +1245,10 @@
       <c r="I1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="39" t="s">
         <v>80</v>
       </c>
       <c r="L1" s="24" t="s">
@@ -1276,20 +1259,20 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="37"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="35"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
         <v>60</v>
@@ -1305,18 +1288,18 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51"/>
-      <c r="B3" s="39" t="s">
+      <c r="A3" s="52"/>
+      <c r="B3" s="37" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
       <c r="G3" s="7" t="s">
         <v>60</v>
       </c>
@@ -1338,16 +1321,18 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
-      <c r="B4" s="39" t="s">
+      <c r="A4" s="52"/>
+      <c r="B4" s="37" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="D4" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7" t="s">
         <v>60</v>
@@ -1363,16 +1348,18 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
-      <c r="B5" s="39" t="s">
+      <c r="A5" s="52"/>
+      <c r="B5" s="37" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
+      <c r="D5" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7" t="s">
@@ -1386,22 +1373,22 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="36" t="s">
         <v>58</v>
       </c>
       <c r="C6" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="E6" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="F6" s="30" t="s">
+      <c r="E6" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="28" t="s">
         <v>135</v>
       </c>
       <c r="G6" s="5"/>
@@ -1417,18 +1404,18 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
-      <c r="B7" s="40" t="s">
+      <c r="A7" s="53"/>
+      <c r="B7" s="38" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
       <c r="G7" s="9"/>
       <c r="H7" s="13"/>
       <c r="I7" s="9" t="s">
@@ -1442,20 +1429,20 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="43" t="s">
         <v>138</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
       <c r="G8" s="26" t="s">
         <v>60</v>
       </c>
@@ -1469,18 +1456,18 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="51"/>
-      <c r="B9" s="46" t="s">
+      <c r="A9" s="52"/>
+      <c r="B9" s="44" t="s">
         <v>141</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
       <c r="G9" s="7" t="s">
         <v>60</v>
       </c>
@@ -1502,18 +1489,18 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51"/>
-      <c r="B10" s="46" t="s">
+      <c r="A10" s="52"/>
+      <c r="B10" s="44" t="s">
         <v>140</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
       <c r="G10" s="26" t="s">
         <v>60</v>
       </c>
@@ -1527,18 +1514,18 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="51"/>
-      <c r="B11" s="46" t="s">
+      <c r="A11" s="52"/>
+      <c r="B11" s="44" t="s">
         <v>142</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
       <c r="G11" s="7" t="s">
         <v>60</v>
       </c>
@@ -1552,18 +1539,18 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="51"/>
-      <c r="B12" s="46" t="s">
+      <c r="A12" s="52"/>
+      <c r="B12" s="44" t="s">
         <v>143</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
       <c r="G12" s="7" t="s">
         <v>60</v>
       </c>
@@ -1577,20 +1564,20 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="40" t="s">
         <v>137</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1606,18 +1593,18 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="51"/>
-      <c r="B14" s="43" t="s">
+      <c r="A14" s="52"/>
+      <c r="B14" s="41" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
+      <c r="D14" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
       <c r="G14" s="7" t="s">
         <v>60</v>
       </c>
@@ -1635,18 +1622,18 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="51"/>
-      <c r="B15" s="43" t="s">
+      <c r="A15" s="52"/>
+      <c r="B15" s="41" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
+      <c r="D15" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -1662,18 +1649,18 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="51"/>
-      <c r="B16" s="43" t="s">
+      <c r="A16" s="52"/>
+      <c r="B16" s="41" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
+      <c r="D16" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -1687,18 +1674,18 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="51"/>
-      <c r="B17" s="43" t="s">
+      <c r="A17" s="52"/>
+      <c r="B17" s="41" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
+      <c r="D17" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -1714,18 +1701,18 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="51"/>
-      <c r="B18" s="43" t="s">
+      <c r="A18" s="52"/>
+      <c r="B18" s="41" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
+      <c r="D18" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -1741,18 +1728,18 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="52"/>
-      <c r="B19" s="44" t="s">
+      <c r="A19" s="53"/>
+      <c r="B19" s="42" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
+      <c r="D19" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -1768,20 +1755,20 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="40" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="D20" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
+      <c r="D20" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1797,18 +1784,18 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="51"/>
-      <c r="B21" s="43" t="s">
+      <c r="A21" s="52"/>
+      <c r="B21" s="41" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
+      <c r="D21" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -1824,18 +1811,18 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="51"/>
-      <c r="B22" s="43" t="s">
+      <c r="A22" s="52"/>
+      <c r="B22" s="41" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
+      <c r="D22" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -1851,18 +1838,18 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="52"/>
-      <c r="B23" s="44" t="s">
+      <c r="A23" s="53"/>
+      <c r="B23" s="42" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
+      <c r="D23" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
@@ -1876,20 +1863,20 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="43" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
       <c r="G24" s="5" t="s">
         <v>60</v>
       </c>
@@ -1903,18 +1890,18 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="51"/>
-      <c r="B25" s="46" t="s">
+      <c r="A25" s="52"/>
+      <c r="B25" s="44" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
       <c r="G25" s="7" t="s">
         <v>60</v>
       </c>
@@ -1928,18 +1915,18 @@
       </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="51"/>
-      <c r="B26" s="46" t="s">
+      <c r="A26" s="52"/>
+      <c r="B26" s="44" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
       <c r="G26" s="7" t="s">
         <v>60</v>
       </c>
@@ -1953,18 +1940,18 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="52"/>
-      <c r="B27" s="47" t="s">
+      <c r="A27" s="53"/>
+      <c r="B27" s="45" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
       <c r="G27" s="9" t="s">
         <v>60</v>
       </c>
@@ -1978,18 +1965,20 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B28" s="36" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D28" s="49"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
+      <c r="D28" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
       <c r="G28" s="5" t="s">
         <v>60</v>
       </c>
@@ -2011,16 +2000,18 @@
       </c>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="51"/>
-      <c r="B29" s="39" t="s">
+      <c r="A29" s="52"/>
+      <c r="B29" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
+      <c r="D29" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7" t="s">
         <v>60</v>
@@ -2034,16 +2025,18 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="51"/>
-      <c r="B30" s="39" t="s">
+      <c r="A30" s="52"/>
+      <c r="B30" s="37" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
+      <c r="D30" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7" t="s">
         <v>60</v>
@@ -2057,16 +2050,18 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="51"/>
-      <c r="B31" s="39" t="s">
+      <c r="A31" s="52"/>
+      <c r="B31" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
+      <c r="D31" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7" t="s">
         <v>60</v>
@@ -2080,16 +2075,18 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="52"/>
-      <c r="B32" s="40" t="s">
+      <c r="A32" s="53"/>
+      <c r="B32" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
+      <c r="D32" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9" t="s">
         <v>60</v>
@@ -2103,18 +2100,20 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="50" t="s">
+      <c r="A33" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
+      <c r="D33" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5" t="s">
@@ -2128,16 +2127,18 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="51"/>
-      <c r="B34" s="39" t="s">
+      <c r="A34" s="52"/>
+      <c r="B34" s="37" t="s">
         <v>30</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
+      <c r="D34" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
       <c r="G34" s="7" t="s">
         <v>60</v>
       </c>
@@ -2159,16 +2160,18 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="51"/>
+      <c r="A35" s="52"/>
       <c r="B35" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
+      <c r="D35" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
       <c r="G35" s="22"/>
       <c r="H35" s="22"/>
       <c r="I35" s="22" t="s">
@@ -2182,16 +2185,18 @@
       </c>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="52"/>
-      <c r="B36" s="40" t="s">
+      <c r="A36" s="53"/>
+      <c r="B36" s="38" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
+      <c r="D36" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9" t="s">
@@ -2205,18 +2210,20 @@
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="50" t="s">
+      <c r="A37" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="36" t="s">
         <v>33</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
+      <c r="D37" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5" t="s">
@@ -2230,16 +2237,18 @@
       </c>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="51"/>
-      <c r="B38" s="39" t="s">
+      <c r="A38" s="52"/>
+      <c r="B38" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C38" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="D38" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7" t="s">
@@ -2253,16 +2262,18 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="51"/>
-      <c r="B39" s="39" t="s">
+      <c r="A39" s="52"/>
+      <c r="B39" s="37" t="s">
         <v>35</v>
       </c>
       <c r="C39" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
+      <c r="D39" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7" t="s">
@@ -2276,16 +2287,18 @@
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="51"/>
+      <c r="A40" s="52"/>
       <c r="B40" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
+      <c r="D40" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
       <c r="G40" s="11"/>
       <c r="H40" s="11" t="s">
         <v>60</v>
@@ -2305,16 +2318,18 @@
       </c>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="52"/>
-      <c r="B41" s="40" t="s">
+      <c r="A41" s="53"/>
+      <c r="B41" s="38" t="s">
         <v>36</v>
       </c>
       <c r="C41" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
+      <c r="D41" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
       <c r="I41" s="9" t="s">
@@ -2328,18 +2343,20 @@
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="38" t="s">
+      <c r="B42" s="36" t="s">
         <v>39</v>
       </c>
       <c r="C42" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
+      <c r="D42" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5" t="s">
@@ -2355,16 +2372,18 @@
       </c>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="51"/>
-      <c r="B43" s="39" t="s">
+      <c r="A43" s="52"/>
+      <c r="B43" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="28" t="s">
+      <c r="C43" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
+      <c r="D43" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7" t="s">
@@ -2380,16 +2399,18 @@
       </c>
     </row>
     <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="51"/>
-      <c r="B44" s="39" t="s">
+      <c r="A44" s="52"/>
+      <c r="B44" s="37" t="s">
         <v>41</v>
       </c>
       <c r="C44" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
+      <c r="D44" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
       <c r="I44" s="7" t="s">
@@ -2405,16 +2426,18 @@
       </c>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="51"/>
+      <c r="A45" s="52"/>
       <c r="B45" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="28" t="s">
+      <c r="C45" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
+      <c r="D45" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
       <c r="G45" s="11" t="s">
         <v>60</v>
       </c>
@@ -2436,16 +2459,18 @@
       </c>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="52"/>
-      <c r="B46" s="40" t="s">
+      <c r="A46" s="53"/>
+      <c r="B46" s="38" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
+      <c r="D46" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
       <c r="I46" s="9" t="s">
@@ -2461,7 +2486,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="50" t="s">
+      <c r="A47" s="51" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="20" t="s">
@@ -2470,9 +2495,9 @@
       <c r="C47" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
@@ -2486,16 +2511,16 @@
       </c>
     </row>
     <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="51"/>
+      <c r="A48" s="52"/>
       <c r="B48" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C48" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
@@ -2509,16 +2534,16 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="51"/>
+      <c r="A49" s="52"/>
       <c r="B49" s="19" t="s">
         <v>46</v>
       </c>
       <c r="C49" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
@@ -2532,16 +2557,16 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="51"/>
+      <c r="A50" s="52"/>
       <c r="B50" s="19" t="s">
         <v>47</v>
       </c>
       <c r="C50" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
@@ -2555,16 +2580,16 @@
       </c>
     </row>
     <row r="51" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="51"/>
+      <c r="A51" s="52"/>
       <c r="B51" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C51" s="28" t="s">
+      <c r="C51" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
       <c r="I51" s="11"/>
@@ -2578,16 +2603,16 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="50" t="s">
+      <c r="A52" s="51" t="s">
         <v>48</v>
       </c>
       <c r="B52" s="20" t="s">
         <v>49</v>
       </c>
       <c r="C52" s="20"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="30"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
@@ -2601,14 +2626,14 @@
       </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="52"/>
+      <c r="A53" s="53"/>
       <c r="B53" s="21" t="s">
         <v>50</v>
       </c>
       <c r="C53" s="21"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
       <c r="G53" s="9"/>
       <c r="H53" s="9"/>
       <c r="I53" s="9"/>
@@ -2629,9 +2654,9 @@
         <v>52</v>
       </c>
       <c r="C54" s="25"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
       <c r="G54" s="16"/>
       <c r="H54" s="16"/>
       <c r="I54" s="16"/>
@@ -2645,16 +2670,16 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="50" t="s">
+      <c r="A55" s="51" t="s">
         <v>53</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>54</v>
       </c>
       <c r="C55" s="27"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
@@ -2666,14 +2691,14 @@
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="51"/>
+      <c r="A56" s="52"/>
       <c r="B56" s="19" t="s">
         <v>55</v>
       </c>
       <c r="C56" s="19"/>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="35"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="33"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
@@ -2685,14 +2710,14 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="51"/>
+      <c r="A57" s="52"/>
       <c r="B57" s="24" t="s">
         <v>66</v>
       </c>
       <c r="C57" s="24"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="34"/>
       <c r="G57" s="11"/>
       <c r="H57" s="11"/>
       <c r="I57" s="11"/>
@@ -2704,14 +2729,14 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="52"/>
+      <c r="A58" s="53"/>
       <c r="B58" s="21" t="s">
         <v>56</v>
       </c>
       <c r="C58" s="21"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="33"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="31"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
@@ -2723,79 +2748,85 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="53"/>
-      <c r="B59" s="38" t="s">
+      <c r="A59" s="47"/>
+      <c r="B59" s="36" t="s">
         <v>146</v>
       </c>
       <c r="C59" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="D59" s="56" t="s">
-        <v>135</v>
-      </c>
-      <c r="G59" s="55"/>
-      <c r="H59" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="I59" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="J59" s="55"/>
-      <c r="K59" s="55"/>
-      <c r="L59" s="55"/>
-      <c r="M59" s="55"/>
+      <c r="D59" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="G59" s="49"/>
+      <c r="H59" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="I59" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="J59" s="49"/>
+      <c r="K59" s="49"/>
+      <c r="L59" s="49"/>
+      <c r="M59" s="49"/>
     </row>
     <row r="60" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="53"/>
-      <c r="B60" s="38" t="s">
+      <c r="A60" s="47"/>
+      <c r="B60" s="36" t="s">
         <v>148</v>
       </c>
       <c r="C60" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="G60" s="55"/>
-      <c r="H60" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="I60" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="J60" s="55"/>
-      <c r="K60" s="55"/>
-      <c r="L60" s="55"/>
-      <c r="M60" s="55"/>
+      <c r="D60" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="G60" s="49"/>
+      <c r="H60" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="I60" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="J60" s="49"/>
+      <c r="K60" s="49"/>
+      <c r="L60" s="49"/>
+      <c r="M60" s="49"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="53"/>
-      <c r="B61" s="38" t="s">
+      <c r="A61" s="47"/>
+      <c r="B61" s="36" t="s">
         <v>149</v>
       </c>
       <c r="C61" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="G61" s="55"/>
-      <c r="H61" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="I61" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="J61" s="55"/>
-      <c r="K61" s="55"/>
-      <c r="L61" s="55"/>
-      <c r="M61" s="55"/>
+      <c r="D61" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="G61" s="49"/>
+      <c r="H61" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="I61" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="J61" s="49"/>
+      <c r="K61" s="49"/>
+      <c r="L61" s="49"/>
+      <c r="M61" s="49"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="53"/>
-      <c r="B62" s="54"/>
-      <c r="C62" s="54"/>
-      <c r="G62" s="55"/>
-      <c r="H62" s="55"/>
-      <c r="I62" s="55"/>
-      <c r="J62" s="55"/>
-      <c r="K62" s="55"/>
-      <c r="L62" s="55"/>
-      <c r="M62" s="55"/>
+      <c r="A62" s="47"/>
+      <c r="B62" s="48"/>
+      <c r="C62" s="48"/>
+      <c r="G62" s="49"/>
+      <c r="H62" s="49"/>
+      <c r="I62" s="49"/>
+      <c r="J62" s="49"/>
+      <c r="K62" s="49"/>
+      <c r="L62" s="49"/>
+      <c r="M62" s="49"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G64" t="s">
@@ -2822,6 +2853,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A33:A36"/>
@@ -2829,12 +2866,6 @@
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#DS y CU de Administración Usuarios #Logs en todas las funcionalidades (falta traducciones varias)
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="152">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -1198,8 +1198,8 @@
   <dimension ref="A1:M64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2495,7 +2495,9 @@
       <c r="C47" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D47" s="28"/>
+      <c r="D47" s="28" t="s">
+        <v>135</v>
+      </c>
       <c r="E47" s="28"/>
       <c r="F47" s="28"/>
       <c r="G47" s="5"/>
@@ -2518,7 +2520,9 @@
       <c r="C48" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="D48" s="29"/>
+      <c r="D48" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="E48" s="29"/>
       <c r="F48" s="29"/>
       <c r="G48" s="7"/>
@@ -2541,7 +2545,9 @@
       <c r="C49" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D49" s="29"/>
+      <c r="D49" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="E49" s="29"/>
       <c r="F49" s="29"/>
       <c r="G49" s="7"/>
@@ -2564,7 +2570,9 @@
       <c r="C50" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="D50" s="29"/>
+      <c r="D50" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="E50" s="29"/>
       <c r="F50" s="29"/>
       <c r="G50" s="7"/>
@@ -2587,7 +2595,9 @@
       <c r="C51" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D51" s="30"/>
+      <c r="D51" s="30" t="s">
+        <v>135</v>
+      </c>
       <c r="E51" s="30"/>
       <c r="F51" s="30"/>
       <c r="G51" s="11"/>
@@ -2853,12 +2863,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A33:A36"/>
@@ -2866,6 +2870,12 @@
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
2da Entrega: - Crear Solicitud revisado OK - Agregar Cotizacion revisado OK
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="152">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -814,7 +814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -886,7 +886,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -915,6 +914,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1195,11 +1198,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M64"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,19 +1210,20 @@
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="41" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>63</v>
@@ -1228,81 +1232,89 @@
         <v>131</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="H1" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="K1" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="L1" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="N1" s="24" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="D2" s="53">
+        <v>43634</v>
+      </c>
+      <c r="E2" s="53">
+        <v>43634</v>
+      </c>
+      <c r="F2" s="53">
+        <v>43634</v>
+      </c>
+      <c r="G2" s="53">
+        <v>43634</v>
+      </c>
+      <c r="H2" s="5"/>
       <c r="I2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="J2" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
-      <c r="M2" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52"/>
-      <c r="B3" s="37" t="s">
+      <c r="M2" s="5"/>
+      <c r="N2" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="51"/>
+      <c r="B3" s="36" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="54"/>
+      <c r="E3" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="29"/>
       <c r="F3" s="29"/>
-      <c r="G3" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="G3" s="29"/>
       <c r="H3" s="7" t="s">
         <v>60</v>
       </c>
@@ -1315,673 +1327,708 @@
       <c r="K3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="52"/>
-      <c r="B4" s="37" t="s">
+      <c r="L3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" s="7"/>
+      <c r="N3" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="51"/>
+      <c r="B4" s="36" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E4" s="29"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F4" s="29"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="G4" s="29"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="7"/>
+      <c r="J4" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
-      <c r="M4" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="37" t="s">
+      <c r="M4" s="7"/>
+      <c r="N4" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="51"/>
+      <c r="B5" s="36" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E5" s="29"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F5" s="29"/>
-      <c r="G5" s="7"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
-      <c r="M5" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="51" t="s">
+      <c r="M5" s="7"/>
+      <c r="N5" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>58</v>
       </c>
       <c r="C6" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="27"/>
+      <c r="E6" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="E6" s="28" t="s">
-        <v>135</v>
-      </c>
       <c r="F6" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="J6" s="5"/>
+      <c r="G6" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="53"/>
-      <c r="B7" s="38" t="s">
+      <c r="M6" s="5"/>
+      <c r="N6" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="52"/>
+      <c r="B7" s="37" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" s="9"/>
+      <c r="D7" s="53">
+        <v>43634</v>
+      </c>
+      <c r="E7" s="53">
+        <v>43634</v>
+      </c>
+      <c r="F7" s="53">
+        <v>43634</v>
+      </c>
+      <c r="G7" s="53">
+        <v>43634</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
-      <c r="M7" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="51" t="s">
+      <c r="M7" s="9"/>
+      <c r="N7" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="42" t="s">
         <v>138</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="27"/>
+      <c r="E8" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="E8" s="28"/>
       <c r="F8" s="28"/>
-      <c r="G8" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="5"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="52"/>
-      <c r="B9" s="44" t="s">
+      <c r="M8" s="5"/>
+      <c r="N8" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="51"/>
+      <c r="B9" s="43" t="s">
         <v>141</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="54"/>
+      <c r="E9" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="29"/>
       <c r="F9" s="29"/>
-      <c r="G9" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="G9" s="29"/>
       <c r="H9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="J9" s="7" t="s">
+      <c r="I9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="22" t="s">
         <v>60</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
-      <c r="B10" s="44" t="s">
+      <c r="L9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="7"/>
+      <c r="N9" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="B10" s="43" t="s">
         <v>140</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="54"/>
+      <c r="E10" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="E10" s="29"/>
       <c r="F10" s="29"/>
-      <c r="G10" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="7"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="15"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
-      <c r="M10" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="52"/>
-      <c r="B11" s="44" t="s">
+      <c r="M10" s="7"/>
+      <c r="N10" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="51"/>
+      <c r="B11" s="43" t="s">
         <v>142</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="54"/>
+      <c r="E11" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="E11" s="29"/>
       <c r="F11" s="29"/>
-      <c r="G11" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="7"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-      <c r="M11" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="52"/>
-      <c r="B12" s="44" t="s">
+      <c r="M11" s="7"/>
+      <c r="N11" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="51"/>
+      <c r="B12" s="43" t="s">
         <v>143</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="54"/>
+      <c r="E12" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="E12" s="29"/>
       <c r="F12" s="29"/>
-      <c r="G12" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="7"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
-      <c r="M12" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="51" t="s">
+      <c r="M12" s="7"/>
+      <c r="N12" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="39" t="s">
         <v>137</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="27"/>
+      <c r="E13" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="5"/>
+      <c r="F13" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>136</v>
+      </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="J13" s="5"/>
       <c r="K13" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="52"/>
-      <c r="B14" s="41" t="s">
+      <c r="L13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="M13" s="5"/>
+      <c r="N13" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="51"/>
+      <c r="B14" s="40" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" s="29"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F14" s="29"/>
-      <c r="G14" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="7"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="I14" s="7"/>
-      <c r="J14" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="J14" s="7"/>
       <c r="K14" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L14" s="7"/>
-      <c r="M14" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="52"/>
-      <c r="B15" s="41" t="s">
+      <c r="L14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M14" s="7"/>
+      <c r="N14" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="51"/>
+      <c r="B15" s="40" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" s="29"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F15" s="29"/>
-      <c r="G15" s="7"/>
+      <c r="G15" s="29"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="J15" s="7"/>
       <c r="K15" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L15" s="7"/>
-      <c r="M15" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="52"/>
-      <c r="B16" s="41" t="s">
+      <c r="L15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M15" s="7"/>
+      <c r="N15" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="51"/>
+      <c r="B16" s="40" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" s="29"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F16" s="29"/>
-      <c r="G16" s="7"/>
+      <c r="G16" s="29"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-      <c r="K16" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="L16" s="7"/>
-      <c r="M16" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="52"/>
-      <c r="B17" s="41" t="s">
+      <c r="K16" s="7"/>
+      <c r="L16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M16" s="7"/>
+      <c r="N16" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="51"/>
+      <c r="B17" s="40" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E17" s="29"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="7"/>
+      <c r="G17" s="29"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="J17" s="7"/>
       <c r="K17" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L17" s="7"/>
-      <c r="M17" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="52"/>
-      <c r="B18" s="41" t="s">
+      <c r="L17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M17" s="7"/>
+      <c r="N17" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="51"/>
+      <c r="B18" s="40" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E18" s="29"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F18" s="29"/>
-      <c r="G18" s="7"/>
+      <c r="G18" s="29"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="J18" s="7"/>
       <c r="K18" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L18" s="7"/>
-      <c r="M18" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="53"/>
-      <c r="B19" s="42" t="s">
+      <c r="L18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M18" s="7"/>
+      <c r="N18" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="52"/>
+      <c r="B19" s="41" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="E19" s="30"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="30" t="s">
+        <v>135</v>
+      </c>
       <c r="F19" s="30"/>
-      <c r="G19" s="9"/>
+      <c r="G19" s="30"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
-      <c r="J19" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="J19" s="9"/>
       <c r="K19" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="L19" s="9"/>
-      <c r="M19" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="51" t="s">
+      <c r="L19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="M19" s="9"/>
+      <c r="N19" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="39" t="s">
         <v>14</v>
       </c>
       <c r="C20" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="D20" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="E20" s="28"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28" t="s">
+        <v>135</v>
+      </c>
       <c r="F20" s="28"/>
-      <c r="G20" s="5"/>
+      <c r="G20" s="28"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="J20" s="5"/>
       <c r="K20" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L20" s="5"/>
-      <c r="M20" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="52"/>
-      <c r="B21" s="41" t="s">
+      <c r="L20" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="M20" s="5"/>
+      <c r="N20" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="51"/>
+      <c r="B21" s="40" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E21" s="29"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="7"/>
+      <c r="G21" s="29"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="J21" s="7"/>
       <c r="K21" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L21" s="7"/>
-      <c r="M21" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="52"/>
-      <c r="B22" s="41" t="s">
+      <c r="L21" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M21" s="7"/>
+      <c r="N21" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="51"/>
+      <c r="B22" s="40" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E22" s="29"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F22" s="29"/>
-      <c r="G22" s="7"/>
+      <c r="G22" s="29"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="J22" s="7"/>
       <c r="K22" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L22" s="7"/>
-      <c r="M22" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="53"/>
-      <c r="B23" s="42" t="s">
+      <c r="L22" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M22" s="7"/>
+      <c r="N22" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="52"/>
+      <c r="B23" s="41" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="E23" s="30"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="30" t="s">
+        <v>135</v>
+      </c>
       <c r="F23" s="30"/>
-      <c r="G23" s="9"/>
+      <c r="G23" s="30"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
-      <c r="K23" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="L23" s="9"/>
-      <c r="M23" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="51" t="s">
+      <c r="K23" s="9"/>
+      <c r="L23" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="M23" s="9"/>
+      <c r="N23" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="42" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="27"/>
+      <c r="E24" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="E24" s="28"/>
       <c r="F24" s="28"/>
-      <c r="G24" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H24" s="5"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
-      <c r="M24" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="52"/>
-      <c r="B25" s="44" t="s">
+      <c r="M24" s="5"/>
+      <c r="N24" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="51"/>
+      <c r="B25" s="43" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="54"/>
+      <c r="E25" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="E25" s="29"/>
       <c r="F25" s="29"/>
-      <c r="G25" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H25" s="7"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
-      <c r="M25" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="52"/>
-      <c r="B26" s="44" t="s">
+      <c r="M25" s="7"/>
+      <c r="N25" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="51"/>
+      <c r="B26" s="43" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="54"/>
+      <c r="E26" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="E26" s="29"/>
       <c r="F26" s="29"/>
-      <c r="G26" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H26" s="7"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
-      <c r="M26" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="53"/>
-      <c r="B27" s="45" t="s">
+      <c r="M26" s="7"/>
+      <c r="N26" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="52"/>
+      <c r="B27" s="44" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D27" s="55"/>
+      <c r="E27" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="E27" s="30"/>
       <c r="F27" s="30"/>
-      <c r="G27" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="H27" s="9"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
-      <c r="M27" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="51" t="s">
+      <c r="M27" s="9"/>
+      <c r="N27" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="35" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D28" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="E28" s="28"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="28" t="s">
+        <v>135</v>
+      </c>
       <c r="F28" s="28"/>
-      <c r="G28" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="G28" s="28"/>
       <c r="H28" s="5" t="s">
         <v>60</v>
       </c>
@@ -1994,154 +2041,160 @@
       <c r="K28" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L28" s="5"/>
-      <c r="M28" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="52"/>
-      <c r="B29" s="37" t="s">
+      <c r="L28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="M28" s="5"/>
+      <c r="N28" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="51"/>
+      <c r="B29" s="36" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="D29" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E29" s="29"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I29" s="7"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
-      <c r="M29" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="52"/>
-      <c r="B30" s="37" t="s">
+      <c r="M29" s="7"/>
+      <c r="N29" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="51"/>
+      <c r="B30" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="D30" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E30" s="29"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F30" s="29"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I30" s="7"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
-      <c r="M30" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="52"/>
-      <c r="B31" s="37" t="s">
+      <c r="M30" s="7"/>
+      <c r="N30" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="51"/>
+      <c r="B31" s="36" t="s">
         <v>27</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E31" s="29"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F31" s="29"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="I31" s="7"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
-      <c r="M31" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="53"/>
-      <c r="B32" s="38" t="s">
+      <c r="M31" s="7"/>
+      <c r="N31" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="52"/>
+      <c r="B32" s="37" t="s">
         <v>37</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="D32" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="E32" s="30"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="30" t="s">
+        <v>135</v>
+      </c>
       <c r="F32" s="30"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="I32" s="9"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
-      <c r="M32" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="51" t="s">
+      <c r="M32" s="9"/>
+      <c r="N32" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="35" t="s">
         <v>29</v>
       </c>
       <c r="C33" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="D33" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="E33" s="28"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="28" t="s">
+        <v>135</v>
+      </c>
       <c r="F33" s="28"/>
-      <c r="G33" s="5"/>
+      <c r="G33" s="28"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="J33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
-      <c r="M33" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="52"/>
-      <c r="B34" s="37" t="s">
+      <c r="M33" s="5"/>
+      <c r="N33" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="51"/>
+      <c r="B34" s="36" t="s">
         <v>30</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="D34" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E34" s="29"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F34" s="29"/>
-      <c r="G34" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="G34" s="29"/>
       <c r="H34" s="7" t="s">
         <v>60</v>
       </c>
@@ -2154,155 +2207,161 @@
       <c r="K34" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="L34" s="7"/>
-      <c r="M34" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="52"/>
+      <c r="L34" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M34" s="7"/>
+      <c r="N34" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="51"/>
       <c r="B35" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C35" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="D35" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="E35" s="30"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="30" t="s">
+        <v>135</v>
+      </c>
       <c r="F35" s="30"/>
-      <c r="G35" s="22"/>
+      <c r="G35" s="30"/>
       <c r="H35" s="22"/>
-      <c r="I35" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="J35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22" t="s">
+        <v>60</v>
+      </c>
       <c r="K35" s="22"/>
       <c r="L35" s="22"/>
-      <c r="M35" s="23" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="53"/>
-      <c r="B36" s="38" t="s">
+      <c r="M35" s="22"/>
+      <c r="N35" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="52"/>
+      <c r="B36" s="37" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="D36" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="E36" s="31"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="31" t="s">
+        <v>135</v>
+      </c>
       <c r="F36" s="31"/>
-      <c r="G36" s="9"/>
+      <c r="G36" s="31"/>
       <c r="H36" s="9"/>
-      <c r="I36" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="J36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="K36" s="9"/>
       <c r="L36" s="9"/>
-      <c r="M36" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="51" t="s">
+      <c r="M36" s="9"/>
+      <c r="N36" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="35" t="s">
         <v>33</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="E37" s="28"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="28" t="s">
+        <v>135</v>
+      </c>
       <c r="F37" s="28"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="28"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="J37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
-      <c r="M37" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="52"/>
-      <c r="B38" s="37" t="s">
+      <c r="M37" s="5"/>
+      <c r="N37" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="51"/>
+      <c r="B38" s="36" t="s">
         <v>34</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="D38" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E38" s="29"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F38" s="29"/>
-      <c r="G38" s="7"/>
+      <c r="G38" s="29"/>
       <c r="H38" s="7"/>
-      <c r="I38" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="K38" s="7"/>
       <c r="L38" s="7"/>
-      <c r="M38" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="52"/>
-      <c r="B39" s="37" t="s">
+      <c r="M38" s="7"/>
+      <c r="N38" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="51"/>
+      <c r="B39" s="36" t="s">
         <v>35</v>
       </c>
       <c r="C39" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="D39" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E39" s="29"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F39" s="29"/>
-      <c r="G39" s="7"/>
+      <c r="G39" s="29"/>
       <c r="H39" s="7"/>
-      <c r="I39" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
-      <c r="M39" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="52"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="51"/>
       <c r="B40" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C40" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="E40" s="30"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="30" t="s">
+        <v>135</v>
+      </c>
       <c r="F40" s="30"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11" t="s">
-        <v>60</v>
-      </c>
+      <c r="G40" s="30"/>
+      <c r="H40" s="11"/>
       <c r="I40" s="11" t="s">
         <v>60</v>
       </c>
@@ -2312,135 +2371,140 @@
       <c r="K40" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="L40" s="11"/>
-      <c r="M40" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="53"/>
-      <c r="B41" s="38" t="s">
+      <c r="L40" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="M40" s="11"/>
+      <c r="N40" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="52"/>
+      <c r="B41" s="37" t="s">
         <v>36</v>
       </c>
       <c r="C41" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="E41" s="30"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="31" t="s">
+        <v>135</v>
+      </c>
       <c r="F41" s="30"/>
-      <c r="G41" s="9"/>
+      <c r="G41" s="30"/>
       <c r="H41" s="9"/>
-      <c r="I41" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="J41" s="13"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="K41" s="13"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="51" t="s">
+      <c r="L41" s="13"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="36" t="s">
+      <c r="B42" s="35" t="s">
         <v>39</v>
       </c>
       <c r="C42" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="E42" s="28"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="28" t="s">
+        <v>135</v>
+      </c>
       <c r="F42" s="28"/>
-      <c r="G42" s="5"/>
+      <c r="G42" s="28"/>
       <c r="H42" s="5"/>
-      <c r="I42" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="L42" s="5"/>
-      <c r="M42" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="52"/>
-      <c r="B43" s="37" t="s">
+      <c r="I42" s="5"/>
+      <c r="J42" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="M42" s="5"/>
+      <c r="N42" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="51"/>
+      <c r="B43" s="36" t="s">
         <v>40</v>
       </c>
       <c r="C43" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D43" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E43" s="29"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F43" s="29"/>
-      <c r="G43" s="7"/>
+      <c r="G43" s="29"/>
       <c r="H43" s="7"/>
-      <c r="I43" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="L43" s="7"/>
-      <c r="M43" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="52"/>
-      <c r="B44" s="37" t="s">
+      <c r="I43" s="7"/>
+      <c r="J43" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="M43" s="7"/>
+      <c r="N43" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="51"/>
+      <c r="B44" s="36" t="s">
         <v>41</v>
       </c>
       <c r="C44" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="D44" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E44" s="29"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F44" s="29"/>
-      <c r="G44" s="7"/>
+      <c r="G44" s="29"/>
       <c r="H44" s="7"/>
-      <c r="I44" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="L44" s="7"/>
-      <c r="M44" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="52"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="M44" s="7"/>
+      <c r="N44" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="51"/>
       <c r="B45" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C45" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D45" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="E45" s="30"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="30" t="s">
+        <v>135</v>
+      </c>
       <c r="F45" s="30"/>
-      <c r="G45" s="11" t="s">
-        <v>60</v>
-      </c>
+      <c r="G45" s="30"/>
       <c r="H45" s="11" t="s">
         <v>60</v>
       </c>
@@ -2453,40 +2517,44 @@
       <c r="K45" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="L45" s="11"/>
-      <c r="M45" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="53"/>
-      <c r="B46" s="38" t="s">
+      <c r="L45" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="M45" s="11"/>
+      <c r="N45" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="52"/>
+      <c r="B46" s="37" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="D46" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="E46" s="30"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="31" t="s">
+        <v>135</v>
+      </c>
       <c r="F46" s="30"/>
-      <c r="G46" s="9"/>
+      <c r="G46" s="30"/>
       <c r="H46" s="9"/>
-      <c r="I46" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="L46" s="9"/>
-      <c r="M46" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="51" t="s">
+      <c r="I46" s="9"/>
+      <c r="J46" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="M46" s="9"/>
+      <c r="N46" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="50" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="20" t="s">
@@ -2495,168 +2563,175 @@
       <c r="C47" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D47" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="E47" s="28"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="28" t="s">
+        <v>135</v>
+      </c>
       <c r="F47" s="28"/>
-      <c r="G47" s="5"/>
+      <c r="G47" s="28"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
       <c r="K47" s="5"/>
-      <c r="L47" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="M47" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="52"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N47" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="51"/>
       <c r="B48" s="19" t="s">
         <v>45</v>
       </c>
       <c r="C48" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="D48" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E48" s="29"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F48" s="29"/>
-      <c r="G48" s="7"/>
+      <c r="G48" s="29"/>
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
-      <c r="L48" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="M48" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="52"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N48" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="51"/>
       <c r="B49" s="19" t="s">
         <v>46</v>
       </c>
       <c r="C49" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D49" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E49" s="29"/>
+      <c r="D49" s="54"/>
+      <c r="E49" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F49" s="29"/>
-      <c r="G49" s="7"/>
+      <c r="G49" s="29"/>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
-      <c r="L49" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="M49" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="52"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N49" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="51"/>
       <c r="B50" s="19" t="s">
         <v>47</v>
       </c>
       <c r="C50" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="D50" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="E50" s="29"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="29" t="s">
+        <v>135</v>
+      </c>
       <c r="F50" s="29"/>
-      <c r="G50" s="7"/>
+      <c r="G50" s="29"/>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
-      <c r="L50" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="M50" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="52"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="N50" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="51"/>
       <c r="B51" s="24" t="s">
         <v>67</v>
       </c>
       <c r="C51" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D51" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="E51" s="30"/>
+      <c r="D51" s="55"/>
+      <c r="E51" s="30" t="s">
+        <v>135</v>
+      </c>
       <c r="F51" s="30"/>
-      <c r="G51" s="11"/>
+      <c r="G51" s="30"/>
       <c r="H51" s="11"/>
       <c r="I51" s="11"/>
       <c r="J51" s="11"/>
       <c r="K51" s="11"/>
-      <c r="L51" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="M51" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="51" t="s">
+      <c r="L51" s="11"/>
+      <c r="M51" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="N51" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="50" t="s">
         <v>48</v>
       </c>
       <c r="B52" s="20" t="s">
         <v>49</v>
       </c>
       <c r="C52" s="20"/>
-      <c r="D52" s="28"/>
+      <c r="D52" s="20"/>
       <c r="E52" s="28"/>
       <c r="F52" s="28"/>
-      <c r="G52" s="5"/>
+      <c r="G52" s="28"/>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
       <c r="K52" s="5"/>
-      <c r="L52" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="M52" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="53"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N52" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="52"/>
       <c r="B53" s="21" t="s">
         <v>50</v>
       </c>
       <c r="C53" s="21"/>
-      <c r="D53" s="31"/>
+      <c r="D53" s="21"/>
       <c r="E53" s="31"/>
       <c r="F53" s="31"/>
-      <c r="G53" s="9"/>
+      <c r="G53" s="31"/>
       <c r="H53" s="9"/>
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
-      <c r="L53" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="M53" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L53" s="9"/>
+      <c r="M53" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="N53" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>51</v>
       </c>
@@ -2664,200 +2739,209 @@
         <v>52</v>
       </c>
       <c r="C54" s="25"/>
-      <c r="D54" s="32"/>
+      <c r="D54" s="25"/>
       <c r="E54" s="32"/>
       <c r="F54" s="32"/>
-      <c r="G54" s="16"/>
+      <c r="G54" s="32"/>
       <c r="H54" s="16"/>
       <c r="I54" s="16"/>
       <c r="J54" s="16"/>
       <c r="K54" s="16"/>
-      <c r="L54" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="M54" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="51" t="s">
+      <c r="L54" s="16"/>
+      <c r="M54" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="N54" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="50" t="s">
         <v>53</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>54</v>
       </c>
       <c r="C55" s="27"/>
-      <c r="D55" s="28"/>
+      <c r="D55" s="27"/>
       <c r="E55" s="28"/>
       <c r="F55" s="28"/>
-      <c r="G55" s="5"/>
+      <c r="G55" s="28"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
-      <c r="M55" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="52"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="51"/>
       <c r="B56" s="19" t="s">
         <v>55</v>
       </c>
       <c r="C56" s="19"/>
-      <c r="D56" s="33"/>
+      <c r="D56" s="19"/>
       <c r="E56" s="33"/>
       <c r="F56" s="33"/>
-      <c r="G56" s="7"/>
+      <c r="G56" s="33"/>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
       <c r="L56" s="7"/>
-      <c r="M56" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="52"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="51"/>
       <c r="B57" s="24" t="s">
         <v>66</v>
       </c>
       <c r="C57" s="24"/>
-      <c r="D57" s="34"/>
+      <c r="D57" s="24"/>
       <c r="E57" s="34"/>
       <c r="F57" s="34"/>
-      <c r="G57" s="11"/>
+      <c r="G57" s="34"/>
       <c r="H57" s="11"/>
       <c r="I57" s="11"/>
       <c r="J57" s="11"/>
       <c r="K57" s="11"/>
       <c r="L57" s="11"/>
-      <c r="M57" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="53"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="52"/>
       <c r="B58" s="21" t="s">
         <v>56</v>
       </c>
       <c r="C58" s="21"/>
-      <c r="D58" s="31"/>
+      <c r="D58" s="21"/>
       <c r="E58" s="31"/>
       <c r="F58" s="31"/>
-      <c r="G58" s="9"/>
+      <c r="G58" s="31"/>
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
       <c r="L58" s="9"/>
-      <c r="M58" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="47"/>
-      <c r="B59" s="36" t="s">
+      <c r="M58" s="9"/>
+      <c r="N58" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="46"/>
+      <c r="B59" s="35" t="s">
         <v>146</v>
       </c>
       <c r="C59" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="D59" s="50" t="s">
-        <v>135</v>
-      </c>
-      <c r="G59" s="49"/>
-      <c r="H59" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="I59" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="J59" s="49"/>
-      <c r="K59" s="49"/>
-      <c r="L59" s="49"/>
-      <c r="M59" s="49"/>
-    </row>
-    <row r="60" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="47"/>
-      <c r="B60" s="36" t="s">
+      <c r="D59" s="56"/>
+      <c r="E59" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="H59" s="48"/>
+      <c r="I59" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="J59" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="K59" s="48"/>
+      <c r="L59" s="48"/>
+      <c r="M59" s="48"/>
+      <c r="N59" s="48"/>
+    </row>
+    <row r="60" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="46"/>
+      <c r="B60" s="35" t="s">
         <v>148</v>
       </c>
       <c r="C60" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="D60" s="50" t="s">
-        <v>135</v>
-      </c>
-      <c r="G60" s="49"/>
-      <c r="H60" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="I60" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="J60" s="49"/>
-      <c r="K60" s="49"/>
-      <c r="L60" s="49"/>
-      <c r="M60" s="49"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="47"/>
-      <c r="B61" s="36" t="s">
+      <c r="D60" s="56"/>
+      <c r="E60" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="H60" s="48"/>
+      <c r="I60" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="J60" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="K60" s="48"/>
+      <c r="L60" s="48"/>
+      <c r="M60" s="48"/>
+      <c r="N60" s="48"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" s="46"/>
+      <c r="B61" s="35" t="s">
         <v>149</v>
       </c>
       <c r="C61" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="D61" s="50" t="s">
-        <v>135</v>
-      </c>
-      <c r="G61" s="49"/>
-      <c r="H61" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="I61" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="J61" s="49"/>
-      <c r="K61" s="49"/>
-      <c r="L61" s="49"/>
-      <c r="M61" s="49"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="47"/>
-      <c r="B62" s="48"/>
-      <c r="C62" s="48"/>
-      <c r="G62" s="49"/>
-      <c r="H62" s="49"/>
-      <c r="I62" s="49"/>
-      <c r="J62" s="49"/>
-      <c r="K62" s="49"/>
-      <c r="L62" s="49"/>
-      <c r="M62" s="49"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G64" t="s">
+      <c r="D61" s="56"/>
+      <c r="E61" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="H61" s="48"/>
+      <c r="I61" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="J61" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="K61" s="48"/>
+      <c r="L61" s="48"/>
+      <c r="M61" s="48"/>
+      <c r="N61" s="48"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="46"/>
+      <c r="B62" s="47"/>
+      <c r="C62" s="47"/>
+      <c r="D62" s="47"/>
+      <c r="H62" s="48"/>
+      <c r="I62" s="48"/>
+      <c r="J62" s="48"/>
+      <c r="K62" s="48"/>
+      <c r="L62" s="48"/>
+      <c r="M62" s="48"/>
+      <c r="N62" s="48"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H64" t="s">
         <v>69</v>
       </c>
-      <c r="H64" t="s">
+      <c r="I64" t="s">
         <v>70</v>
       </c>
-      <c r="I64" t="s">
+      <c r="J64" t="s">
         <v>68</v>
       </c>
-      <c r="J64" t="s">
+      <c r="K64" t="s">
         <v>74</v>
       </c>
-      <c r="K64" t="s">
+      <c r="L64" t="s">
         <v>71</v>
       </c>
-      <c r="L64" t="s">
+      <c r="M64" t="s">
         <v>73</v>
       </c>
-      <c r="M64" s="18" t="s">
+      <c r="N64" s="18" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2da Entrega (Completa con estos 3 que agrego) - Solicitar Partida Especial - Registrar Adquisición - Crear Asignación
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="152">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -905,6 +905,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -914,10 +918,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1201,8 +1201,8 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,7 +1266,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="54" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="35" t="s">
@@ -1275,16 +1275,16 @@
       <c r="C2" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="53">
+      <c r="D2" s="50">
         <v>43634</v>
       </c>
-      <c r="E2" s="53">
+      <c r="E2" s="50">
         <v>43634</v>
       </c>
-      <c r="F2" s="53">
+      <c r="F2" s="50">
         <v>43634</v>
       </c>
-      <c r="G2" s="53">
+      <c r="G2" s="50">
         <v>43634</v>
       </c>
       <c r="H2" s="5"/>
@@ -1302,14 +1302,14 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="36" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="54"/>
+      <c r="D3" s="51"/>
       <c r="E3" s="29" t="s">
         <v>136</v>
       </c>
@@ -1336,14 +1336,14 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51"/>
+      <c r="A4" s="55"/>
       <c r="B4" s="36" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="54"/>
+      <c r="D4" s="51"/>
       <c r="E4" s="29" t="s">
         <v>135</v>
       </c>
@@ -1364,14 +1364,14 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
+      <c r="A5" s="55"/>
       <c r="B5" s="36" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="54"/>
+      <c r="D5" s="51"/>
       <c r="E5" s="29" t="s">
         <v>135</v>
       </c>
@@ -1390,7 +1390,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="54" t="s">
         <v>57</v>
       </c>
       <c r="B6" s="35" t="s">
@@ -1422,23 +1422,23 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="37" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="53">
+      <c r="D7" s="50">
         <v>43634</v>
       </c>
-      <c r="E7" s="53">
+      <c r="E7" s="50">
         <v>43634</v>
       </c>
-      <c r="F7" s="53">
+      <c r="F7" s="50">
         <v>43634</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="50">
         <v>43634</v>
       </c>
       <c r="H7" s="9"/>
@@ -1454,7 +1454,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="54" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="42" t="s">
@@ -1463,12 +1463,18 @@
       <c r="C8" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+      <c r="D8" s="50">
+        <v>43634</v>
+      </c>
+      <c r="E8" s="50">
+        <v>43634</v>
+      </c>
+      <c r="F8" s="50">
+        <v>43634</v>
+      </c>
+      <c r="G8" s="50">
+        <v>43634</v>
+      </c>
       <c r="H8" s="26" t="s">
         <v>60</v>
       </c>
@@ -1482,14 +1488,14 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="51"/>
+      <c r="A9" s="55"/>
       <c r="B9" s="43" t="s">
         <v>141</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="54"/>
+      <c r="D9" s="51"/>
       <c r="E9" s="29" t="s">
         <v>139</v>
       </c>
@@ -1516,14 +1522,14 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="51"/>
+      <c r="A10" s="55"/>
       <c r="B10" s="43" t="s">
         <v>140</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="54"/>
+      <c r="D10" s="51"/>
       <c r="E10" s="29" t="s">
         <v>136</v>
       </c>
@@ -1542,14 +1548,14 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="51"/>
+      <c r="A11" s="55"/>
       <c r="B11" s="43" t="s">
         <v>142</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="54"/>
+      <c r="D11" s="51"/>
       <c r="E11" s="29" t="s">
         <v>136</v>
       </c>
@@ -1568,14 +1574,14 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="51"/>
+      <c r="A12" s="55"/>
       <c r="B12" s="43" t="s">
         <v>143</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="54"/>
+      <c r="D12" s="51"/>
       <c r="E12" s="29" t="s">
         <v>139</v>
       </c>
@@ -1594,7 +1600,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="54" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="39" t="s">
@@ -1603,15 +1609,17 @@
       <c r="C13" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>136</v>
+      <c r="D13" s="50">
+        <v>43634</v>
+      </c>
+      <c r="E13" s="50">
+        <v>43634</v>
+      </c>
+      <c r="F13" s="50">
+        <v>43634</v>
+      </c>
+      <c r="G13" s="50">
+        <v>43634</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1628,14 +1636,14 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="51"/>
+      <c r="A14" s="55"/>
       <c r="B14" s="40" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="54"/>
+      <c r="D14" s="51"/>
       <c r="E14" s="29" t="s">
         <v>135</v>
       </c>
@@ -1658,14 +1666,14 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="51"/>
+      <c r="A15" s="55"/>
       <c r="B15" s="40" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="54"/>
+      <c r="D15" s="51"/>
       <c r="E15" s="29" t="s">
         <v>135</v>
       </c>
@@ -1686,14 +1694,14 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="51"/>
+      <c r="A16" s="55"/>
       <c r="B16" s="40" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="54"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="29" t="s">
         <v>135</v>
       </c>
@@ -1712,14 +1720,14 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="51"/>
+      <c r="A17" s="55"/>
       <c r="B17" s="40" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="54"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="29" t="s">
         <v>135</v>
       </c>
@@ -1740,14 +1748,14 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="51"/>
+      <c r="A18" s="55"/>
       <c r="B18" s="40" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="54"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="29" t="s">
         <v>135</v>
       </c>
@@ -1768,14 +1776,14 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="52"/>
+      <c r="A19" s="56"/>
       <c r="B19" s="41" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="55"/>
+      <c r="D19" s="52"/>
       <c r="E19" s="30" t="s">
         <v>135</v>
       </c>
@@ -1796,7 +1804,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="54" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="39" t="s">
@@ -1805,12 +1813,18 @@
       <c r="C20" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
+      <c r="D20" s="50">
+        <v>43634</v>
+      </c>
+      <c r="E20" s="50">
+        <v>43634</v>
+      </c>
+      <c r="F20" s="50">
+        <v>43634</v>
+      </c>
+      <c r="G20" s="50">
+        <v>43634</v>
+      </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -1826,14 +1840,14 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="51"/>
+      <c r="A21" s="55"/>
       <c r="B21" s="40" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="54"/>
+      <c r="D21" s="51"/>
       <c r="E21" s="29" t="s">
         <v>135</v>
       </c>
@@ -1854,14 +1868,14 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="51"/>
+      <c r="A22" s="55"/>
       <c r="B22" s="40" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="54"/>
+      <c r="D22" s="51"/>
       <c r="E22" s="29" t="s">
         <v>135</v>
       </c>
@@ -1882,14 +1896,14 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="52"/>
+      <c r="A23" s="56"/>
       <c r="B23" s="41" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="55"/>
+      <c r="D23" s="52"/>
       <c r="E23" s="30" t="s">
         <v>135</v>
       </c>
@@ -1908,7 +1922,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="54" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="42" t="s">
@@ -1936,14 +1950,14 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="51"/>
+      <c r="A25" s="55"/>
       <c r="B25" s="43" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="54"/>
+      <c r="D25" s="51"/>
       <c r="E25" s="29" t="s">
         <v>136</v>
       </c>
@@ -1962,14 +1976,14 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="51"/>
+      <c r="A26" s="55"/>
       <c r="B26" s="43" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="54"/>
+      <c r="D26" s="51"/>
       <c r="E26" s="29" t="s">
         <v>144</v>
       </c>
@@ -1988,14 +2002,14 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="52"/>
+      <c r="A27" s="56"/>
       <c r="B27" s="44" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="55"/>
+      <c r="D27" s="52"/>
       <c r="E27" s="30" t="s">
         <v>145</v>
       </c>
@@ -2014,7 +2028,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="54" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="35" t="s">
@@ -2050,14 +2064,14 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="51"/>
+      <c r="A29" s="55"/>
       <c r="B29" s="36" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="D29" s="54"/>
+      <c r="D29" s="51"/>
       <c r="E29" s="29" t="s">
         <v>135</v>
       </c>
@@ -2076,14 +2090,14 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="51"/>
+      <c r="A30" s="55"/>
       <c r="B30" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="D30" s="54"/>
+      <c r="D30" s="51"/>
       <c r="E30" s="29" t="s">
         <v>135</v>
       </c>
@@ -2102,14 +2116,14 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="51"/>
+      <c r="A31" s="55"/>
       <c r="B31" s="36" t="s">
         <v>27</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="54"/>
+      <c r="D31" s="51"/>
       <c r="E31" s="29" t="s">
         <v>135</v>
       </c>
@@ -2128,14 +2142,14 @@
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="52"/>
+      <c r="A32" s="56"/>
       <c r="B32" s="37" t="s">
         <v>37</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="D32" s="55"/>
+      <c r="D32" s="52"/>
       <c r="E32" s="30" t="s">
         <v>135</v>
       </c>
@@ -2154,7 +2168,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="50" t="s">
+      <c r="A33" s="54" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="35" t="s">
@@ -2182,14 +2196,14 @@
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="51"/>
+      <c r="A34" s="55"/>
       <c r="B34" s="36" t="s">
         <v>30</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="D34" s="54"/>
+      <c r="D34" s="51"/>
       <c r="E34" s="29" t="s">
         <v>135</v>
       </c>
@@ -2216,14 +2230,14 @@
       </c>
     </row>
     <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="51"/>
+      <c r="A35" s="55"/>
       <c r="B35" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C35" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="D35" s="55"/>
+      <c r="D35" s="52"/>
       <c r="E35" s="30" t="s">
         <v>135</v>
       </c>
@@ -2242,14 +2256,14 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="52"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="37" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="D36" s="55"/>
+      <c r="D36" s="52"/>
       <c r="E36" s="31" t="s">
         <v>135</v>
       </c>
@@ -2268,7 +2282,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="50" t="s">
+      <c r="A37" s="54" t="s">
         <v>32</v>
       </c>
       <c r="B37" s="35" t="s">
@@ -2296,14 +2310,14 @@
       </c>
     </row>
     <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="51"/>
+      <c r="A38" s="55"/>
       <c r="B38" s="36" t="s">
         <v>34</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="D38" s="54"/>
+      <c r="D38" s="51"/>
       <c r="E38" s="29" t="s">
         <v>135</v>
       </c>
@@ -2322,14 +2336,14 @@
       </c>
     </row>
     <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="51"/>
+      <c r="A39" s="55"/>
       <c r="B39" s="36" t="s">
         <v>35</v>
       </c>
       <c r="C39" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="D39" s="54"/>
+      <c r="D39" s="51"/>
       <c r="E39" s="29" t="s">
         <v>135</v>
       </c>
@@ -2348,14 +2362,14 @@
       </c>
     </row>
     <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="51"/>
+      <c r="A40" s="55"/>
       <c r="B40" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C40" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="55"/>
+      <c r="D40" s="52"/>
       <c r="E40" s="30" t="s">
         <v>135</v>
       </c>
@@ -2380,14 +2394,14 @@
       </c>
     </row>
     <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="52"/>
+      <c r="A41" s="56"/>
       <c r="B41" s="37" t="s">
         <v>36</v>
       </c>
       <c r="C41" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="55"/>
+      <c r="D41" s="52"/>
       <c r="E41" s="31" t="s">
         <v>135</v>
       </c>
@@ -2406,7 +2420,7 @@
       </c>
     </row>
     <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="54" t="s">
         <v>38</v>
       </c>
       <c r="B42" s="35" t="s">
@@ -2436,14 +2450,14 @@
       </c>
     </row>
     <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="51"/>
+      <c r="A43" s="55"/>
       <c r="B43" s="36" t="s">
         <v>40</v>
       </c>
       <c r="C43" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D43" s="54"/>
+      <c r="D43" s="51"/>
       <c r="E43" s="29" t="s">
         <v>135</v>
       </c>
@@ -2464,14 +2478,14 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="51"/>
+      <c r="A44" s="55"/>
       <c r="B44" s="36" t="s">
         <v>41</v>
       </c>
       <c r="C44" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="D44" s="54"/>
+      <c r="D44" s="51"/>
       <c r="E44" s="29" t="s">
         <v>135</v>
       </c>
@@ -2492,14 +2506,14 @@
       </c>
     </row>
     <row r="45" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="51"/>
+      <c r="A45" s="55"/>
       <c r="B45" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C45" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D45" s="55"/>
+      <c r="D45" s="52"/>
       <c r="E45" s="30" t="s">
         <v>135</v>
       </c>
@@ -2526,14 +2540,14 @@
       </c>
     </row>
     <row r="46" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="52"/>
+      <c r="A46" s="56"/>
       <c r="B46" s="37" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="D46" s="55"/>
+      <c r="D46" s="52"/>
       <c r="E46" s="31" t="s">
         <v>135</v>
       </c>
@@ -2554,7 +2568,7 @@
       </c>
     </row>
     <row r="47" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="50" t="s">
+      <c r="A47" s="54" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="20" t="s">
@@ -2582,14 +2596,14 @@
       </c>
     </row>
     <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="51"/>
+      <c r="A48" s="55"/>
       <c r="B48" s="19" t="s">
         <v>45</v>
       </c>
       <c r="C48" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="D48" s="54"/>
+      <c r="D48" s="51"/>
       <c r="E48" s="29" t="s">
         <v>135</v>
       </c>
@@ -2608,14 +2622,14 @@
       </c>
     </row>
     <row r="49" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="51"/>
+      <c r="A49" s="55"/>
       <c r="B49" s="19" t="s">
         <v>46</v>
       </c>
       <c r="C49" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D49" s="54"/>
+      <c r="D49" s="51"/>
       <c r="E49" s="29" t="s">
         <v>135</v>
       </c>
@@ -2634,14 +2648,14 @@
       </c>
     </row>
     <row r="50" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="51"/>
+      <c r="A50" s="55"/>
       <c r="B50" s="19" t="s">
         <v>47</v>
       </c>
       <c r="C50" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="D50" s="54"/>
+      <c r="D50" s="51"/>
       <c r="E50" s="29" t="s">
         <v>135</v>
       </c>
@@ -2660,14 +2674,14 @@
       </c>
     </row>
     <row r="51" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="51"/>
+      <c r="A51" s="55"/>
       <c r="B51" s="24" t="s">
         <v>67</v>
       </c>
       <c r="C51" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D51" s="55"/>
+      <c r="D51" s="52"/>
       <c r="E51" s="30" t="s">
         <v>135</v>
       </c>
@@ -2686,7 +2700,7 @@
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="50" t="s">
+      <c r="A52" s="54" t="s">
         <v>48</v>
       </c>
       <c r="B52" s="20" t="s">
@@ -2710,7 +2724,7 @@
       </c>
     </row>
     <row r="53" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="52"/>
+      <c r="A53" s="56"/>
       <c r="B53" s="21" t="s">
         <v>50</v>
       </c>
@@ -2756,7 +2770,7 @@
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="50" t="s">
+      <c r="A55" s="54" t="s">
         <v>53</v>
       </c>
       <c r="B55" s="20" t="s">
@@ -2778,7 +2792,7 @@
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="51"/>
+      <c r="A56" s="55"/>
       <c r="B56" s="19" t="s">
         <v>55</v>
       </c>
@@ -2798,7 +2812,7 @@
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="51"/>
+      <c r="A57" s="55"/>
       <c r="B57" s="24" t="s">
         <v>66</v>
       </c>
@@ -2818,7 +2832,7 @@
       </c>
     </row>
     <row r="58" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="52"/>
+      <c r="A58" s="56"/>
       <c r="B58" s="21" t="s">
         <v>56</v>
       </c>
@@ -2845,7 +2859,7 @@
       <c r="C59" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="D59" s="56"/>
+      <c r="D59" s="53"/>
       <c r="E59" s="49" t="s">
         <v>135</v>
       </c>
@@ -2869,7 +2883,7 @@
       <c r="C60" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="D60" s="56"/>
+      <c r="D60" s="53"/>
       <c r="E60" s="49" t="s">
         <v>135</v>
       </c>
@@ -2893,7 +2907,7 @@
       <c r="C61" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="D61" s="56"/>
+      <c r="D61" s="53"/>
       <c r="E61" s="49" t="s">
         <v>135</v>
       </c>
@@ -2947,6 +2961,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A33:A36"/>
@@ -2954,12 +2974,6 @@
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#CU y Der BuscarPartida Revisado OK #Se quito totalmente todo lo de "Caja"
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="152">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -1201,8 +1201,8 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1495,11 +1495,15 @@
       <c r="C9" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="F9" s="29"/>
+      <c r="D9" s="50">
+        <v>43644</v>
+      </c>
+      <c r="E9" s="50">
+        <v>43644</v>
+      </c>
+      <c r="F9" s="50">
+        <v>43644</v>
+      </c>
       <c r="G9" s="29"/>
       <c r="H9" s="7" t="s">
         <v>60</v>
@@ -2961,12 +2965,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A33:A36"/>
@@ -2974,6 +2972,12 @@
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#Buscar Solicitud	SC002 Todos los diag OK #Modificar Solicitud	SC003 Todos los Diag OK #Agregar Detalle de Solicitud	SC026 Todos los diag OK
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="152">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -1201,8 +1201,8 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,12 +1309,18 @@
       <c r="C3" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
+      <c r="D3" s="50">
+        <v>43647</v>
+      </c>
+      <c r="E3" s="50">
+        <v>43647</v>
+      </c>
+      <c r="F3" s="50">
+        <v>43647</v>
+      </c>
+      <c r="G3" s="50">
+        <v>43647</v>
+      </c>
       <c r="H3" s="7" t="s">
         <v>60</v>
       </c>
@@ -1343,12 +1349,18 @@
       <c r="C4" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="51"/>
-      <c r="E4" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+      <c r="D4" s="50">
+        <v>43647</v>
+      </c>
+      <c r="E4" s="50">
+        <v>43647</v>
+      </c>
+      <c r="F4" s="50">
+        <v>43647</v>
+      </c>
+      <c r="G4" s="50">
+        <v>43647</v>
+      </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
         <v>60</v>
@@ -2863,9 +2875,17 @@
       <c r="C59" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="D59" s="53"/>
-      <c r="E59" s="49" t="s">
-        <v>135</v>
+      <c r="D59" s="50">
+        <v>43647</v>
+      </c>
+      <c r="E59" s="50">
+        <v>43647</v>
+      </c>
+      <c r="F59" s="50">
+        <v>43647</v>
+      </c>
+      <c r="G59" s="50">
+        <v>43647</v>
       </c>
       <c r="H59" s="48"/>
       <c r="I59" s="48" t="s">
@@ -2965,6 +2985,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A33:A36"/>
@@ -2972,12 +2998,6 @@
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#Arreglo de ignore, hice un reset a un commit anterior
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -1201,8 +1201,8 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2985,12 +2985,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A33:A36"/>
@@ -2998,6 +2992,12 @@
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#Fix Orientación a Objetos SolicDetalle #La mayoría de los casos de uso revisados y DER y Diag Clases en carpeta (faltan los AA000) #Der revisado #Diagrama de clases revisado y mejorado
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="148">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -434,18 +434,12 @@
     <t>OK</t>
   </si>
   <si>
-    <t>CARPETA</t>
-  </si>
-  <si>
     <t>Registrar Adquisicion</t>
   </si>
   <si>
     <t>Solicitar Partida Especial</t>
   </si>
   <si>
-    <t>ALT CARPETA</t>
-  </si>
-  <si>
     <t>Modificar Partida Especial</t>
   </si>
   <si>
@@ -456,12 +450,6 @@
   </si>
   <si>
     <t>Asociar Partida Especial</t>
-  </si>
-  <si>
-    <t>Recopiar Sec</t>
-  </si>
-  <si>
-    <t>Recopiar Todo</t>
   </si>
   <si>
     <t>Agregar Detalle de Solicitud</t>
@@ -814,7 +802,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -904,11 +892,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1200,9 +1186,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,7 +1252,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="52" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="35" t="s">
@@ -1275,17 +1261,17 @@
       <c r="C2" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="50">
-        <v>43634</v>
-      </c>
-      <c r="E2" s="50">
-        <v>43634</v>
-      </c>
-      <c r="F2" s="50">
-        <v>43634</v>
-      </c>
-      <c r="G2" s="50">
-        <v>43634</v>
+      <c r="D2" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E2" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F2" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G2" s="49">
+        <v>43685</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5" t="s">
@@ -1302,24 +1288,24 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55"/>
+      <c r="A3" s="53"/>
       <c r="B3" s="36" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="50">
-        <v>43647</v>
-      </c>
-      <c r="E3" s="50">
-        <v>43647</v>
-      </c>
-      <c r="F3" s="50">
-        <v>43647</v>
-      </c>
-      <c r="G3" s="50">
-        <v>43647</v>
+      <c r="D3" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E3" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F3" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G3" s="49">
+        <v>43685</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>60</v>
@@ -1342,24 +1328,24 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55"/>
+      <c r="A4" s="53"/>
       <c r="B4" s="36" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="50">
-        <v>43647</v>
-      </c>
-      <c r="E4" s="50">
-        <v>43647</v>
-      </c>
-      <c r="F4" s="50">
-        <v>43647</v>
-      </c>
-      <c r="G4" s="50">
-        <v>43647</v>
+      <c r="D4" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E4" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F4" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G4" s="49">
+        <v>43685</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7" t="s">
@@ -1376,19 +1362,25 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="55"/>
+      <c r="A5" s="53"/>
       <c r="B5" s="36" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
+      <c r="D5" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E5" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F5" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G5" s="49">
+        <v>43685</v>
+      </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7" t="s">
@@ -1402,7 +1394,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="52" t="s">
         <v>57</v>
       </c>
       <c r="B6" s="35" t="s">
@@ -1411,15 +1403,17 @@
       <c r="C6" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>135</v>
+      <c r="D6" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E6" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F6" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G6" s="49">
+        <v>43685</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="14"/>
@@ -1434,24 +1428,24 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="56"/>
+      <c r="A7" s="54"/>
       <c r="B7" s="37" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="50">
-        <v>43634</v>
-      </c>
-      <c r="E7" s="50">
-        <v>43634</v>
-      </c>
-      <c r="F7" s="50">
-        <v>43634</v>
-      </c>
-      <c r="G7" s="50">
-        <v>43634</v>
+      <c r="D7" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E7" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F7" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G7" s="49">
+        <v>43685</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="13"/>
@@ -1466,26 +1460,26 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="52" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="50">
-        <v>43634</v>
-      </c>
-      <c r="E8" s="50">
-        <v>43634</v>
-      </c>
-      <c r="F8" s="50">
-        <v>43634</v>
-      </c>
-      <c r="G8" s="50">
-        <v>43634</v>
+      <c r="D8" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E8" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F8" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G8" s="49">
+        <v>43685</v>
       </c>
       <c r="H8" s="26" t="s">
         <v>60</v>
@@ -1500,23 +1494,25 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="55"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="43" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="50">
-        <v>43644</v>
-      </c>
-      <c r="E9" s="50">
-        <v>43644</v>
-      </c>
-      <c r="F9" s="50">
-        <v>43644</v>
-      </c>
-      <c r="G9" s="29"/>
+      <c r="D9" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E9" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F9" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G9" s="49">
+        <v>43685</v>
+      </c>
       <c r="H9" s="7" t="s">
         <v>60</v>
       </c>
@@ -1538,19 +1534,25 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="55"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="43" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="51"/>
-      <c r="E10" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
+      <c r="D10" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E10" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F10" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G10" s="49">
+        <v>43685</v>
+      </c>
       <c r="H10" s="26" t="s">
         <v>60</v>
       </c>
@@ -1564,19 +1566,25 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="55"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="43" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="51"/>
-      <c r="E11" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E11" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F11" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G11" s="49">
+        <v>43685</v>
+      </c>
       <c r="H11" s="7" t="s">
         <v>60</v>
       </c>
@@ -1590,19 +1598,25 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="55"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="43" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="51"/>
-      <c r="E12" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
+      <c r="D12" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E12" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F12" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G12" s="49">
+        <v>43685</v>
+      </c>
       <c r="H12" s="7" t="s">
         <v>60</v>
       </c>
@@ -1616,25 +1630,25 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="52" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="50">
+      <c r="D13" s="49">
         <v>43634</v>
       </c>
-      <c r="E13" s="50">
+      <c r="E13" s="49">
         <v>43634</v>
       </c>
-      <c r="F13" s="50">
+      <c r="F13" s="49">
         <v>43634</v>
       </c>
-      <c r="G13" s="50">
+      <c r="G13" s="49">
         <v>43634</v>
       </c>
       <c r="H13" s="5"/>
@@ -1652,14 +1666,14 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="55"/>
+      <c r="A14" s="53"/>
       <c r="B14" s="40" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="51"/>
+      <c r="D14" s="50"/>
       <c r="E14" s="29" t="s">
         <v>135</v>
       </c>
@@ -1682,14 +1696,14 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="55"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="40" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="51"/>
+      <c r="D15" s="50"/>
       <c r="E15" s="29" t="s">
         <v>135</v>
       </c>
@@ -1710,14 +1724,14 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="55"/>
+      <c r="A16" s="53"/>
       <c r="B16" s="40" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="51"/>
+      <c r="D16" s="50"/>
       <c r="E16" s="29" t="s">
         <v>135</v>
       </c>
@@ -1736,14 +1750,14 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="55"/>
+      <c r="A17" s="53"/>
       <c r="B17" s="40" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="51"/>
+      <c r="D17" s="50"/>
       <c r="E17" s="29" t="s">
         <v>135</v>
       </c>
@@ -1764,14 +1778,14 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="55"/>
+      <c r="A18" s="53"/>
       <c r="B18" s="40" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="51"/>
+      <c r="D18" s="50"/>
       <c r="E18" s="29" t="s">
         <v>135</v>
       </c>
@@ -1792,14 +1806,14 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="56"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="41" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="52"/>
+      <c r="D19" s="51"/>
       <c r="E19" s="30" t="s">
         <v>135</v>
       </c>
@@ -1820,7 +1834,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="52" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="39" t="s">
@@ -1829,16 +1843,16 @@
       <c r="C20" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="D20" s="50">
+      <c r="D20" s="49">
         <v>43634</v>
       </c>
-      <c r="E20" s="50">
+      <c r="E20" s="49">
         <v>43634</v>
       </c>
-      <c r="F20" s="50">
+      <c r="F20" s="49">
         <v>43634</v>
       </c>
-      <c r="G20" s="50">
+      <c r="G20" s="49">
         <v>43634</v>
       </c>
       <c r="H20" s="5"/>
@@ -1856,14 +1870,14 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="55"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="40" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="51"/>
+      <c r="D21" s="50"/>
       <c r="E21" s="29" t="s">
         <v>135</v>
       </c>
@@ -1884,14 +1898,14 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="55"/>
+      <c r="A22" s="53"/>
       <c r="B22" s="40" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="51"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="29" t="s">
         <v>135</v>
       </c>
@@ -1912,14 +1926,14 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="56"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="41" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="52"/>
+      <c r="D23" s="51"/>
       <c r="E23" s="30" t="s">
         <v>135</v>
       </c>
@@ -1938,7 +1952,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="52" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="42" t="s">
@@ -1947,12 +1961,18 @@
       <c r="C24" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
+      <c r="D24" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E24" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F24" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G24" s="49">
+        <v>43685</v>
+      </c>
       <c r="H24" s="5" t="s">
         <v>60</v>
       </c>
@@ -1966,19 +1986,25 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="55"/>
+      <c r="A25" s="53"/>
       <c r="B25" s="43" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="51"/>
-      <c r="E25" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
+      <c r="D25" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E25" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F25" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G25" s="49">
+        <v>43685</v>
+      </c>
       <c r="H25" s="7" t="s">
         <v>60</v>
       </c>
@@ -1992,19 +2018,25 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="55"/>
+      <c r="A26" s="53"/>
       <c r="B26" s="43" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="51"/>
-      <c r="E26" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
+      <c r="D26" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E26" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F26" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G26" s="49">
+        <v>43685</v>
+      </c>
       <c r="H26" s="7" t="s">
         <v>60</v>
       </c>
@@ -2018,19 +2050,25 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="56"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="44" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="52"/>
-      <c r="E27" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
+      <c r="D27" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E27" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F27" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G27" s="49">
+        <v>43685</v>
+      </c>
       <c r="H27" s="9" t="s">
         <v>60</v>
       </c>
@@ -2044,7 +2082,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="52" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="35" t="s">
@@ -2053,12 +2091,18 @@
       <c r="C28" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
+      <c r="D28" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E28" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F28" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G28" s="49">
+        <v>43685</v>
+      </c>
       <c r="H28" s="5" t="s">
         <v>60</v>
       </c>
@@ -2080,19 +2124,25 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="55"/>
+      <c r="A29" s="53"/>
       <c r="B29" s="36" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="D29" s="51"/>
-      <c r="E29" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
+      <c r="D29" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E29" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F29" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G29" s="49">
+        <v>43685</v>
+      </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7" t="s">
         <v>60</v>
@@ -2106,19 +2156,25 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="55"/>
+      <c r="A30" s="53"/>
       <c r="B30" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="D30" s="51"/>
-      <c r="E30" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
+      <c r="D30" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E30" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F30" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G30" s="49">
+        <v>43685</v>
+      </c>
       <c r="H30" s="7"/>
       <c r="I30" s="7" t="s">
         <v>60</v>
@@ -2132,19 +2188,25 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="55"/>
+      <c r="A31" s="53"/>
       <c r="B31" s="36" t="s">
         <v>27</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="51"/>
-      <c r="E31" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
+      <c r="D31" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E31" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F31" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G31" s="49">
+        <v>43685</v>
+      </c>
       <c r="H31" s="7"/>
       <c r="I31" s="7" t="s">
         <v>60</v>
@@ -2158,19 +2220,25 @@
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="56"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="37" t="s">
         <v>37</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="D32" s="52"/>
-      <c r="E32" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
+      <c r="D32" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E32" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F32" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G32" s="49">
+        <v>43685</v>
+      </c>
       <c r="H32" s="9"/>
       <c r="I32" s="9" t="s">
         <v>60</v>
@@ -2184,7 +2252,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="54" t="s">
+      <c r="A33" s="52" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="35" t="s">
@@ -2193,12 +2261,18 @@
       <c r="C33" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="D33" s="27"/>
-      <c r="E33" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
+      <c r="D33" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E33" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F33" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G33" s="49">
+        <v>43685</v>
+      </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5" t="s">
@@ -2212,19 +2286,25 @@
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="55"/>
+      <c r="A34" s="53"/>
       <c r="B34" s="36" t="s">
         <v>30</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="D34" s="51"/>
-      <c r="E34" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
+      <c r="D34" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E34" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F34" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G34" s="49">
+        <v>43685</v>
+      </c>
       <c r="H34" s="7" t="s">
         <v>60</v>
       </c>
@@ -2246,19 +2326,25 @@
       </c>
     </row>
     <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="55"/>
+      <c r="A35" s="53"/>
       <c r="B35" s="1" t="s">
         <v>75</v>
       </c>
       <c r="C35" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="D35" s="52"/>
-      <c r="E35" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
+      <c r="D35" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E35" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F35" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G35" s="49">
+        <v>43685</v>
+      </c>
       <c r="H35" s="22"/>
       <c r="I35" s="22"/>
       <c r="J35" s="22" t="s">
@@ -2272,19 +2358,25 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="56"/>
+      <c r="A36" s="54"/>
       <c r="B36" s="37" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="D36" s="52"/>
-      <c r="E36" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
+      <c r="D36" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E36" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F36" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G36" s="49">
+        <v>43685</v>
+      </c>
       <c r="H36" s="9"/>
       <c r="I36" s="9"/>
       <c r="J36" s="9" t="s">
@@ -2298,7 +2390,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="54" t="s">
+      <c r="A37" s="52" t="s">
         <v>32</v>
       </c>
       <c r="B37" s="35" t="s">
@@ -2307,12 +2399,18 @@
       <c r="C37" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="27"/>
-      <c r="E37" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
+      <c r="D37" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E37" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F37" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G37" s="49">
+        <v>43685</v>
+      </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5" t="s">
@@ -2326,19 +2424,25 @@
       </c>
     </row>
     <row r="38" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="55"/>
+      <c r="A38" s="53"/>
       <c r="B38" s="36" t="s">
         <v>34</v>
       </c>
       <c r="C38" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="D38" s="51"/>
-      <c r="E38" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
+      <c r="D38" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E38" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F38" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G38" s="49">
+        <v>43685</v>
+      </c>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7" t="s">
@@ -2352,19 +2456,25 @@
       </c>
     </row>
     <row r="39" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="55"/>
+      <c r="A39" s="53"/>
       <c r="B39" s="36" t="s">
         <v>35</v>
       </c>
       <c r="C39" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="D39" s="51"/>
-      <c r="E39" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
+      <c r="D39" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E39" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F39" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G39" s="49">
+        <v>43685</v>
+      </c>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
       <c r="J39" s="7" t="s">
@@ -2378,19 +2488,25 @@
       </c>
     </row>
     <row r="40" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="55"/>
+      <c r="A40" s="53"/>
       <c r="B40" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C40" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="52"/>
-      <c r="E40" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
+      <c r="D40" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E40" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F40" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G40" s="49">
+        <v>43685</v>
+      </c>
       <c r="H40" s="11"/>
       <c r="I40" s="11" t="s">
         <v>60</v>
@@ -2410,19 +2526,25 @@
       </c>
     </row>
     <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="56"/>
+      <c r="A41" s="54"/>
       <c r="B41" s="37" t="s">
         <v>36</v>
       </c>
       <c r="C41" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="52"/>
-      <c r="E41" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
+      <c r="D41" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E41" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F41" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G41" s="49">
+        <v>43685</v>
+      </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
       <c r="J41" s="9" t="s">
@@ -2436,7 +2558,7 @@
       </c>
     </row>
     <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="54" t="s">
+      <c r="A42" s="52" t="s">
         <v>38</v>
       </c>
       <c r="B42" s="35" t="s">
@@ -2445,12 +2567,18 @@
       <c r="C42" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
+      <c r="D42" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E42" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F42" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G42" s="49">
+        <v>43685</v>
+      </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5" t="s">
@@ -2466,19 +2594,25 @@
       </c>
     </row>
     <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="55"/>
+      <c r="A43" s="53"/>
       <c r="B43" s="36" t="s">
         <v>40</v>
       </c>
       <c r="C43" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D43" s="51"/>
-      <c r="E43" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
+      <c r="D43" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E43" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F43" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G43" s="49">
+        <v>43685</v>
+      </c>
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
       <c r="J43" s="7" t="s">
@@ -2494,19 +2628,25 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="55"/>
+      <c r="A44" s="53"/>
       <c r="B44" s="36" t="s">
         <v>41</v>
       </c>
       <c r="C44" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="D44" s="51"/>
-      <c r="E44" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
+      <c r="D44" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E44" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F44" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G44" s="49">
+        <v>43685</v>
+      </c>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
       <c r="J44" s="7" t="s">
@@ -2522,19 +2662,25 @@
       </c>
     </row>
     <row r="45" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="55"/>
+      <c r="A45" s="53"/>
       <c r="B45" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C45" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="D45" s="52"/>
-      <c r="E45" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="F45" s="30"/>
-      <c r="G45" s="30"/>
+      <c r="D45" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E45" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F45" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G45" s="49">
+        <v>43685</v>
+      </c>
       <c r="H45" s="11" t="s">
         <v>60</v>
       </c>
@@ -2556,19 +2702,25 @@
       </c>
     </row>
     <row r="46" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="56"/>
+      <c r="A46" s="54"/>
       <c r="B46" s="37" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="D46" s="52"/>
-      <c r="E46" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="F46" s="30"/>
-      <c r="G46" s="30"/>
+      <c r="D46" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E46" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F46" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G46" s="49">
+        <v>43685</v>
+      </c>
       <c r="H46" s="9"/>
       <c r="I46" s="9"/>
       <c r="J46" s="9" t="s">
@@ -2584,7 +2736,7 @@
       </c>
     </row>
     <row r="47" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="54" t="s">
+      <c r="A47" s="52" t="s">
         <v>43</v>
       </c>
       <c r="B47" s="20" t="s">
@@ -2612,14 +2764,14 @@
       </c>
     </row>
     <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="55"/>
+      <c r="A48" s="53"/>
       <c r="B48" s="19" t="s">
         <v>45</v>
       </c>
       <c r="C48" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="D48" s="51"/>
+      <c r="D48" s="50"/>
       <c r="E48" s="29" t="s">
         <v>135</v>
       </c>
@@ -2638,14 +2790,14 @@
       </c>
     </row>
     <row r="49" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="55"/>
+      <c r="A49" s="53"/>
       <c r="B49" s="19" t="s">
         <v>46</v>
       </c>
       <c r="C49" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="D49" s="51"/>
+      <c r="D49" s="50"/>
       <c r="E49" s="29" t="s">
         <v>135</v>
       </c>
@@ -2664,14 +2816,14 @@
       </c>
     </row>
     <row r="50" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="55"/>
+      <c r="A50" s="53"/>
       <c r="B50" s="19" t="s">
         <v>47</v>
       </c>
       <c r="C50" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="D50" s="51"/>
+      <c r="D50" s="50"/>
       <c r="E50" s="29" t="s">
         <v>135</v>
       </c>
@@ -2690,14 +2842,14 @@
       </c>
     </row>
     <row r="51" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="55"/>
+      <c r="A51" s="53"/>
       <c r="B51" s="24" t="s">
         <v>67</v>
       </c>
       <c r="C51" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D51" s="52"/>
+      <c r="D51" s="51"/>
       <c r="E51" s="30" t="s">
         <v>135</v>
       </c>
@@ -2716,7 +2868,7 @@
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="54" t="s">
+      <c r="A52" s="52" t="s">
         <v>48</v>
       </c>
       <c r="B52" s="20" t="s">
@@ -2740,7 +2892,7 @@
       </c>
     </row>
     <row r="53" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="56"/>
+      <c r="A53" s="54"/>
       <c r="B53" s="21" t="s">
         <v>50</v>
       </c>
@@ -2786,7 +2938,7 @@
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="54" t="s">
+      <c r="A55" s="52" t="s">
         <v>53</v>
       </c>
       <c r="B55" s="20" t="s">
@@ -2808,7 +2960,7 @@
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="55"/>
+      <c r="A56" s="53"/>
       <c r="B56" s="19" t="s">
         <v>55</v>
       </c>
@@ -2828,7 +2980,7 @@
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="55"/>
+      <c r="A57" s="53"/>
       <c r="B57" s="24" t="s">
         <v>66</v>
       </c>
@@ -2848,7 +3000,7 @@
       </c>
     </row>
     <row r="58" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="56"/>
+      <c r="A58" s="54"/>
       <c r="B58" s="21" t="s">
         <v>56</v>
       </c>
@@ -2870,22 +3022,22 @@
     <row r="59" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="46"/>
       <c r="B59" s="35" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C59" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="D59" s="50">
-        <v>43647</v>
-      </c>
-      <c r="E59" s="50">
-        <v>43647</v>
-      </c>
-      <c r="F59" s="50">
-        <v>43647</v>
-      </c>
-      <c r="G59" s="50">
-        <v>43647</v>
+        <v>143</v>
+      </c>
+      <c r="D59" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E59" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F59" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G59" s="49">
+        <v>43685</v>
       </c>
       <c r="H59" s="48"/>
       <c r="I59" s="48" t="s">
@@ -2902,14 +3054,22 @@
     <row r="60" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="46"/>
       <c r="B60" s="35" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C60" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="D60" s="53"/>
-      <c r="E60" s="49" t="s">
-        <v>135</v>
+        <v>146</v>
+      </c>
+      <c r="D60" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E60" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F60" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G60" s="49">
+        <v>43685</v>
       </c>
       <c r="H60" s="48"/>
       <c r="I60" s="48" t="s">
@@ -2926,14 +3086,22 @@
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="46"/>
       <c r="B61" s="35" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C61" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="D61" s="53"/>
-      <c r="E61" s="49" t="s">
-        <v>135</v>
+        <v>147</v>
+      </c>
+      <c r="D61" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E61" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F61" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G61" s="49">
+        <v>43685</v>
       </c>
       <c r="H61" s="48"/>
       <c r="I61" s="48" t="s">
@@ -2985,6 +3153,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A33:A36"/>
@@ -2992,12 +3166,6 @@
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#Ders y Diagramas Clases revisados terminado
</commit_message>
<xml_diff>
--- a/Anotaciones/Patentes y Familias Definidas.xlsx
+++ b/Anotaciones/Patentes y Familias Definidas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="148">
   <si>
     <t>Crear Solicitud</t>
   </si>
@@ -1187,8 +1187,8 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27:G27"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,16 +1640,16 @@
         <v>96</v>
       </c>
       <c r="D13" s="49">
-        <v>43634</v>
+        <v>43685</v>
       </c>
       <c r="E13" s="49">
-        <v>43634</v>
+        <v>43685</v>
       </c>
       <c r="F13" s="49">
-        <v>43634</v>
+        <v>43685</v>
       </c>
       <c r="G13" s="49">
-        <v>43634</v>
+        <v>43685</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1673,12 +1673,18 @@
       <c r="C14" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
+      <c r="D14" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E14" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F14" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G14" s="49">
+        <v>43685</v>
+      </c>
       <c r="H14" s="7" t="s">
         <v>60</v>
       </c>
@@ -1703,12 +1709,18 @@
       <c r="C15" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
+      <c r="D15" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E15" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F15" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G15" s="49">
+        <v>43685</v>
+      </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
@@ -1731,12 +1743,18 @@
       <c r="C16" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
+      <c r="D16" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E16" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F16" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G16" s="49">
+        <v>43685</v>
+      </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
@@ -1757,12 +1775,18 @@
       <c r="C17" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="50"/>
-      <c r="E17" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
+      <c r="D17" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E17" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F17" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G17" s="49">
+        <v>43685</v>
+      </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -1785,12 +1809,18 @@
       <c r="C18" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
+      <c r="D18" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E18" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F18" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G18" s="49">
+        <v>43685</v>
+      </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
@@ -1813,12 +1843,18 @@
       <c r="C19" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
+      <c r="D19" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E19" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F19" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G19" s="49">
+        <v>43685</v>
+      </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
@@ -1844,16 +1880,16 @@
         <v>103</v>
       </c>
       <c r="D20" s="49">
-        <v>43634</v>
+        <v>43685</v>
       </c>
       <c r="E20" s="49">
-        <v>43634</v>
+        <v>43685</v>
       </c>
       <c r="F20" s="49">
-        <v>43634</v>
+        <v>43685</v>
       </c>
       <c r="G20" s="49">
-        <v>43634</v>
+        <v>43685</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1877,12 +1913,18 @@
       <c r="C21" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
+      <c r="D21" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E21" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F21" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G21" s="49">
+        <v>43685</v>
+      </c>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
@@ -1905,12 +1947,18 @@
       <c r="C22" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="50"/>
-      <c r="E22" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
+      <c r="D22" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E22" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F22" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G22" s="49">
+        <v>43685</v>
+      </c>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
@@ -1933,12 +1981,18 @@
       <c r="C23" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="51"/>
-      <c r="E23" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
+      <c r="D23" s="49">
+        <v>43685</v>
+      </c>
+      <c r="E23" s="49">
+        <v>43685</v>
+      </c>
+      <c r="F23" s="49">
+        <v>43685</v>
+      </c>
+      <c r="G23" s="49">
+        <v>43685</v>
+      </c>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -3153,12 +3207,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="A20:A23"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A28:A32"/>
     <mergeCell ref="A33:A36"/>
@@ -3166,6 +3214,12 @@
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="A47:A51"/>
     <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>